<commit_message>
added geonovum respec,and configured MIMLM
</commit_message>
<xml_diff>
--- a/src/main/resources/input/Geonovum/props/Geonovum.xlsx
+++ b/src/main/resources/input/Geonovum/props/Geonovum.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="577" uniqueCount="290">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="581" uniqueCount="289">
   <si>
     <t>Name</t>
   </si>
@@ -838,9 +838,6 @@
   </si>
   <si>
     <t>The name of the variant of the XML schema generated.</t>
-  </si>
-  <si>
-    <t>ISO19136</t>
   </si>
   <si>
     <t>OBSOLETE</t>
@@ -1033,7 +1030,7 @@
     <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -1123,6 +1120,12 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="6" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1438,10 +1441,10 @@
   <dimension ref="A1:Q125"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="D85" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E101" sqref="E101"/>
+      <selection pane="bottomRight" activeCell="O47" sqref="O47:P47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -1517,29 +1520,29 @@
       <c r="F2" s="3"/>
       <c r="G2" s="19"/>
       <c r="H2" s="3" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="I2" s="3" t="s">
+        <v>276</v>
+      </c>
+      <c r="J2" s="3" t="s">
         <v>277</v>
       </c>
-      <c r="J2" s="3" t="s">
+      <c r="K2" s="3" t="s">
         <v>278</v>
-      </c>
-      <c r="K2" s="3" t="s">
-        <v>279</v>
       </c>
       <c r="L2" s="19"/>
       <c r="M2" s="3" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="N2" s="3" t="s">
+        <v>279</v>
+      </c>
+      <c r="O2" s="3" t="s">
         <v>280</v>
       </c>
-      <c r="O2" s="3" t="s">
+      <c r="P2" s="3" t="s">
         <v>281</v>
-      </c>
-      <c r="P2" s="3" t="s">
-        <v>282</v>
       </c>
       <c r="Q2" s="5"/>
     </row>
@@ -1642,16 +1645,16 @@
       <c r="Q6"/>
     </row>
     <row r="7" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A7" s="41" t="s">
+      <c r="A7" s="43" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="41" t="s">
+      <c r="B7" s="43" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="41" t="s">
+      <c r="C7" s="43" t="s">
         <v>11</v>
       </c>
-      <c r="D7" s="41" t="b">
+      <c r="D7" s="43" t="b">
         <v>1</v>
       </c>
       <c r="E7" s="2" t="b">
@@ -1666,10 +1669,10 @@
       <c r="Q7"/>
     </row>
     <row r="8" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="41"/>
-      <c r="B8" s="41"/>
-      <c r="C8" s="41"/>
-      <c r="D8" s="41"/>
+      <c r="A8" s="43"/>
+      <c r="B8" s="43"/>
+      <c r="C8" s="43"/>
+      <c r="D8" s="43"/>
       <c r="G8" s="20"/>
       <c r="L8" s="20"/>
       <c r="M8" s="17"/>
@@ -1940,7 +1943,7 @@
         <v>1</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="G18" s="20"/>
       <c r="L18" s="20"/>
@@ -1991,7 +1994,7 @@
         <v>1</v>
       </c>
       <c r="F20" s="34" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="G20" s="20"/>
       <c r="L20" s="20"/>
@@ -2018,7 +2021,7 @@
         <v>1</v>
       </c>
       <c r="F21" s="34" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="G21" s="20"/>
       <c r="L21" s="20"/>
@@ -2454,7 +2457,7 @@
         <v>1</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="G33" s="20"/>
       <c r="L33" s="20"/>
@@ -2600,13 +2603,13 @@
         <v>16</v>
       </c>
       <c r="I37" s="2" t="s">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="J37" s="2" t="s">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="K37" s="2" t="s">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="L37" s="20"/>
       <c r="M37" s="17" t="s">
@@ -2653,17 +2656,17 @@
         <v>25</v>
       </c>
       <c r="L38" s="27"/>
-      <c r="M38" s="30" t="s">
-        <v>271</v>
-      </c>
-      <c r="N38" s="31" t="s">
-        <v>271</v>
-      </c>
-      <c r="O38" s="31" t="s">
-        <v>271</v>
-      </c>
-      <c r="P38" s="31" t="s">
-        <v>271</v>
+      <c r="M38" s="41" t="s">
+        <v>25</v>
+      </c>
+      <c r="N38" s="41" t="s">
+        <v>25</v>
+      </c>
+      <c r="O38" s="41" t="s">
+        <v>25</v>
+      </c>
+      <c r="P38" s="41" t="s">
+        <v>25</v>
       </c>
       <c r="Q38"/>
     </row>
@@ -2741,16 +2744,16 @@
       <c r="Q41"/>
     </row>
     <row r="42" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A42" s="41" t="s">
+      <c r="A42" s="43" t="s">
         <v>51</v>
       </c>
-      <c r="B42" s="41" t="s">
+      <c r="B42" s="43" t="s">
         <v>5</v>
       </c>
-      <c r="C42" s="41" t="s">
+      <c r="C42" s="43" t="s">
         <v>52</v>
       </c>
-      <c r="D42" s="41" t="b">
+      <c r="D42" s="43" t="b">
         <v>0</v>
       </c>
       <c r="E42" s="2" t="b">
@@ -2768,10 +2771,10 @@
       <c r="Q42"/>
     </row>
     <row r="43" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A43" s="41"/>
-      <c r="B43" s="41"/>
-      <c r="C43" s="41"/>
-      <c r="D43" s="41"/>
+      <c r="A43" s="43"/>
+      <c r="B43" s="43"/>
+      <c r="C43" s="43"/>
+      <c r="D43" s="43"/>
       <c r="G43" s="20"/>
       <c r="L43" s="20"/>
       <c r="M43" s="17"/>
@@ -2868,26 +2871,34 @@
         <v>0</v>
       </c>
       <c r="F47" s="2" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="G47" s="21"/>
       <c r="H47" s="33" t="s">
+        <v>282</v>
+      </c>
+      <c r="I47" s="40" t="s">
+        <v>282</v>
+      </c>
+      <c r="J47" s="40" t="s">
+        <v>282</v>
+      </c>
+      <c r="K47" s="40" t="s">
+        <v>282</v>
+      </c>
+      <c r="L47" s="21"/>
+      <c r="M47" s="42" t="s">
         <v>283</v>
       </c>
-      <c r="I47" s="40" t="s">
+      <c r="N47" s="42" t="s">
         <v>283</v>
       </c>
-      <c r="J47" s="40" t="s">
+      <c r="O47" s="42" t="s">
         <v>283</v>
       </c>
-      <c r="K47" s="40" t="s">
+      <c r="P47" s="42" t="s">
         <v>283</v>
       </c>
-      <c r="L47" s="21"/>
-      <c r="M47" s="33"/>
-      <c r="N47" s="33"/>
-      <c r="O47" s="33"/>
-      <c r="P47" s="33"/>
       <c r="Q47"/>
     </row>
     <row r="48" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.4">
@@ -3228,7 +3239,7 @@
         <v>0</v>
       </c>
       <c r="F61" s="2" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="G61" s="20"/>
       <c r="L61" s="20"/>
@@ -3306,29 +3317,29 @@
       </c>
       <c r="G64" s="20"/>
       <c r="H64" s="2" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="I64" s="39" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="J64" s="39" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="K64" s="39" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="L64" s="20"/>
       <c r="M64" s="39" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="N64" s="39" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="O64" s="39" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="P64" s="39" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="Q64"/>
     </row>
@@ -3455,29 +3466,29 @@
       <c r="F69" s="33"/>
       <c r="G69" s="20"/>
       <c r="H69" s="38" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="I69" s="38" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="J69" s="38" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="K69" s="38" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="L69" s="27"/>
       <c r="M69" s="38" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="N69" s="38" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="O69" s="38" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="P69" s="38" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="Q69"/>
     </row>
@@ -3525,7 +3536,7 @@
         <v>0</v>
       </c>
       <c r="F71" s="7" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="G71" s="20"/>
       <c r="L71" s="20"/>
@@ -3599,29 +3610,29 @@
       </c>
       <c r="G74" s="20"/>
       <c r="H74" s="38" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="I74" s="38" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="J74" s="38" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="K74" s="38" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="L74" s="27"/>
       <c r="M74" s="38" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="N74" s="38" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="O74" s="38" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="P74" s="38" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="Q74"/>
     </row>
@@ -3809,7 +3820,7 @@
         <v>0</v>
       </c>
       <c r="F81" s="31" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="G81" s="27"/>
       <c r="L81" s="27"/>
@@ -3882,7 +3893,7 @@
         <v>1</v>
       </c>
       <c r="F84" s="17" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="G84" s="20"/>
       <c r="I84" s="35"/>
@@ -4045,29 +4056,29 @@
       </c>
       <c r="G90" s="20"/>
       <c r="H90" s="38" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="I90" s="38" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="J90" s="38" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="K90" s="38" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="L90" s="27"/>
       <c r="M90" s="38" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="N90" s="38" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="O90" s="38" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="P90" s="38" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="Q90"/>
     </row>
@@ -4441,7 +4452,7 @@
         <v>0</v>
       </c>
       <c r="F101" s="2" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="G101" s="20"/>
       <c r="L101" s="20"/>

</xml_diff>

<commit_message>
Geonovum Default geen json schema's genereren
</commit_message>
<xml_diff>
--- a/src/main/resources/input/Geonovum/props/Geonovum.xlsx
+++ b/src/main/resources/input/Geonovum/props/Geonovum.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="581" uniqueCount="289">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="574" uniqueCount="289">
   <si>
     <t>Name</t>
   </si>
@@ -1441,10 +1441,10 @@
   <dimension ref="A1:Q125"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B15" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="O47" sqref="O47:P47"/>
+      <selection pane="bottomRight" activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -2314,32 +2314,14 @@
       <c r="E29" s="28" t="b">
         <v>1</v>
       </c>
+      <c r="F29" s="28" t="s">
+        <v>16</v>
+      </c>
       <c r="G29" s="27"/>
-      <c r="H29" s="28" t="s">
-        <v>16</v>
-      </c>
-      <c r="I29" s="29" t="s">
-        <v>16</v>
-      </c>
-      <c r="J29" s="29" t="s">
-        <v>16</v>
-      </c>
-      <c r="K29" s="29" t="s">
-        <v>16</v>
-      </c>
+      <c r="I29" s="29"/>
+      <c r="J29" s="29"/>
+      <c r="K29" s="29"/>
       <c r="L29" s="27"/>
-      <c r="M29" s="28" t="s">
-        <v>16</v>
-      </c>
-      <c r="N29" s="28" t="s">
-        <v>4</v>
-      </c>
-      <c r="O29" s="28" t="s">
-        <v>4</v>
-      </c>
-      <c r="P29" s="28" t="s">
-        <v>4</v>
-      </c>
       <c r="Q29"/>
     </row>
     <row r="30" spans="1:17" s="30" customFormat="1" x14ac:dyDescent="0.4">

</xml_diff>

<commit_message>
Geonovum: Respec documents follow BRO setup.
</commit_message>
<xml_diff>
--- a/src/main/resources/input/Geonovum/props/Geonovum.xlsx
+++ b/src/main/resources/input/Geonovum/props/Geonovum.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="622" uniqueCount="313">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="615" uniqueCount="314">
   <si>
     <t>Name</t>
   </si>
@@ -900,9 +900,6 @@
     <t>Specify the type of office file. Multiple formats are allowed, separate list by whitespace.</t>
   </si>
   <si>
-    <t>[project-name]-[application-name]-[phase]-[release]</t>
-  </si>
-  <si>
     <t>respec</t>
   </si>
   <si>
@@ -964,6 +961,12 @@
   </si>
   <si>
     <t>git</t>
+  </si>
+  <si>
+    <t>[model-abbreviation]-cat</t>
+  </si>
+  <si>
+    <t>ISO19136</t>
   </si>
 </sst>
 </file>
@@ -1108,7 +1111,7 @@
     <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -1234,6 +1237,9 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1528,10 +1534,10 @@
   <dimension ref="A1:R132"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B59" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B28" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F77" sqref="F77"/>
+      <selection pane="bottomRight" activeCell="A39" sqref="A39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -2587,7 +2593,7 @@
         <v>1</v>
       </c>
       <c r="F34" s="43" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="G34" s="27"/>
       <c r="L34" s="27"/>
@@ -2640,13 +2646,13 @@
     </row>
     <row r="36" spans="1:18" s="44" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A36" s="44" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B36" s="44" t="s">
         <v>5</v>
       </c>
       <c r="C36" s="44" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="D36" s="44" t="b">
         <v>0</v>
@@ -2817,32 +2823,19 @@
       <c r="E40" s="30" t="b">
         <v>1</v>
       </c>
+      <c r="F40" s="47" t="s">
+        <v>313</v>
+      </c>
       <c r="G40" s="27"/>
-      <c r="H40" s="36" t="s">
-        <v>25</v>
-      </c>
-      <c r="I40" s="37" t="s">
-        <v>25</v>
-      </c>
-      <c r="J40" s="36" t="s">
-        <v>25</v>
-      </c>
-      <c r="K40" s="37" t="s">
-        <v>25</v>
-      </c>
+      <c r="H40" s="36"/>
+      <c r="I40" s="37"/>
+      <c r="J40" s="36"/>
+      <c r="K40" s="37"/>
       <c r="L40" s="27"/>
-      <c r="M40" s="41" t="s">
-        <v>25</v>
-      </c>
-      <c r="N40" s="41" t="s">
-        <v>25</v>
-      </c>
-      <c r="O40" s="41" t="s">
-        <v>25</v>
-      </c>
-      <c r="P40" s="41" t="s">
-        <v>25</v>
-      </c>
+      <c r="M40" s="41"/>
+      <c r="N40" s="41"/>
+      <c r="O40" s="41"/>
+      <c r="P40" s="41"/>
       <c r="Q40" s="27"/>
       <c r="R40"/>
     </row>
@@ -3244,22 +3237,22 @@
     </row>
     <row r="56" spans="1:18" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A56" s="16" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="B56" s="16" t="s">
         <v>10</v>
       </c>
       <c r="C56" s="15" t="s">
+        <v>301</v>
+      </c>
+      <c r="D56" s="16" t="b">
+        <v>0</v>
+      </c>
+      <c r="E56" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="F56" s="16" t="s">
         <v>302</v>
-      </c>
-      <c r="D56" s="16" t="b">
-        <v>0</v>
-      </c>
-      <c r="E56" s="16" t="b">
-        <v>1</v>
-      </c>
-      <c r="F56" s="16" t="s">
-        <v>303</v>
       </c>
       <c r="G56" s="22"/>
       <c r="H56" s="16"/>
@@ -3276,22 +3269,22 @@
     </row>
     <row r="57" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A57" s="7" t="s">
+        <v>305</v>
+      </c>
+      <c r="B57" s="7" t="s">
         <v>306</v>
       </c>
-      <c r="B57" s="7" t="s">
+      <c r="C57" s="7" t="s">
         <v>307</v>
       </c>
-      <c r="C57" s="7" t="s">
+      <c r="D57" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="E57" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="F57" s="7" t="s">
         <v>308</v>
-      </c>
-      <c r="D57" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="E57" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="F57" s="7" t="s">
-        <v>309</v>
       </c>
       <c r="G57" s="27"/>
       <c r="L57" s="27"/>
@@ -3299,13 +3292,13 @@
     </row>
     <row r="58" spans="1:18" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A58" s="7" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B58" s="7" t="s">
         <v>90</v>
       </c>
       <c r="C58" s="7" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="D58" s="7" t="b">
         <v>0</v>
@@ -3314,7 +3307,7 @@
         <v>1</v>
       </c>
       <c r="F58" s="34" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="G58" s="27"/>
       <c r="H58" s="34"/>
@@ -3345,7 +3338,7 @@
         <v>1</v>
       </c>
       <c r="F59" s="7" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="G59" s="27"/>
       <c r="L59" s="27"/>
@@ -3807,7 +3800,7 @@
         <v>0</v>
       </c>
       <c r="F75" s="2" t="s">
-        <v>291</v>
+        <v>312</v>
       </c>
       <c r="G75" s="20"/>
       <c r="L75" s="20"/>
@@ -3863,13 +3856,13 @@
       </c>
       <c r="G77" s="20"/>
       <c r="I77" s="2" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="J77" s="2" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="K77" s="2" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="L77" s="20"/>
       <c r="M77" s="17"/>
@@ -4258,13 +4251,13 @@
     </row>
     <row r="91" spans="1:18" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A91" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="B91" t="s">
         <v>10</v>
       </c>
       <c r="C91" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="D91" t="b">
         <v>1</v>
@@ -4685,18 +4678,18 @@
       </c>
       <c r="Q103" s="27"/>
       <c r="R103" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="104" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A104" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B104" t="s">
         <v>5</v>
       </c>
       <c r="C104" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="D104" t="b">
         <v>0</v>
@@ -4733,7 +4726,7 @@
       </c>
       <c r="Q104" s="27"/>
       <c r="R104" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="105" spans="1:18" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">

</xml_diff>

<commit_message>
[geonovum] min/maximum waarde toegevoegd
</commit_message>
<xml_diff>
--- a/src/main/resources/input/Geonovum/props/Geonovum.xlsx
+++ b/src/main/resources/input/Geonovum/props/Geonovum.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="644" uniqueCount="323">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="655" uniqueCount="325">
   <si>
     <t>Name</t>
   </si>
@@ -994,6 +994,12 @@
   </si>
   <si>
     <t>Yes if scalar types may be entered without reference to a UML datatype</t>
+  </si>
+  <si>
+    <t>createeatoolbox</t>
+  </si>
+  <si>
+    <t>Should an EA toolbox be generated?</t>
   </si>
 </sst>
 </file>
@@ -1138,7 +1144,7 @@
     <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -1267,6 +1273,9 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1570,13 +1579,13 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:R136"/>
+  <dimension ref="A1:R137"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B62" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="F20" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A74" sqref="A74:XFD74"/>
+      <selection pane="bottomRight" activeCell="A27" sqref="A27:XFD27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -1784,16 +1793,16 @@
       <c r="R6"/>
     </row>
     <row r="7" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A7" s="51" t="s">
+      <c r="A7" s="52" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="51" t="s">
+      <c r="B7" s="52" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="51" t="s">
+      <c r="C7" s="52" t="s">
         <v>11</v>
       </c>
-      <c r="D7" s="51" t="b">
+      <c r="D7" s="52" t="b">
         <v>1</v>
       </c>
       <c r="E7" s="2" t="b">
@@ -1809,10 +1818,10 @@
       <c r="R7"/>
     </row>
     <row r="8" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="51"/>
-      <c r="B8" s="51"/>
-      <c r="C8" s="51"/>
-      <c r="D8" s="51"/>
+      <c r="A8" s="52"/>
+      <c r="B8" s="52"/>
+      <c r="C8" s="52"/>
+      <c r="D8" s="52"/>
       <c r="G8" s="20"/>
       <c r="L8" s="20"/>
       <c r="M8" s="17"/>
@@ -2369,63 +2378,62 @@
       <c r="Q26" s="27"/>
       <c r="R26"/>
     </row>
-    <row r="27" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A27" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="B27" s="2" t="s">
+    <row r="27" spans="1:18" s="51" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A27" s="51" t="s">
+        <v>323</v>
+      </c>
+      <c r="B27" s="51" t="s">
         <v>5</v>
       </c>
-      <c r="C27" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="D27" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E27" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="G27" s="20"/>
-      <c r="H27" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="I27" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="J27" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="K27" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="L27" s="20"/>
-      <c r="M27" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="N27" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="O27" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="P27" s="17" t="s">
+      <c r="C27" s="51" t="s">
+        <v>324</v>
+      </c>
+      <c r="D27" s="51" t="b">
+        <v>0</v>
+      </c>
+      <c r="E27" s="51" t="b">
+        <v>1</v>
+      </c>
+      <c r="G27" s="27"/>
+      <c r="H27" s="51" t="s">
+        <v>16</v>
+      </c>
+      <c r="I27" s="51" t="s">
+        <v>4</v>
+      </c>
+      <c r="J27" s="51" t="s">
+        <v>4</v>
+      </c>
+      <c r="K27" s="51" t="s">
+        <v>4</v>
+      </c>
+      <c r="L27" s="27"/>
+      <c r="M27" s="51" t="s">
+        <v>16</v>
+      </c>
+      <c r="N27" s="51" t="s">
+        <v>4</v>
+      </c>
+      <c r="O27" s="51" t="s">
+        <v>4</v>
+      </c>
+      <c r="P27" s="51" t="s">
         <v>4</v>
       </c>
       <c r="Q27" s="27"/>
-      <c r="R27"/>
     </row>
     <row r="28" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A28" s="2" t="s">
-        <v>146</v>
+        <v>32</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>147</v>
+        <v>33</v>
       </c>
       <c r="D28" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E28" s="2" t="b">
         <v>1</v>
@@ -2435,7 +2443,7 @@
         <v>16</v>
       </c>
       <c r="I28" s="2" t="s">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="J28" s="2" t="s">
         <v>4</v>
@@ -2448,7 +2456,7 @@
         <v>16</v>
       </c>
       <c r="N28" s="17" t="s">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="O28" s="17" t="s">
         <v>4</v>
@@ -2459,159 +2467,176 @@
       <c r="Q28" s="27"/>
       <c r="R28"/>
     </row>
-    <row r="29" spans="1:18" s="46" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A29" s="46" t="s">
+    <row r="29" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A29" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="D29" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E29" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="G29" s="20"/>
+      <c r="H29" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I29" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="J29" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="K29" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="L29" s="20"/>
+      <c r="M29" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="N29" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="O29" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="P29" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q29" s="27"/>
+      <c r="R29"/>
+    </row>
+    <row r="30" spans="1:18" s="46" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A30" s="46" t="s">
         <v>316</v>
       </c>
-      <c r="B29" s="46" t="s">
+      <c r="B30" s="46" t="s">
         <v>5</v>
       </c>
-      <c r="C29" s="46" t="s">
+      <c r="C30" s="46" t="s">
         <v>317</v>
       </c>
-      <c r="D29" s="46" t="b">
-        <v>0</v>
-      </c>
-      <c r="E29" s="46" t="b">
-        <v>1</v>
-      </c>
-      <c r="G29" s="27"/>
-      <c r="H29" s="46" t="s">
-        <v>16</v>
-      </c>
-      <c r="I29" s="46" t="s">
-        <v>4</v>
-      </c>
-      <c r="J29" s="46" t="s">
-        <v>4</v>
-      </c>
-      <c r="K29" s="46" t="s">
-        <v>4</v>
-      </c>
-      <c r="L29" s="27"/>
-      <c r="M29" s="46" t="s">
-        <v>16</v>
-      </c>
-      <c r="N29" s="46" t="s">
-        <v>16</v>
-      </c>
-      <c r="O29" s="46" t="s">
-        <v>16</v>
-      </c>
-      <c r="P29" s="46" t="s">
-        <v>16</v>
-      </c>
-      <c r="Q29" s="27"/>
-    </row>
-    <row r="30" spans="1:18" s="28" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A30" s="28" t="s">
+      <c r="D30" s="46" t="b">
+        <v>0</v>
+      </c>
+      <c r="E30" s="46" t="b">
+        <v>1</v>
+      </c>
+      <c r="G30" s="27"/>
+      <c r="H30" s="46" t="s">
+        <v>16</v>
+      </c>
+      <c r="I30" s="46" t="s">
+        <v>4</v>
+      </c>
+      <c r="J30" s="46" t="s">
+        <v>4</v>
+      </c>
+      <c r="K30" s="46" t="s">
+        <v>4</v>
+      </c>
+      <c r="L30" s="27"/>
+      <c r="M30" s="46" t="s">
+        <v>16</v>
+      </c>
+      <c r="N30" s="46" t="s">
+        <v>16</v>
+      </c>
+      <c r="O30" s="46" t="s">
+        <v>16</v>
+      </c>
+      <c r="P30" s="46" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q30" s="27"/>
+    </row>
+    <row r="31" spans="1:18" s="28" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A31" s="28" t="s">
         <v>261</v>
       </c>
-      <c r="B30" s="28" t="s">
+      <c r="B31" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="C30" s="28" t="s">
+      <c r="C31" s="28" t="s">
         <v>262</v>
       </c>
-      <c r="D30" s="28" t="b">
-        <v>0</v>
-      </c>
-      <c r="E30" s="28" t="b">
-        <v>1</v>
-      </c>
-      <c r="F30" s="28" t="s">
-        <v>16</v>
-      </c>
-      <c r="G30" s="27"/>
-      <c r="I30" s="29"/>
-      <c r="J30" s="29"/>
-      <c r="K30" s="29"/>
-      <c r="L30" s="27"/>
-      <c r="Q30" s="27"/>
-      <c r="R30"/>
-    </row>
-    <row r="31" spans="1:18" s="30" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A31" s="30" t="s">
-        <v>266</v>
-      </c>
-      <c r="B31" s="30" t="s">
-        <v>10</v>
-      </c>
-      <c r="C31" s="30" t="s">
-        <v>267</v>
-      </c>
-      <c r="D31" s="30" t="b">
-        <v>0</v>
-      </c>
-      <c r="E31" s="30" t="b">
-        <v>1</v>
+      <c r="D31" s="28" t="b">
+        <v>0</v>
+      </c>
+      <c r="E31" s="28" t="b">
+        <v>1</v>
+      </c>
+      <c r="F31" s="28" t="s">
+        <v>16</v>
       </c>
       <c r="G31" s="27"/>
-      <c r="H31" s="31" t="s">
-        <v>25</v>
-      </c>
-      <c r="I31" s="32" t="s">
-        <v>25</v>
-      </c>
-      <c r="J31" s="32" t="s">
-        <v>25</v>
-      </c>
-      <c r="K31" s="32" t="s">
-        <v>25</v>
-      </c>
+      <c r="I31" s="29"/>
+      <c r="J31" s="29"/>
+      <c r="K31" s="29"/>
       <c r="L31" s="27"/>
-      <c r="M31" s="32" t="s">
-        <v>25</v>
-      </c>
-      <c r="N31" s="32" t="s">
-        <v>25</v>
-      </c>
-      <c r="O31" s="32" t="s">
-        <v>25</v>
-      </c>
-      <c r="P31" s="32" t="s">
-        <v>25</v>
-      </c>
       <c r="Q31" s="27"/>
       <c r="R31"/>
     </row>
-    <row r="32" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A32" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="B32" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="C32" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="D32" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E32" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F32" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="G32" s="20"/>
-      <c r="L32" s="20"/>
-      <c r="M32" s="17"/>
-      <c r="N32" s="17"/>
-      <c r="O32" s="17"/>
-      <c r="P32" s="17"/>
+    <row r="32" spans="1:18" s="30" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A32" s="30" t="s">
+        <v>266</v>
+      </c>
+      <c r="B32" s="30" t="s">
+        <v>10</v>
+      </c>
+      <c r="C32" s="30" t="s">
+        <v>267</v>
+      </c>
+      <c r="D32" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="E32" s="30" t="b">
+        <v>1</v>
+      </c>
+      <c r="G32" s="27"/>
+      <c r="H32" s="31" t="s">
+        <v>25</v>
+      </c>
+      <c r="I32" s="32" t="s">
+        <v>25</v>
+      </c>
+      <c r="J32" s="32" t="s">
+        <v>25</v>
+      </c>
+      <c r="K32" s="32" t="s">
+        <v>25</v>
+      </c>
+      <c r="L32" s="27"/>
+      <c r="M32" s="32" t="s">
+        <v>25</v>
+      </c>
+      <c r="N32" s="32" t="s">
+        <v>25</v>
+      </c>
+      <c r="O32" s="32" t="s">
+        <v>25</v>
+      </c>
+      <c r="P32" s="32" t="s">
+        <v>25</v>
+      </c>
       <c r="Q32" s="27"/>
       <c r="R32"/>
     </row>
     <row r="33" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A33" s="2" t="s">
-        <v>169</v>
+        <v>34</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>170</v>
+        <v>36</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>171</v>
+        <v>37</v>
       </c>
       <c r="D33" s="2" t="b">
         <v>0</v>
@@ -2620,7 +2645,7 @@
         <v>1</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>10</v>
+        <v>35</v>
       </c>
       <c r="G33" s="20"/>
       <c r="L33" s="20"/>
@@ -2631,15 +2656,15 @@
       <c r="Q33" s="27"/>
       <c r="R33"/>
     </row>
-    <row r="34" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A34" s="2" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="D34" s="2" t="b">
         <v>0</v>
@@ -2648,7 +2673,7 @@
         <v>1</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>271</v>
+        <v>10</v>
       </c>
       <c r="G34" s="20"/>
       <c r="L34" s="20"/>
@@ -2659,330 +2684,334 @@
       <c r="Q34" s="27"/>
       <c r="R34"/>
     </row>
-    <row r="35" spans="1:18" s="43" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A35" s="43" t="s">
+    <row r="35" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A35" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="D35" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E35" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F35" s="2" t="s">
+        <v>271</v>
+      </c>
+      <c r="G35" s="20"/>
+      <c r="L35" s="20"/>
+      <c r="M35" s="17"/>
+      <c r="N35" s="17"/>
+      <c r="O35" s="17"/>
+      <c r="P35" s="17"/>
+      <c r="Q35" s="27"/>
+      <c r="R35"/>
+    </row>
+    <row r="36" spans="1:18" s="43" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A36" s="43" t="s">
         <v>287</v>
       </c>
-      <c r="B35" s="43" t="s">
+      <c r="B36" s="43" t="s">
         <v>288</v>
       </c>
-      <c r="C35" s="43" t="s">
+      <c r="C36" s="43" t="s">
         <v>289</v>
       </c>
-      <c r="D35" s="43" t="b">
-        <v>0</v>
-      </c>
-      <c r="E35" s="43" t="b">
-        <v>1</v>
-      </c>
-      <c r="F35" s="43" t="s">
+      <c r="D36" s="43" t="b">
+        <v>0</v>
+      </c>
+      <c r="E36" s="43" t="b">
+        <v>1</v>
+      </c>
+      <c r="F36" s="43" t="s">
         <v>290</v>
       </c>
-      <c r="G35" s="27"/>
-      <c r="L35" s="27"/>
-      <c r="Q35" s="27"/>
-    </row>
-    <row r="36" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A36" s="2" t="s">
+      <c r="G36" s="27"/>
+      <c r="L36" s="27"/>
+      <c r="Q36" s="27"/>
+    </row>
+    <row r="37" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A37" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="B36" s="2" t="s">
+      <c r="B37" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C36" s="2" t="s">
+      <c r="C37" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="D36" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E36" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="G36" s="20"/>
-      <c r="H36" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="I36" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="J36" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="K36" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="L36" s="20"/>
-      <c r="M36" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="N36" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="O36" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="P36" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q36" s="27"/>
-      <c r="R36"/>
-    </row>
-    <row r="37" spans="1:18" s="44" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A37" s="44" t="s">
-        <v>291</v>
-      </c>
-      <c r="B37" s="44" t="s">
-        <v>5</v>
-      </c>
-      <c r="C37" s="44" t="s">
-        <v>292</v>
-      </c>
-      <c r="D37" s="44" t="b">
-        <v>0</v>
-      </c>
-      <c r="E37" s="44" t="b">
-        <v>1</v>
-      </c>
-      <c r="G37" s="45"/>
-      <c r="H37" s="44" t="s">
-        <v>16</v>
-      </c>
-      <c r="I37" s="44" t="s">
-        <v>16</v>
-      </c>
-      <c r="J37" s="44" t="s">
-        <v>4</v>
-      </c>
-      <c r="K37" s="44" t="s">
-        <v>4</v>
-      </c>
-      <c r="L37" s="45"/>
-      <c r="M37" s="44" t="s">
-        <v>16</v>
-      </c>
-      <c r="N37" s="44" t="s">
-        <v>16</v>
-      </c>
-      <c r="O37" s="44" t="s">
-        <v>4</v>
-      </c>
-      <c r="P37" s="44" t="s">
+      <c r="D37" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E37" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="G37" s="20"/>
+      <c r="H37" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I37" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="J37" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="K37" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="L37" s="20"/>
+      <c r="M37" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="N37" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="O37" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="P37" s="17" t="s">
         <v>4</v>
       </c>
       <c r="Q37" s="27"/>
       <c r="R37"/>
     </row>
-    <row r="38" spans="1:18" s="2" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
-      <c r="A38" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="B38" s="2" t="s">
+    <row r="38" spans="1:18" s="44" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A38" s="44" t="s">
+        <v>291</v>
+      </c>
+      <c r="B38" s="44" t="s">
         <v>5</v>
       </c>
-      <c r="C38" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="D38" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E38" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="G38" s="20"/>
-      <c r="H38" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="I38" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="J38" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="K38" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="L38" s="20"/>
-      <c r="M38" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="N38" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="O38" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="P38" s="17" t="s">
+      <c r="C38" s="44" t="s">
+        <v>292</v>
+      </c>
+      <c r="D38" s="44" t="b">
+        <v>0</v>
+      </c>
+      <c r="E38" s="44" t="b">
+        <v>1</v>
+      </c>
+      <c r="G38" s="45"/>
+      <c r="H38" s="44" t="s">
+        <v>16</v>
+      </c>
+      <c r="I38" s="44" t="s">
+        <v>16</v>
+      </c>
+      <c r="J38" s="44" t="s">
+        <v>4</v>
+      </c>
+      <c r="K38" s="44" t="s">
+        <v>4</v>
+      </c>
+      <c r="L38" s="45"/>
+      <c r="M38" s="44" t="s">
+        <v>16</v>
+      </c>
+      <c r="N38" s="44" t="s">
+        <v>16</v>
+      </c>
+      <c r="O38" s="44" t="s">
+        <v>4</v>
+      </c>
+      <c r="P38" s="44" t="s">
         <v>4</v>
       </c>
       <c r="Q38" s="27"/>
       <c r="R38"/>
     </row>
-    <row r="39" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="39" spans="1:18" s="2" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A39" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B39" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D39" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E39" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F39" s="2" t="s">
-        <v>16</v>
+        <v>1</v>
       </c>
       <c r="G39" s="20"/>
+      <c r="H39" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I39" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="J39" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="K39" s="2" t="s">
+        <v>4</v>
+      </c>
       <c r="L39" s="20"/>
-      <c r="M39" s="17"/>
-      <c r="N39" s="17"/>
-      <c r="O39" s="17"/>
-      <c r="P39" s="17"/>
+      <c r="M39" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="N39" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="O39" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="P39" s="17" t="s">
+        <v>4</v>
+      </c>
       <c r="Q39" s="27"/>
       <c r="R39"/>
     </row>
-    <row r="40" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="40" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A40" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B40" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D40" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E40" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="F40" s="2" t="s">
+        <v>16</v>
       </c>
       <c r="G40" s="20"/>
-      <c r="H40" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="I40" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="J40" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="K40" s="2" t="s">
-        <v>16</v>
-      </c>
       <c r="L40" s="20"/>
-      <c r="M40" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="N40" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="O40" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="P40" s="17" t="s">
-        <v>4</v>
-      </c>
+      <c r="M40" s="17"/>
+      <c r="N40" s="17"/>
+      <c r="O40" s="17"/>
+      <c r="P40" s="17"/>
       <c r="Q40" s="27"/>
       <c r="R40"/>
     </row>
-    <row r="41" spans="1:18" s="30" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A41" s="30" t="s">
-        <v>265</v>
-      </c>
-      <c r="B41" s="30" t="s">
-        <v>10</v>
-      </c>
-      <c r="C41" s="30" t="s">
-        <v>268</v>
-      </c>
-      <c r="D41" s="30" t="b">
-        <v>0</v>
-      </c>
-      <c r="E41" s="30" t="b">
-        <v>1</v>
-      </c>
-      <c r="F41" s="47" t="s">
-        <v>312</v>
-      </c>
-      <c r="G41" s="27"/>
-      <c r="H41" s="36"/>
-      <c r="I41" s="37"/>
-      <c r="J41" s="36"/>
-      <c r="K41" s="37"/>
-      <c r="L41" s="27"/>
-      <c r="M41" s="41"/>
-      <c r="N41" s="41"/>
-      <c r="O41" s="41"/>
-      <c r="P41" s="41"/>
+    <row r="41" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A41" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D41" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E41" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="G41" s="20"/>
+      <c r="H41" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I41" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="J41" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="K41" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="L41" s="20"/>
+      <c r="M41" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="N41" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="O41" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="P41" s="17" t="s">
+        <v>4</v>
+      </c>
       <c r="Q41" s="27"/>
       <c r="R41"/>
     </row>
-    <row r="42" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A42" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="B42" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C42" s="2" t="s">
-        <v>176</v>
-      </c>
-      <c r="D42" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E42" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F42" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="G42" s="20"/>
-      <c r="L42" s="20"/>
-      <c r="M42" s="17"/>
-      <c r="N42" s="17"/>
-      <c r="O42" s="17"/>
-      <c r="P42" s="17"/>
+    <row r="42" spans="1:18" s="30" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A42" s="30" t="s">
+        <v>265</v>
+      </c>
+      <c r="B42" s="30" t="s">
+        <v>10</v>
+      </c>
+      <c r="C42" s="30" t="s">
+        <v>268</v>
+      </c>
+      <c r="D42" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="E42" s="30" t="b">
+        <v>1</v>
+      </c>
+      <c r="F42" s="47" t="s">
+        <v>312</v>
+      </c>
+      <c r="G42" s="27"/>
+      <c r="H42" s="36"/>
+      <c r="I42" s="37"/>
+      <c r="J42" s="36"/>
+      <c r="K42" s="37"/>
+      <c r="L42" s="27"/>
+      <c r="M42" s="41"/>
+      <c r="N42" s="41"/>
+      <c r="O42" s="41"/>
+      <c r="P42" s="41"/>
       <c r="Q42" s="27"/>
       <c r="R42"/>
     </row>
-    <row r="43" spans="1:18" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A43" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="B43" s="7" t="s">
+    <row r="43" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A43" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="B43" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C43" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="D43" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="E43" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="F43" s="7" t="s">
+      <c r="C43" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="D43" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E43" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F43" s="2" t="s">
         <v>16</v>
       </c>
       <c r="G43" s="20"/>
       <c r="L43" s="20"/>
+      <c r="M43" s="17"/>
+      <c r="N43" s="17"/>
+      <c r="O43" s="17"/>
+      <c r="P43" s="17"/>
       <c r="Q43" s="27"/>
       <c r="R43"/>
     </row>
-    <row r="44" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="44" spans="1:18" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A44" s="7" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B44" s="7" t="s">
-        <v>49</v>
+        <v>5</v>
       </c>
       <c r="C44" s="7" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D44" s="7" t="b">
         <v>1</v>
@@ -2991,46 +3020,56 @@
         <v>0</v>
       </c>
       <c r="F44" s="7" t="s">
-        <v>220</v>
+        <v>16</v>
       </c>
       <c r="G44" s="20"/>
       <c r="L44" s="20"/>
       <c r="Q44" s="27"/>
       <c r="R44"/>
     </row>
-    <row r="45" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A45" s="51" t="s">
-        <v>51</v>
-      </c>
-      <c r="B45" s="51" t="s">
-        <v>5</v>
-      </c>
-      <c r="C45" s="51" t="s">
-        <v>52</v>
-      </c>
-      <c r="D45" s="51" t="b">
-        <v>0</v>
-      </c>
-      <c r="E45" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F45" s="2" t="s">
-        <v>16</v>
+    <row r="45" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A45" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="B45" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="C45" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="D45" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="E45" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="F45" s="7" t="s">
+        <v>220</v>
       </c>
       <c r="G45" s="20"/>
       <c r="L45" s="20"/>
-      <c r="M45" s="17"/>
-      <c r="N45" s="17"/>
-      <c r="O45" s="17"/>
-      <c r="P45" s="17"/>
       <c r="Q45" s="27"/>
       <c r="R45"/>
     </row>
     <row r="46" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A46" s="51"/>
-      <c r="B46" s="51"/>
-      <c r="C46" s="51"/>
-      <c r="D46" s="51"/>
+      <c r="A46" s="52" t="s">
+        <v>51</v>
+      </c>
+      <c r="B46" s="52" t="s">
+        <v>5</v>
+      </c>
+      <c r="C46" s="52" t="s">
+        <v>52</v>
+      </c>
+      <c r="D46" s="52" t="b">
+        <v>0</v>
+      </c>
+      <c r="E46" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F46" s="2" t="s">
+        <v>16</v>
+      </c>
       <c r="G46" s="20"/>
       <c r="L46" s="20"/>
       <c r="M46" s="17"/>
@@ -3040,22 +3079,11 @@
       <c r="Q46" s="27"/>
       <c r="R46"/>
     </row>
-    <row r="47" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A47" s="2" t="s">
-        <v>177</v>
-      </c>
-      <c r="B47" s="2" t="s">
-        <v>178</v>
-      </c>
-      <c r="C47" s="2" t="s">
-        <v>179</v>
-      </c>
-      <c r="D47" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E47" s="2" t="b">
-        <v>0</v>
-      </c>
+    <row r="47" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A47" s="52"/>
+      <c r="B47" s="52"/>
+      <c r="C47" s="52"/>
+      <c r="D47" s="52"/>
       <c r="G47" s="20"/>
       <c r="L47" s="20"/>
       <c r="M47" s="17"/>
@@ -3065,21 +3093,21 @@
       <c r="Q47" s="27"/>
       <c r="R47"/>
     </row>
-    <row r="48" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="48" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A48" s="2" t="s">
-        <v>53</v>
+        <v>177</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>5</v>
+        <v>178</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>54</v>
+        <v>179</v>
       </c>
       <c r="D48" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E48" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G48" s="20"/>
       <c r="L48" s="20"/>
@@ -3090,15 +3118,15 @@
       <c r="Q48" s="27"/>
       <c r="R48"/>
     </row>
-    <row r="49" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="49" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A49" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>56</v>
+        <v>5</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="D49" s="2" t="b">
         <v>0</v>
@@ -3106,11 +3134,8 @@
       <c r="E49" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="F49" s="6" t="s">
-        <v>207</v>
-      </c>
-      <c r="G49" s="21"/>
-      <c r="L49" s="21"/>
+      <c r="G49" s="20"/>
+      <c r="L49" s="20"/>
       <c r="M49" s="17"/>
       <c r="N49" s="17"/>
       <c r="O49" s="17"/>
@@ -3118,83 +3143,87 @@
       <c r="Q49" s="27"/>
       <c r="R49"/>
     </row>
-    <row r="50" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="50" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A50" s="2" t="s">
-        <v>221</v>
-      </c>
-      <c r="B50" s="8"/>
-      <c r="C50" s="8"/>
+        <v>55</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C50" s="2" t="s">
+        <v>57</v>
+      </c>
       <c r="D50" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E50" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F50" s="2" t="s">
-        <v>284</v>
+        <v>1</v>
+      </c>
+      <c r="F50" s="6" t="s">
+        <v>207</v>
       </c>
       <c r="G50" s="21"/>
-      <c r="H50" s="33" t="s">
-        <v>280</v>
-      </c>
-      <c r="I50" s="40" t="s">
-        <v>280</v>
-      </c>
-      <c r="J50" s="40" t="s">
-        <v>280</v>
-      </c>
-      <c r="K50" s="40" t="s">
-        <v>280</v>
-      </c>
       <c r="L50" s="21"/>
-      <c r="M50" s="42" t="s">
-        <v>281</v>
-      </c>
-      <c r="N50" s="42" t="s">
-        <v>281</v>
-      </c>
-      <c r="O50" s="42" t="s">
-        <v>281</v>
-      </c>
-      <c r="P50" s="42" t="s">
-        <v>281</v>
-      </c>
+      <c r="M50" s="17"/>
+      <c r="N50" s="17"/>
+      <c r="O50" s="17"/>
+      <c r="P50" s="17"/>
       <c r="Q50" s="27"/>
       <c r="R50"/>
     </row>
-    <row r="51" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A51" s="7" t="s">
-        <v>180</v>
-      </c>
-      <c r="B51" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="C51" s="7" t="s">
-        <v>181</v>
-      </c>
-      <c r="D51" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="E51" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="F51" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="G51" s="20"/>
-      <c r="L51" s="20"/>
+    <row r="51" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A51" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="B51" s="8"/>
+      <c r="C51" s="8"/>
+      <c r="D51" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E51" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F51" s="2" t="s">
+        <v>284</v>
+      </c>
+      <c r="G51" s="21"/>
+      <c r="H51" s="33" t="s">
+        <v>280</v>
+      </c>
+      <c r="I51" s="40" t="s">
+        <v>280</v>
+      </c>
+      <c r="J51" s="40" t="s">
+        <v>280</v>
+      </c>
+      <c r="K51" s="40" t="s">
+        <v>280</v>
+      </c>
+      <c r="L51" s="21"/>
+      <c r="M51" s="42" t="s">
+        <v>281</v>
+      </c>
+      <c r="N51" s="42" t="s">
+        <v>281</v>
+      </c>
+      <c r="O51" s="42" t="s">
+        <v>281</v>
+      </c>
+      <c r="P51" s="42" t="s">
+        <v>281</v>
+      </c>
       <c r="Q51" s="27"/>
       <c r="R51"/>
     </row>
-    <row r="52" spans="1:18" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="52" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A52" s="7" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="B52" s="7" t="s">
-        <v>183</v>
+        <v>5</v>
       </c>
       <c r="C52" s="7" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="D52" s="7" t="b">
         <v>0</v>
@@ -3203,50 +3232,46 @@
         <v>1</v>
       </c>
       <c r="F52" s="7" t="s">
-        <v>210</v>
+        <v>4</v>
       </c>
       <c r="G52" s="20"/>
       <c r="L52" s="20"/>
       <c r="Q52" s="27"/>
       <c r="R52"/>
     </row>
-    <row r="53" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A53" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="B53" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C53" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="D53" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E53" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F53" s="2" t="s">
-        <v>16</v>
+    <row r="53" spans="1:18" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A53" s="7" t="s">
+        <v>182</v>
+      </c>
+      <c r="B53" s="7" t="s">
+        <v>183</v>
+      </c>
+      <c r="C53" s="7" t="s">
+        <v>184</v>
+      </c>
+      <c r="D53" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="E53" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="F53" s="7" t="s">
+        <v>210</v>
       </c>
       <c r="G53" s="20"/>
       <c r="L53" s="20"/>
-      <c r="M53" s="17"/>
-      <c r="N53" s="17"/>
-      <c r="O53" s="17"/>
-      <c r="P53" s="17"/>
       <c r="Q53" s="27"/>
       <c r="R53"/>
     </row>
     <row r="54" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A54" s="2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B54" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D54" s="2" t="b">
         <v>0</v>
@@ -3266,359 +3291,359 @@
       <c r="Q54" s="27"/>
       <c r="R54"/>
     </row>
-    <row r="55" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A55" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="B55" s="7" t="s">
+    <row r="55" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A55" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B55" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C55" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="D55" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="E55" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="F55" s="7" t="s">
+      <c r="C55" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="D55" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E55" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F55" s="2" t="s">
         <v>16</v>
       </c>
       <c r="G55" s="20"/>
       <c r="L55" s="20"/>
+      <c r="M55" s="17"/>
+      <c r="N55" s="17"/>
+      <c r="O55" s="17"/>
+      <c r="P55" s="17"/>
       <c r="Q55" s="27"/>
       <c r="R55"/>
     </row>
-    <row r="56" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A56" s="2" t="s">
-        <v>185</v>
-      </c>
-      <c r="B56" s="2" t="s">
+    <row r="56" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A56" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="B56" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C56" s="2" t="s">
-        <v>186</v>
-      </c>
-      <c r="D56" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E56" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F56" s="2" t="s">
+      <c r="C56" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="D56" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="E56" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="F56" s="7" t="s">
         <v>16</v>
       </c>
       <c r="G56" s="20"/>
       <c r="L56" s="20"/>
-      <c r="M56" s="17"/>
-      <c r="N56" s="17"/>
-      <c r="O56" s="17"/>
-      <c r="P56" s="17"/>
       <c r="Q56" s="27"/>
       <c r="R56"/>
     </row>
-    <row r="57" spans="1:18" ht="43.75" x14ac:dyDescent="0.4">
-      <c r="A57" s="16" t="s">
+    <row r="57" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A57" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="B57" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C57" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="D57" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E57" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F57" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G57" s="20"/>
+      <c r="L57" s="20"/>
+      <c r="M57" s="17"/>
+      <c r="N57" s="17"/>
+      <c r="O57" s="17"/>
+      <c r="P57" s="17"/>
+      <c r="Q57" s="27"/>
+      <c r="R57"/>
+    </row>
+    <row r="58" spans="1:18" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="A58" s="16" t="s">
         <v>299</v>
       </c>
-      <c r="B57" s="16" t="s">
+      <c r="B58" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="C57" s="15" t="s">
+      <c r="C58" s="15" t="s">
         <v>300</v>
       </c>
-      <c r="D57" s="16" t="b">
-        <v>0</v>
-      </c>
-      <c r="E57" s="16" t="b">
-        <v>1</v>
-      </c>
-      <c r="F57" s="16" t="s">
+      <c r="D58" s="16" t="b">
+        <v>0</v>
+      </c>
+      <c r="E58" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="F58" s="16" t="s">
         <v>301</v>
       </c>
-      <c r="G57" s="22"/>
-      <c r="H57" s="16"/>
-      <c r="I57" s="16"/>
-      <c r="J57" s="16"/>
-      <c r="K57" s="16"/>
-      <c r="L57" s="22"/>
-      <c r="M57" s="16"/>
-      <c r="N57" s="16"/>
-      <c r="O57" s="16"/>
-      <c r="P57" s="16"/>
-      <c r="Q57" s="22"/>
-      <c r="R57" s="16"/>
-    </row>
-    <row r="58" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A58" s="7" t="s">
+      <c r="G58" s="22"/>
+      <c r="H58" s="16"/>
+      <c r="I58" s="16"/>
+      <c r="J58" s="16"/>
+      <c r="K58" s="16"/>
+      <c r="L58" s="22"/>
+      <c r="M58" s="16"/>
+      <c r="N58" s="16"/>
+      <c r="O58" s="16"/>
+      <c r="P58" s="16"/>
+      <c r="Q58" s="22"/>
+      <c r="R58" s="16"/>
+    </row>
+    <row r="59" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A59" s="7" t="s">
         <v>304</v>
       </c>
-      <c r="B58" s="7" t="s">
+      <c r="B59" s="7" t="s">
         <v>305</v>
       </c>
-      <c r="C58" s="7" t="s">
+      <c r="C59" s="7" t="s">
         <v>306</v>
       </c>
-      <c r="D58" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="E58" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="F58" s="7" t="s">
+      <c r="D59" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="E59" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="F59" s="7" t="s">
         <v>307</v>
       </c>
-      <c r="G58" s="27"/>
-      <c r="L58" s="27"/>
-      <c r="Q58" s="27"/>
-    </row>
-    <row r="59" spans="1:18" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A59" s="7" t="s">
-        <v>302</v>
-      </c>
-      <c r="B59" s="7" t="s">
-        <v>90</v>
-      </c>
-      <c r="C59" s="7" t="s">
-        <v>308</v>
-      </c>
-      <c r="D59" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="E59" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="F59" s="34" t="s">
-        <v>303</v>
-      </c>
       <c r="G59" s="27"/>
-      <c r="H59" s="34"/>
-      <c r="I59" s="34"/>
-      <c r="J59" s="34"/>
-      <c r="K59" s="34"/>
       <c r="L59" s="27"/>
-      <c r="M59" s="34"/>
-      <c r="N59" s="34"/>
-      <c r="O59" s="34"/>
-      <c r="P59" s="34"/>
       <c r="Q59" s="27"/>
     </row>
     <row r="60" spans="1:18" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A60" s="7" t="s">
+        <v>302</v>
+      </c>
+      <c r="B60" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="C60" s="7" t="s">
+        <v>308</v>
+      </c>
+      <c r="D60" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="E60" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="F60" s="34" t="s">
+        <v>303</v>
+      </c>
+      <c r="G60" s="27"/>
+      <c r="H60" s="34"/>
+      <c r="I60" s="34"/>
+      <c r="J60" s="34"/>
+      <c r="K60" s="34"/>
+      <c r="L60" s="27"/>
+      <c r="M60" s="34"/>
+      <c r="N60" s="34"/>
+      <c r="O60" s="34"/>
+      <c r="P60" s="34"/>
+      <c r="Q60" s="27"/>
+    </row>
+    <row r="61" spans="1:18" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A61" s="7" t="s">
         <v>187</v>
       </c>
-      <c r="B60" s="7" t="s">
+      <c r="B61" s="7" t="s">
         <v>159</v>
       </c>
-      <c r="C60" s="7" t="s">
+      <c r="C61" s="7" t="s">
         <v>188</v>
       </c>
-      <c r="D60" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="E60" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="F60" s="7" t="s">
+      <c r="D61" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="E61" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="F61" s="7" t="s">
         <v>309</v>
       </c>
-      <c r="G60" s="27"/>
-      <c r="L60" s="27"/>
-      <c r="Q60"/>
-    </row>
-    <row r="61" spans="1:18" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A61" s="16" t="s">
+      <c r="G61" s="27"/>
+      <c r="L61" s="27"/>
+      <c r="Q61"/>
+    </row>
+    <row r="62" spans="1:18" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A62" s="16" t="s">
         <v>241</v>
       </c>
-      <c r="B61" s="16" t="s">
+      <c r="B62" s="16" t="s">
         <v>242</v>
       </c>
-      <c r="C61" s="15" t="s">
+      <c r="C62" s="15" t="s">
         <v>243</v>
       </c>
-      <c r="D61" s="16" t="b">
-        <v>0</v>
-      </c>
-      <c r="E61" s="16" t="b">
-        <v>1</v>
-      </c>
-      <c r="F61" s="16" t="s">
+      <c r="D62" s="16" t="b">
+        <v>0</v>
+      </c>
+      <c r="E62" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="F62" s="16" t="s">
         <v>244</v>
       </c>
-      <c r="G61" s="22"/>
-      <c r="H61" s="16"/>
-      <c r="I61" s="16"/>
-      <c r="J61" s="16"/>
-      <c r="K61" s="16"/>
-      <c r="L61" s="22"/>
-      <c r="M61" s="16"/>
-      <c r="N61" s="16"/>
-      <c r="O61" s="16"/>
-      <c r="P61" s="16"/>
-      <c r="Q61" s="22"/>
-      <c r="R61"/>
-    </row>
-    <row r="62" spans="1:18" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A62" s="7" t="s">
+      <c r="G62" s="22"/>
+      <c r="H62" s="16"/>
+      <c r="I62" s="16"/>
+      <c r="J62" s="16"/>
+      <c r="K62" s="16"/>
+      <c r="L62" s="22"/>
+      <c r="M62" s="16"/>
+      <c r="N62" s="16"/>
+      <c r="O62" s="16"/>
+      <c r="P62" s="16"/>
+      <c r="Q62" s="22"/>
+      <c r="R62"/>
+    </row>
+    <row r="63" spans="1:18" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A63" s="7" t="s">
         <v>189</v>
       </c>
-      <c r="B62" s="7" t="s">
+      <c r="B63" s="7" t="s">
         <v>190</v>
       </c>
-      <c r="C62" s="7" t="s">
+      <c r="C63" s="7" t="s">
         <v>191</v>
       </c>
-      <c r="D62" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="E62" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="F62" s="7" t="s">
+      <c r="D63" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="E63" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="F63" s="7" t="s">
         <v>19</v>
-      </c>
-      <c r="G62" s="20"/>
-      <c r="L62" s="20"/>
-      <c r="Q62" s="27"/>
-      <c r="R62"/>
-    </row>
-    <row r="63" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A63" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="B63" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C63" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="D63" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E63" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F63" s="2" t="s">
-        <v>208</v>
       </c>
       <c r="G63" s="20"/>
       <c r="L63" s="20"/>
-      <c r="M63" s="17"/>
-      <c r="N63" s="17"/>
-      <c r="O63" s="17"/>
-      <c r="P63" s="17"/>
       <c r="Q63" s="27"/>
       <c r="R63"/>
     </row>
-    <row r="64" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A64" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="B64" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="C64" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="D64" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="E64" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="F64" s="7" t="s">
-        <v>220</v>
+    <row r="64" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A64" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="B64" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C64" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D64" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E64" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F64" s="2" t="s">
+        <v>208</v>
       </c>
       <c r="G64" s="20"/>
       <c r="L64" s="20"/>
+      <c r="M64" s="17"/>
+      <c r="N64" s="17"/>
+      <c r="O64" s="17"/>
+      <c r="P64" s="17"/>
       <c r="Q64" s="27"/>
       <c r="R64"/>
     </row>
-    <row r="65" spans="1:18" s="46" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A65" s="46" t="s">
+    <row r="65" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A65" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="B65" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="C65" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="D65" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="E65" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="F65" s="7" t="s">
+        <v>220</v>
+      </c>
+      <c r="G65" s="20"/>
+      <c r="L65" s="20"/>
+      <c r="Q65" s="27"/>
+      <c r="R65"/>
+    </row>
+    <row r="66" spans="1:18" s="46" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A66" s="46" t="s">
         <v>313</v>
       </c>
-      <c r="B65" s="46" t="s">
+      <c r="B66" s="46" t="s">
         <v>10</v>
       </c>
-      <c r="C65" s="46" t="s">
+      <c r="C66" s="46" t="s">
         <v>314</v>
       </c>
-      <c r="D65" s="46" t="b">
-        <v>0</v>
-      </c>
-      <c r="E65" s="46" t="b">
-        <v>1</v>
-      </c>
-      <c r="F65" s="46" t="s">
+      <c r="D66" s="46" t="b">
+        <v>0</v>
+      </c>
+      <c r="E66" s="46" t="b">
+        <v>1</v>
+      </c>
+      <c r="F66" s="46" t="s">
         <v>315</v>
-      </c>
-      <c r="G65" s="27"/>
-      <c r="L65" s="27"/>
-      <c r="Q65" s="27"/>
-    </row>
-    <row r="66" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A66" t="s">
-        <v>263</v>
-      </c>
-      <c r="B66" t="s">
-        <v>82</v>
-      </c>
-      <c r="C66" t="s">
-        <v>264</v>
-      </c>
-      <c r="D66" t="b">
-        <v>0</v>
-      </c>
-      <c r="E66" t="b">
-        <v>1</v>
-      </c>
-      <c r="F66" t="s">
-        <v>228</v>
       </c>
       <c r="G66" s="27"/>
       <c r="L66" s="27"/>
       <c r="Q66" s="27"/>
-      <c r="R66"/>
-    </row>
-    <row r="67" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A67" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="B67" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="C67" s="2" t="s">
-        <v>148</v>
-      </c>
-      <c r="D67" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E67" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F67" s="2" t="s">
-        <v>211</v>
-      </c>
-      <c r="G67" s="20"/>
-      <c r="L67" s="20"/>
-      <c r="M67" s="17"/>
-      <c r="N67" s="17"/>
-      <c r="O67" s="17"/>
-      <c r="P67" s="17"/>
+    </row>
+    <row r="67" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A67" t="s">
+        <v>263</v>
+      </c>
+      <c r="B67" t="s">
+        <v>82</v>
+      </c>
+      <c r="C67" t="s">
+        <v>264</v>
+      </c>
+      <c r="D67" t="b">
+        <v>0</v>
+      </c>
+      <c r="E67" t="b">
+        <v>1</v>
+      </c>
+      <c r="F67" t="s">
+        <v>228</v>
+      </c>
+      <c r="G67" s="27"/>
+      <c r="L67" s="27"/>
       <c r="Q67" s="27"/>
       <c r="R67"/>
     </row>
-    <row r="68" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="68" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A68" s="2" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>10</v>
+        <v>70</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>72</v>
+        <v>148</v>
       </c>
       <c r="D68" s="2" t="b">
         <v>0</v>
@@ -3627,7 +3652,7 @@
         <v>0</v>
       </c>
       <c r="F68" s="2" t="s">
-        <v>270</v>
+        <v>211</v>
       </c>
       <c r="G68" s="20"/>
       <c r="L68" s="20"/>
@@ -3638,24 +3663,24 @@
       <c r="Q68" s="27"/>
       <c r="R68"/>
     </row>
-    <row r="69" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="69" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A69" s="2" t="s">
-        <v>192</v>
+        <v>71</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>193</v>
+        <v>10</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>194</v>
+        <v>72</v>
       </c>
       <c r="D69" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E69" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F69" s="2" t="s">
-        <v>209</v>
+        <v>270</v>
       </c>
       <c r="G69" s="20"/>
       <c r="L69" s="20"/>
@@ -3666,193 +3691,193 @@
       <c r="Q69" s="27"/>
       <c r="R69"/>
     </row>
-    <row r="70" spans="1:18" s="24" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A70" s="24" t="s">
-        <v>255</v>
-      </c>
-      <c r="B70" s="24" t="s">
-        <v>5</v>
-      </c>
-      <c r="C70" s="24" t="s">
-        <v>257</v>
-      </c>
-      <c r="D70" s="24" t="b">
-        <v>0</v>
-      </c>
-      <c r="E70" s="24" t="b">
-        <v>1</v>
-      </c>
-      <c r="F70" s="24" t="s">
-        <v>256</v>
+    <row r="70" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A70" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="B70" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="C70" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="D70" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E70" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F70" s="2" t="s">
+        <v>209</v>
       </c>
       <c r="G70" s="20"/>
       <c r="L70" s="20"/>
+      <c r="M70" s="17"/>
+      <c r="N70" s="17"/>
+      <c r="O70" s="17"/>
+      <c r="P70" s="17"/>
       <c r="Q70" s="27"/>
       <c r="R70"/>
     </row>
-    <row r="71" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A71" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="B71" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C71" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="D71" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E71" s="2" t="b">
-        <v>0</v>
+    <row r="71" spans="1:18" s="24" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A71" s="24" t="s">
+        <v>255</v>
+      </c>
+      <c r="B71" s="24" t="s">
+        <v>5</v>
+      </c>
+      <c r="C71" s="24" t="s">
+        <v>257</v>
+      </c>
+      <c r="D71" s="24" t="b">
+        <v>0</v>
+      </c>
+      <c r="E71" s="24" t="b">
+        <v>1</v>
+      </c>
+      <c r="F71" s="24" t="s">
+        <v>256</v>
       </c>
       <c r="G71" s="20"/>
-      <c r="H71" s="2" t="s">
-        <v>282</v>
-      </c>
-      <c r="I71" s="39" t="s">
-        <v>282</v>
-      </c>
-      <c r="J71" s="39" t="s">
-        <v>282</v>
-      </c>
-      <c r="K71" s="39" t="s">
-        <v>282</v>
-      </c>
       <c r="L71" s="20"/>
-      <c r="M71" s="39" t="s">
-        <v>283</v>
-      </c>
-      <c r="N71" s="39" t="s">
-        <v>283</v>
-      </c>
-      <c r="O71" s="39" t="s">
-        <v>283</v>
-      </c>
-      <c r="P71" s="39" t="s">
-        <v>283</v>
-      </c>
       <c r="Q71" s="27"/>
       <c r="R71"/>
     </row>
     <row r="72" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A72" s="48" t="s">
-        <v>195</v>
-      </c>
-      <c r="B72" s="48" t="s">
+      <c r="A72" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="B72" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C72" s="48" t="s">
-        <v>318</v>
-      </c>
-      <c r="D72" s="48" t="b">
-        <v>0</v>
-      </c>
-      <c r="E72" s="48" t="b">
-        <v>1</v>
+      <c r="C72" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="D72" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E72" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="G72" s="20"/>
+      <c r="H72" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="I72" s="39" t="s">
+        <v>282</v>
+      </c>
+      <c r="J72" s="39" t="s">
+        <v>282</v>
+      </c>
+      <c r="K72" s="39" t="s">
+        <v>282</v>
+      </c>
       <c r="L72" s="20"/>
-      <c r="M72" s="17"/>
-      <c r="N72" s="17"/>
-      <c r="O72" s="17"/>
-      <c r="P72" s="17"/>
+      <c r="M72" s="39" t="s">
+        <v>283</v>
+      </c>
+      <c r="N72" s="39" t="s">
+        <v>283</v>
+      </c>
+      <c r="O72" s="39" t="s">
+        <v>283</v>
+      </c>
+      <c r="P72" s="39" t="s">
+        <v>283</v>
+      </c>
       <c r="Q72" s="27"/>
       <c r="R72"/>
     </row>
-    <row r="73" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A73" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="B73" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="C73" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="D73" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="E73" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="F73" s="7" t="s">
-        <v>16</v>
+    <row r="73" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A73" s="48" t="s">
+        <v>195</v>
+      </c>
+      <c r="B73" s="48" t="s">
+        <v>10</v>
+      </c>
+      <c r="C73" s="48" t="s">
+        <v>318</v>
+      </c>
+      <c r="D73" s="48" t="b">
+        <v>0</v>
+      </c>
+      <c r="E73" s="48" t="b">
+        <v>1</v>
       </c>
       <c r="G73" s="20"/>
       <c r="L73" s="20"/>
+      <c r="M73" s="17"/>
+      <c r="N73" s="17"/>
+      <c r="O73" s="17"/>
+      <c r="P73" s="17"/>
       <c r="Q73" s="27"/>
       <c r="R73"/>
     </row>
-    <row r="74" spans="1:18" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A74" s="44" t="s">
+    <row r="74" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A74" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="B74" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C74" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="D74" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="E74" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="F74" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="G74" s="20"/>
+      <c r="L74" s="20"/>
+      <c r="Q74" s="27"/>
+      <c r="R74"/>
+    </row>
+    <row r="75" spans="1:18" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A75" s="44" t="s">
         <v>321</v>
       </c>
-      <c r="B74" s="44" t="s">
+      <c r="B75" s="44" t="s">
         <v>5</v>
       </c>
-      <c r="C74" s="44" t="s">
+      <c r="C75" s="44" t="s">
         <v>322</v>
       </c>
-      <c r="D74" s="50" t="b">
-        <v>0</v>
-      </c>
-      <c r="E74" s="50" t="b">
-        <v>1</v>
-      </c>
-      <c r="F74" s="50" t="s">
-        <v>4</v>
-      </c>
-      <c r="G74" s="27"/>
-      <c r="L74" s="27"/>
-      <c r="Q74" s="27"/>
-    </row>
-    <row r="75" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A75" s="2" t="s">
-        <v>219</v>
-      </c>
-      <c r="B75" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C75" s="2" t="s">
-        <v>231</v>
-      </c>
-      <c r="D75" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E75" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F75" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="G75" s="20"/>
-      <c r="L75" s="20"/>
-      <c r="M75" s="17"/>
-      <c r="N75" s="17"/>
-      <c r="O75" s="17"/>
-      <c r="P75" s="17"/>
+      <c r="D75" s="50" t="b">
+        <v>0</v>
+      </c>
+      <c r="E75" s="50" t="b">
+        <v>1</v>
+      </c>
+      <c r="F75" s="50" t="s">
+        <v>4</v>
+      </c>
+      <c r="G75" s="27"/>
+      <c r="L75" s="27"/>
       <c r="Q75" s="27"/>
-      <c r="R75"/>
     </row>
     <row r="76" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A76" s="2" t="s">
-        <v>77</v>
+        <v>219</v>
       </c>
       <c r="B76" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>78</v>
+        <v>231</v>
       </c>
       <c r="D76" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E76" s="2" t="b">
         <v>0</v>
       </c>
       <c r="F76" s="2" t="s">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="G76" s="20"/>
       <c r="L76" s="20"/>
@@ -3863,453 +3888,453 @@
       <c r="Q76" s="27"/>
       <c r="R76"/>
     </row>
-    <row r="77" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="77" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A77" s="2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D77" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E77" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="F77" s="33"/>
+      <c r="F77" s="2" t="s">
+        <v>4</v>
+      </c>
       <c r="G77" s="20"/>
-      <c r="H77" s="38" t="s">
-        <v>280</v>
-      </c>
-      <c r="I77" s="38" t="s">
-        <v>280</v>
-      </c>
-      <c r="J77" s="38" t="s">
-        <v>280</v>
-      </c>
-      <c r="K77" s="38" t="s">
-        <v>280</v>
-      </c>
-      <c r="L77" s="27"/>
-      <c r="M77" s="38" t="s">
-        <v>281</v>
-      </c>
-      <c r="N77" s="38" t="s">
-        <v>281</v>
-      </c>
-      <c r="O77" s="38" t="s">
-        <v>281</v>
-      </c>
-      <c r="P77" s="38" t="s">
-        <v>281</v>
-      </c>
+      <c r="L77" s="20"/>
+      <c r="M77" s="17"/>
+      <c r="N77" s="17"/>
+      <c r="O77" s="17"/>
+      <c r="P77" s="17"/>
       <c r="Q77" s="27"/>
       <c r="R77"/>
     </row>
-    <row r="78" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="78" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A78" s="2" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>82</v>
+        <v>10</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="D78" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E78" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="F78" s="2" t="s">
-        <v>311</v>
-      </c>
+      <c r="F78" s="33"/>
       <c r="G78" s="20"/>
-      <c r="L78" s="20"/>
-      <c r="M78" s="17"/>
-      <c r="N78" s="17"/>
-      <c r="O78" s="17"/>
-      <c r="P78" s="17"/>
+      <c r="H78" s="38" t="s">
+        <v>280</v>
+      </c>
+      <c r="I78" s="38" t="s">
+        <v>280</v>
+      </c>
+      <c r="J78" s="38" t="s">
+        <v>280</v>
+      </c>
+      <c r="K78" s="38" t="s">
+        <v>280</v>
+      </c>
+      <c r="L78" s="27"/>
+      <c r="M78" s="38" t="s">
+        <v>281</v>
+      </c>
+      <c r="N78" s="38" t="s">
+        <v>281</v>
+      </c>
+      <c r="O78" s="38" t="s">
+        <v>281</v>
+      </c>
+      <c r="P78" s="38" t="s">
+        <v>281</v>
+      </c>
       <c r="Q78" s="27"/>
       <c r="R78"/>
     </row>
-    <row r="79" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A79" s="7" t="s">
-        <v>84</v>
-      </c>
-      <c r="B79" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="C79" s="7" t="s">
-        <v>85</v>
-      </c>
-      <c r="D79" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="E79" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="F79" s="7" t="s">
-        <v>284</v>
+    <row r="79" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A79" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="B79" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="C79" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="D79" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E79" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F79" s="2" t="s">
+        <v>311</v>
       </c>
       <c r="G79" s="20"/>
       <c r="L79" s="20"/>
+      <c r="M79" s="17"/>
+      <c r="N79" s="17"/>
+      <c r="O79" s="17"/>
+      <c r="P79" s="17"/>
       <c r="Q79" s="27"/>
       <c r="R79"/>
     </row>
-    <row r="80" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A80" s="2" t="s">
-        <v>196</v>
-      </c>
-      <c r="B80" s="2" t="s">
-        <v>197</v>
-      </c>
-      <c r="C80" s="2" t="s">
-        <v>198</v>
-      </c>
-      <c r="D80" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E80" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F80" s="2" t="s">
-        <v>19</v>
+    <row r="80" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A80" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="B80" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C80" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="D80" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="E80" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="F80" s="7" t="s">
+        <v>284</v>
       </c>
       <c r="G80" s="20"/>
-      <c r="I80" s="2" t="s">
-        <v>310</v>
-      </c>
-      <c r="J80" s="2" t="s">
-        <v>310</v>
-      </c>
-      <c r="K80" s="2" t="s">
-        <v>310</v>
-      </c>
       <c r="L80" s="20"/>
-      <c r="M80" s="17"/>
-      <c r="N80" s="17"/>
-      <c r="O80" s="17"/>
-      <c r="P80" s="17"/>
       <c r="Q80" s="27"/>
       <c r="R80"/>
     </row>
-    <row r="81" spans="1:18" s="7" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
-      <c r="A81" s="7" t="s">
-        <v>199</v>
-      </c>
-      <c r="B81" s="7" t="s">
-        <v>178</v>
-      </c>
-      <c r="C81" s="7" t="s">
-        <v>200</v>
-      </c>
-      <c r="D81" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="E81" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="F81" s="7" t="s">
-        <v>212</v>
+    <row r="81" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A81" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="B81" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="C81" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="D81" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E81" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F81" s="2" t="s">
+        <v>19</v>
       </c>
       <c r="G81" s="20"/>
+      <c r="I81" s="2" t="s">
+        <v>310</v>
+      </c>
+      <c r="J81" s="2" t="s">
+        <v>310</v>
+      </c>
+      <c r="K81" s="2" t="s">
+        <v>310</v>
+      </c>
       <c r="L81" s="20"/>
+      <c r="M81" s="17"/>
+      <c r="N81" s="17"/>
+      <c r="O81" s="17"/>
+      <c r="P81" s="17"/>
       <c r="Q81" s="27"/>
       <c r="R81"/>
     </row>
-    <row r="82" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A82" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="B82" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C82" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="D82" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E82" s="2" t="b">
-        <v>0</v>
+    <row r="82" spans="1:18" s="7" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="A82" s="7" t="s">
+        <v>199</v>
+      </c>
+      <c r="B82" s="7" t="s">
+        <v>178</v>
+      </c>
+      <c r="C82" s="7" t="s">
+        <v>200</v>
+      </c>
+      <c r="D82" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="E82" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="F82" s="7" t="s">
+        <v>212</v>
       </c>
       <c r="G82" s="20"/>
-      <c r="H82" s="38" t="s">
-        <v>280</v>
-      </c>
-      <c r="I82" s="38" t="s">
-        <v>280</v>
-      </c>
-      <c r="J82" s="38" t="s">
-        <v>280</v>
-      </c>
-      <c r="K82" s="38" t="s">
-        <v>280</v>
-      </c>
-      <c r="L82" s="27"/>
-      <c r="M82" s="38" t="s">
-        <v>281</v>
-      </c>
-      <c r="N82" s="38" t="s">
-        <v>281</v>
-      </c>
-      <c r="O82" s="38" t="s">
-        <v>281</v>
-      </c>
-      <c r="P82" s="38" t="s">
-        <v>281</v>
-      </c>
+      <c r="L82" s="20"/>
       <c r="Q82" s="27"/>
       <c r="R82"/>
     </row>
     <row r="83" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A83" s="2" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>90</v>
+        <v>10</v>
       </c>
       <c r="C83" s="2" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="D83" s="2" t="b">
         <v>1</v>
       </c>
       <c r="E83" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F83" s="2" t="s">
-        <v>89</v>
+        <v>0</v>
       </c>
       <c r="G83" s="20"/>
-      <c r="L83" s="20"/>
-      <c r="M83" s="17"/>
-      <c r="N83" s="17"/>
-      <c r="O83" s="17"/>
-      <c r="P83" s="17"/>
+      <c r="H83" s="38" t="s">
+        <v>280</v>
+      </c>
+      <c r="I83" s="38" t="s">
+        <v>280</v>
+      </c>
+      <c r="J83" s="38" t="s">
+        <v>280</v>
+      </c>
+      <c r="K83" s="38" t="s">
+        <v>280</v>
+      </c>
+      <c r="L83" s="27"/>
+      <c r="M83" s="38" t="s">
+        <v>281</v>
+      </c>
+      <c r="N83" s="38" t="s">
+        <v>281</v>
+      </c>
+      <c r="O83" s="38" t="s">
+        <v>281</v>
+      </c>
+      <c r="P83" s="38" t="s">
+        <v>281</v>
+      </c>
       <c r="Q83" s="27"/>
       <c r="R83"/>
     </row>
-    <row r="84" spans="1:18" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A84" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="B84" s="7" t="s">
-        <v>94</v>
-      </c>
-      <c r="C84" s="7" t="s">
-        <v>95</v>
-      </c>
-      <c r="D84" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="E84" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="F84" s="7" t="s">
-        <v>93</v>
+    <row r="84" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A84" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="B84" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="C84" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="D84" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E84" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F84" s="2" t="s">
+        <v>89</v>
       </c>
       <c r="G84" s="20"/>
       <c r="L84" s="20"/>
+      <c r="M84" s="17"/>
+      <c r="N84" s="17"/>
+      <c r="O84" s="17"/>
+      <c r="P84" s="17"/>
       <c r="Q84" s="27"/>
       <c r="R84"/>
     </row>
     <row r="85" spans="1:18" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A85" s="7" t="s">
-        <v>149</v>
+        <v>92</v>
       </c>
       <c r="B85" s="7" t="s">
-        <v>5</v>
+        <v>94</v>
       </c>
       <c r="C85" s="7" t="s">
-        <v>150</v>
+        <v>95</v>
       </c>
       <c r="D85" s="7" t="b">
         <v>0</v>
       </c>
       <c r="E85" s="7" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F85" s="7" t="s">
-        <v>16</v>
+        <v>93</v>
       </c>
       <c r="G85" s="20"/>
       <c r="L85" s="20"/>
       <c r="Q85" s="27"/>
       <c r="R85"/>
     </row>
-    <row r="86" spans="1:18" s="2" customFormat="1" ht="58.3" x14ac:dyDescent="0.4">
-      <c r="A86" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="B86" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="C86" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="D86" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E86" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F86" s="2" t="s">
-        <v>97</v>
+    <row r="86" spans="1:18" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A86" s="7" t="s">
+        <v>149</v>
+      </c>
+      <c r="B86" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C86" s="7" t="s">
+        <v>150</v>
+      </c>
+      <c r="D86" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="E86" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="F86" s="7" t="s">
+        <v>16</v>
       </c>
       <c r="G86" s="20"/>
       <c r="L86" s="20"/>
-      <c r="M86" s="17"/>
-      <c r="N86" s="17"/>
-      <c r="O86" s="17"/>
-      <c r="P86" s="17"/>
       <c r="Q86" s="27"/>
       <c r="R86"/>
     </row>
-    <row r="87" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="87" spans="1:18" s="2" customFormat="1" ht="58.3" x14ac:dyDescent="0.4">
       <c r="A87" s="2" t="s">
-        <v>226</v>
-      </c>
-      <c r="B87" s="8"/>
-      <c r="C87" s="8"/>
+        <v>96</v>
+      </c>
+      <c r="B87" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="C87" s="2" t="s">
+        <v>98</v>
+      </c>
       <c r="D87" s="2" t="b">
         <v>1</v>
       </c>
       <c r="E87" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="F87" s="2" t="s">
+        <v>97</v>
       </c>
       <c r="G87" s="20"/>
-      <c r="H87" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="I87" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="J87" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="K87" s="2" t="s">
-        <v>4</v>
-      </c>
       <c r="L87" s="20"/>
-      <c r="M87" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="N87" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="O87" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="P87" s="17" t="s">
-        <v>4</v>
-      </c>
+      <c r="M87" s="17"/>
+      <c r="N87" s="17"/>
+      <c r="O87" s="17"/>
+      <c r="P87" s="17"/>
       <c r="Q87" s="27"/>
       <c r="R87"/>
     </row>
     <row r="88" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A88" s="2" t="s">
-        <v>151</v>
-      </c>
-      <c r="B88" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C88" s="2" t="s">
-        <v>152</v>
-      </c>
+        <v>226</v>
+      </c>
+      <c r="B88" s="8"/>
+      <c r="C88" s="8"/>
       <c r="D88" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E88" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="F88" s="2" t="s">
-        <v>4</v>
-      </c>
       <c r="G88" s="20"/>
+      <c r="H88" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I88" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="J88" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="K88" s="2" t="s">
+        <v>4</v>
+      </c>
       <c r="L88" s="20"/>
-      <c r="M88" s="17"/>
-      <c r="N88" s="17"/>
-      <c r="O88" s="17"/>
-      <c r="P88" s="17"/>
+      <c r="M88" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="N88" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="O88" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="P88" s="17" t="s">
+        <v>4</v>
+      </c>
       <c r="Q88" s="27"/>
       <c r="R88"/>
     </row>
-    <row r="89" spans="1:18" s="31" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A89" s="31" t="s">
-        <v>99</v>
-      </c>
-      <c r="B89" s="31" t="s">
-        <v>10</v>
-      </c>
-      <c r="C89" s="31" t="s">
-        <v>100</v>
-      </c>
-      <c r="D89" s="31" t="b">
-        <v>1</v>
-      </c>
-      <c r="E89" s="31" t="b">
-        <v>0</v>
-      </c>
-      <c r="F89" s="31" t="s">
-        <v>269</v>
-      </c>
-      <c r="G89" s="27"/>
-      <c r="L89" s="27"/>
+    <row r="89" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A89" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="B89" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C89" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="D89" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E89" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F89" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G89" s="20"/>
+      <c r="L89" s="20"/>
+      <c r="M89" s="17"/>
+      <c r="N89" s="17"/>
+      <c r="O89" s="17"/>
+      <c r="P89" s="17"/>
       <c r="Q89" s="27"/>
       <c r="R89"/>
     </row>
-    <row r="90" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A90" s="2" t="s">
-        <v>201</v>
-      </c>
-      <c r="B90" s="2" t="s">
-        <v>202</v>
-      </c>
-      <c r="C90" s="2" t="s">
-        <v>203</v>
-      </c>
-      <c r="D90" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E90" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F90" s="12" t="s">
-        <v>253</v>
-      </c>
-      <c r="G90" s="20"/>
-      <c r="L90" s="20"/>
-      <c r="M90" s="17"/>
-      <c r="N90" s="17"/>
-      <c r="O90" s="17"/>
-      <c r="P90" s="17"/>
+    <row r="90" spans="1:18" s="31" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A90" s="31" t="s">
+        <v>99</v>
+      </c>
+      <c r="B90" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="C90" s="31" t="s">
+        <v>100</v>
+      </c>
+      <c r="D90" s="31" t="b">
+        <v>1</v>
+      </c>
+      <c r="E90" s="31" t="b">
+        <v>0</v>
+      </c>
+      <c r="F90" s="31" t="s">
+        <v>269</v>
+      </c>
+      <c r="G90" s="27"/>
+      <c r="L90" s="27"/>
       <c r="Q90" s="27"/>
       <c r="R90"/>
     </row>
-    <row r="91" spans="1:18" s="14" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A91" s="14" t="s">
-        <v>249</v>
-      </c>
-      <c r="B91" s="14" t="s">
-        <v>250</v>
-      </c>
-      <c r="C91" s="14" t="s">
-        <v>251</v>
-      </c>
-      <c r="D91" s="14" t="b">
-        <v>0</v>
-      </c>
-      <c r="E91" s="14" t="b">
-        <v>1</v>
-      </c>
-      <c r="F91" s="6" t="s">
-        <v>252</v>
+    <row r="91" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A91" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="B91" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="C91" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="D91" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E91" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F91" s="12" t="s">
+        <v>253</v>
       </c>
       <c r="G91" s="20"/>
       <c r="L91" s="20"/>
@@ -4320,122 +4345,122 @@
       <c r="Q91" s="27"/>
       <c r="R91"/>
     </row>
-    <row r="92" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A92" s="2" t="s">
-        <v>222</v>
-      </c>
-      <c r="B92" s="8"/>
-      <c r="C92" s="8"/>
-      <c r="D92" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E92" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F92" s="17" t="s">
-        <v>284</v>
+    <row r="92" spans="1:18" s="14" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A92" s="14" t="s">
+        <v>249</v>
+      </c>
+      <c r="B92" s="14" t="s">
+        <v>250</v>
+      </c>
+      <c r="C92" s="14" t="s">
+        <v>251</v>
+      </c>
+      <c r="D92" s="14" t="b">
+        <v>0</v>
+      </c>
+      <c r="E92" s="14" t="b">
+        <v>1</v>
+      </c>
+      <c r="F92" s="6" t="s">
+        <v>252</v>
       </c>
       <c r="G92" s="20"/>
-      <c r="I92" s="35"/>
-      <c r="J92" s="35"/>
-      <c r="K92" s="35"/>
       <c r="L92" s="20"/>
-      <c r="M92" s="35"/>
-      <c r="N92" s="35"/>
-      <c r="O92" s="35"/>
-      <c r="P92" s="35"/>
+      <c r="M92" s="17"/>
+      <c r="N92" s="17"/>
+      <c r="O92" s="17"/>
+      <c r="P92" s="17"/>
       <c r="Q92" s="27"/>
       <c r="R92"/>
     </row>
-    <row r="93" spans="1:18" s="2" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="93" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A93" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="B93" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C93" s="2" t="s">
-        <v>102</v>
-      </c>
+        <v>222</v>
+      </c>
+      <c r="B93" s="8"/>
+      <c r="C93" s="8"/>
       <c r="D93" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E93" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="F93" s="2" t="s">
-        <v>16</v>
+      <c r="F93" s="17" t="s">
+        <v>284</v>
       </c>
       <c r="G93" s="20"/>
+      <c r="I93" s="35"/>
+      <c r="J93" s="35"/>
+      <c r="K93" s="35"/>
       <c r="L93" s="20"/>
-      <c r="M93" s="17"/>
-      <c r="N93" s="17"/>
-      <c r="O93" s="17"/>
-      <c r="P93" s="17"/>
+      <c r="M93" s="35"/>
+      <c r="N93" s="35"/>
+      <c r="O93" s="35"/>
+      <c r="P93" s="35"/>
       <c r="Q93" s="27"/>
       <c r="R93"/>
     </row>
-    <row r="94" spans="1:18" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A94" t="s">
-        <v>293</v>
-      </c>
-      <c r="B94" t="s">
-        <v>10</v>
-      </c>
-      <c r="C94" t="s">
-        <v>294</v>
-      </c>
-      <c r="D94" t="b">
-        <v>1</v>
-      </c>
-      <c r="E94" t="b">
-        <v>1</v>
-      </c>
-      <c r="F94" t="s">
-        <v>284</v>
-      </c>
-      <c r="G94" s="27"/>
-      <c r="L94" s="27"/>
+    <row r="94" spans="1:18" s="2" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A94" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="B94" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C94" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="D94" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E94" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F94" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G94" s="20"/>
+      <c r="L94" s="20"/>
+      <c r="M94" s="17"/>
+      <c r="N94" s="17"/>
+      <c r="O94" s="17"/>
+      <c r="P94" s="17"/>
       <c r="Q94" s="27"/>
       <c r="R94"/>
     </row>
-    <row r="95" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A95" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="B95" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="C95" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="D95" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E95" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F95" s="6" t="s">
-        <v>213</v>
-      </c>
-      <c r="G95" s="20"/>
-      <c r="L95" s="20"/>
-      <c r="M95" s="17"/>
-      <c r="N95" s="17"/>
-      <c r="O95" s="17"/>
-      <c r="P95" s="17"/>
+    <row r="95" spans="1:18" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A95" t="s">
+        <v>293</v>
+      </c>
+      <c r="B95" t="s">
+        <v>10</v>
+      </c>
+      <c r="C95" t="s">
+        <v>294</v>
+      </c>
+      <c r="D95" t="b">
+        <v>1</v>
+      </c>
+      <c r="E95" t="b">
+        <v>1</v>
+      </c>
+      <c r="F95" t="s">
+        <v>284</v>
+      </c>
+      <c r="G95" s="27"/>
+      <c r="L95" s="27"/>
       <c r="Q95" s="27"/>
       <c r="R95"/>
     </row>
     <row r="96" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A96" s="2" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B96" s="2" t="s">
-        <v>5</v>
+        <v>56</v>
       </c>
       <c r="C96" s="2" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D96" s="2" t="b">
         <v>0</v>
@@ -4443,8 +4468,8 @@
       <c r="E96" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="F96" s="2" t="s">
-        <v>16</v>
+      <c r="F96" s="6" t="s">
+        <v>213</v>
       </c>
       <c r="G96" s="20"/>
       <c r="L96" s="20"/>
@@ -4455,21 +4480,24 @@
       <c r="Q96" s="27"/>
       <c r="R96"/>
     </row>
-    <row r="97" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="97" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A97" s="2" t="s">
-        <v>204</v>
+        <v>105</v>
       </c>
       <c r="B97" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C97" s="2" t="s">
-        <v>205</v>
+        <v>106</v>
       </c>
       <c r="D97" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E97" s="2" t="b">
         <v>1</v>
+      </c>
+      <c r="F97" s="2" t="s">
+        <v>16</v>
       </c>
       <c r="G97" s="20"/>
       <c r="L97" s="20"/>
@@ -4482,22 +4510,19 @@
     </row>
     <row r="98" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A98" s="2" t="s">
-        <v>107</v>
+        <v>204</v>
       </c>
       <c r="B98" s="2" t="s">
-        <v>109</v>
+        <v>5</v>
       </c>
       <c r="C98" s="2" t="s">
-        <v>110</v>
+        <v>205</v>
       </c>
       <c r="D98" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E98" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F98" s="2" t="s">
-        <v>108</v>
+        <v>1</v>
       </c>
       <c r="G98" s="20"/>
       <c r="L98" s="20"/>
@@ -4508,15 +4533,15 @@
       <c r="Q98" s="27"/>
       <c r="R98"/>
     </row>
-    <row r="99" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="99" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A99" s="2" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="B99" s="2" t="s">
-        <v>10</v>
+        <v>109</v>
       </c>
       <c r="C99" s="2" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D99" s="2" t="b">
         <v>1</v>
@@ -4524,68 +4549,72 @@
       <c r="E99" s="2" t="b">
         <v>0</v>
       </c>
+      <c r="F99" s="2" t="s">
+        <v>108</v>
+      </c>
       <c r="G99" s="20"/>
-      <c r="H99" s="38" t="s">
-        <v>280</v>
-      </c>
-      <c r="I99" s="38" t="s">
-        <v>280</v>
-      </c>
-      <c r="J99" s="38" t="s">
-        <v>280</v>
-      </c>
-      <c r="K99" s="38" t="s">
-        <v>280</v>
-      </c>
-      <c r="L99" s="27"/>
-      <c r="M99" s="38" t="s">
-        <v>281</v>
-      </c>
-      <c r="N99" s="38" t="s">
-        <v>281</v>
-      </c>
-      <c r="O99" s="38" t="s">
-        <v>281</v>
-      </c>
-      <c r="P99" s="38" t="s">
-        <v>281</v>
-      </c>
+      <c r="L99" s="20"/>
+      <c r="M99" s="17"/>
+      <c r="N99" s="17"/>
+      <c r="O99" s="17"/>
+      <c r="P99" s="17"/>
       <c r="Q99" s="27"/>
       <c r="R99"/>
     </row>
-    <row r="100" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A100" s="7" t="s">
-        <v>113</v>
-      </c>
-      <c r="B100" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="C100" s="7" t="s">
-        <v>114</v>
-      </c>
-      <c r="D100" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="E100" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="F100" s="7" t="s">
-        <v>220</v>
+    <row r="100" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A100" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="B100" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C100" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="D100" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E100" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="G100" s="20"/>
-      <c r="L100" s="20"/>
+      <c r="H100" s="38" t="s">
+        <v>280</v>
+      </c>
+      <c r="I100" s="38" t="s">
+        <v>280</v>
+      </c>
+      <c r="J100" s="38" t="s">
+        <v>280</v>
+      </c>
+      <c r="K100" s="38" t="s">
+        <v>280</v>
+      </c>
+      <c r="L100" s="27"/>
+      <c r="M100" s="38" t="s">
+        <v>281</v>
+      </c>
+      <c r="N100" s="38" t="s">
+        <v>281</v>
+      </c>
+      <c r="O100" s="38" t="s">
+        <v>281</v>
+      </c>
+      <c r="P100" s="38" t="s">
+        <v>281</v>
+      </c>
       <c r="Q100" s="27"/>
       <c r="R100"/>
     </row>
     <row r="101" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A101" s="7" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B101" s="7" t="s">
-        <v>67</v>
+        <v>12</v>
       </c>
       <c r="C101" s="7" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="D101" s="7" t="b">
         <v>1</v>
@@ -4603,85 +4632,64 @@
     </row>
     <row r="102" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A102" s="7" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B102" s="7" t="s">
-        <v>5</v>
+        <v>67</v>
       </c>
       <c r="C102" s="7" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="D102" s="7" t="b">
         <v>1</v>
       </c>
       <c r="E102" s="7" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F102" s="7" t="s">
-        <v>16</v>
+        <v>220</v>
       </c>
       <c r="G102" s="20"/>
       <c r="L102" s="20"/>
       <c r="Q102" s="27"/>
       <c r="R102"/>
     </row>
-    <row r="103" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A103" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="B103" s="2" t="s">
+    <row r="103" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A103" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="B103" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C103" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="D103" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E103" s="2" t="b">
-        <v>1</v>
+      <c r="C103" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="D103" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="E103" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="F103" s="7" t="s">
+        <v>16</v>
       </c>
       <c r="G103" s="20"/>
-      <c r="H103" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="I103" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="J103" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="K103" s="2" t="s">
-        <v>4</v>
-      </c>
       <c r="L103" s="20"/>
-      <c r="M103" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="N103" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="O103" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="P103" s="17" t="s">
-        <v>4</v>
-      </c>
       <c r="Q103" s="27"/>
       <c r="R103"/>
     </row>
     <row r="104" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A104" s="2" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B104" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C104" s="2" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="D104" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E104" s="2" t="b">
         <v>1</v>
@@ -4717,23 +4725,23 @@
     </row>
     <row r="105" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A105" s="2" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B105" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C105" s="2" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="D105" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E105" s="2" t="b">
         <v>1</v>
       </c>
       <c r="G105" s="20"/>
       <c r="H105" s="2" t="s">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="I105" s="2" t="s">
         <v>4</v>
@@ -4746,7 +4754,7 @@
       </c>
       <c r="L105" s="20"/>
       <c r="M105" s="17" t="s">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="N105" s="17" t="s">
         <v>4</v>
@@ -4760,15 +4768,15 @@
       <c r="Q105" s="27"/>
       <c r="R105"/>
     </row>
-    <row r="106" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="106" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A106" s="2" t="s">
-        <v>153</v>
+        <v>123</v>
       </c>
       <c r="B106" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C106" s="2" t="s">
-        <v>154</v>
+        <v>124</v>
       </c>
       <c r="D106" s="2" t="b">
         <v>0</v>
@@ -4781,7 +4789,7 @@
         <v>16</v>
       </c>
       <c r="I106" s="2" t="s">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="J106" s="2" t="s">
         <v>4</v>
@@ -4794,7 +4802,7 @@
         <v>16</v>
       </c>
       <c r="N106" s="17" t="s">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="O106" s="17" t="s">
         <v>4</v>
@@ -4803,134 +4811,135 @@
         <v>4</v>
       </c>
       <c r="Q106" s="27"/>
-      <c r="R106" t="s">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="107" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A107" t="s">
-        <v>295</v>
-      </c>
-      <c r="B107" t="s">
+      <c r="R106"/>
+    </row>
+    <row r="107" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A107" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="B107" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C107" t="s">
-        <v>296</v>
-      </c>
-      <c r="D107" t="b">
-        <v>0</v>
-      </c>
-      <c r="E107" t="b">
-        <v>1</v>
-      </c>
-      <c r="F107"/>
-      <c r="G107" s="27"/>
-      <c r="H107" t="s">
-        <v>16</v>
-      </c>
-      <c r="I107" t="s">
-        <v>16</v>
-      </c>
-      <c r="J107" t="s">
-        <v>4</v>
-      </c>
-      <c r="K107" t="s">
-        <v>4</v>
-      </c>
-      <c r="L107" s="27"/>
-      <c r="M107" t="s">
-        <v>16</v>
-      </c>
-      <c r="N107" t="s">
-        <v>16</v>
-      </c>
-      <c r="O107" t="s">
-        <v>4</v>
-      </c>
-      <c r="P107" t="s">
+      <c r="C107" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="D107" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E107" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="G107" s="20"/>
+      <c r="H107" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I107" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="J107" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="K107" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="L107" s="20"/>
+      <c r="M107" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="N107" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="O107" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="P107" s="17" t="s">
         <v>4</v>
       </c>
       <c r="Q107" s="27"/>
       <c r="R107" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="108" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A108" t="s">
+        <v>295</v>
+      </c>
+      <c r="B108" t="s">
+        <v>5</v>
+      </c>
+      <c r="C108" t="s">
+        <v>296</v>
+      </c>
+      <c r="D108" t="b">
+        <v>0</v>
+      </c>
+      <c r="E108" t="b">
+        <v>1</v>
+      </c>
+      <c r="F108"/>
+      <c r="G108" s="27"/>
+      <c r="H108" t="s">
+        <v>16</v>
+      </c>
+      <c r="I108" t="s">
+        <v>16</v>
+      </c>
+      <c r="J108" t="s">
+        <v>4</v>
+      </c>
+      <c r="K108" t="s">
+        <v>4</v>
+      </c>
+      <c r="L108" s="27"/>
+      <c r="M108" t="s">
+        <v>16</v>
+      </c>
+      <c r="N108" t="s">
+        <v>16</v>
+      </c>
+      <c r="O108" t="s">
+        <v>4</v>
+      </c>
+      <c r="P108" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q108" s="27"/>
+      <c r="R108" t="s">
         <v>298</v>
       </c>
     </row>
-    <row r="108" spans="1:18" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A108" s="7" t="s">
+    <row r="109" spans="1:18" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A109" s="7" t="s">
         <v>125</v>
       </c>
-      <c r="B108" s="7" t="s">
+      <c r="B109" s="7" t="s">
         <v>126</v>
       </c>
-      <c r="C108" s="7" t="s">
+      <c r="C109" s="7" t="s">
         <v>127</v>
       </c>
-      <c r="D108" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="E108" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="F108" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="G108" s="20"/>
-      <c r="L108" s="20"/>
-      <c r="Q108" s="27"/>
-    </row>
-    <row r="109" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A109" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="B109" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C109" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="D109" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E109" s="2" t="b">
-        <v>1</v>
+      <c r="D109" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="E109" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="F109" s="7" t="s">
+        <v>16</v>
       </c>
       <c r="G109" s="20"/>
-      <c r="H109" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="I109" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="J109" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="K109" s="2" t="s">
-        <v>4</v>
-      </c>
       <c r="L109" s="20"/>
-      <c r="M109" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="N109" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="O109" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="P109" s="17" t="s">
-        <v>4</v>
-      </c>
       <c r="Q109" s="27"/>
     </row>
     <row r="110" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A110" s="2" t="s">
-        <v>240</v>
+        <v>128</v>
       </c>
       <c r="B110" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C110" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D110" s="2" t="b">
         <v>1</v>
@@ -4968,132 +4977,173 @@
     </row>
     <row r="111" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A111" s="2" t="s">
+        <v>240</v>
+      </c>
+      <c r="B111" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C111" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="D111" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E111" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="G111" s="20"/>
+      <c r="H111" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I111" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="J111" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="K111" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="L111" s="20"/>
+      <c r="M111" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="N111" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="O111" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="P111" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q111" s="27"/>
+    </row>
+    <row r="112" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A112" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="B111" s="2" t="s">
+      <c r="B112" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C111" s="2" t="s">
+      <c r="C112" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="D111" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E111" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F111" s="2" t="s">
+      <c r="D112" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E112" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F112" s="2" t="s">
         <v>284</v>
       </c>
-      <c r="G111" s="20"/>
-      <c r="L111" s="20"/>
-      <c r="M111" s="17"/>
-      <c r="N111" s="17"/>
-      <c r="O111" s="17"/>
-      <c r="P111" s="17"/>
-      <c r="Q111" s="27"/>
-    </row>
-    <row r="112" spans="1:18" s="49" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A112" s="49" t="s">
+      <c r="G112" s="20"/>
+      <c r="L112" s="20"/>
+      <c r="M112" s="17"/>
+      <c r="N112" s="17"/>
+      <c r="O112" s="17"/>
+      <c r="P112" s="17"/>
+      <c r="Q112" s="27"/>
+    </row>
+    <row r="113" spans="1:18" s="49" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A113" s="49" t="s">
         <v>319</v>
       </c>
-      <c r="B112" s="49" t="s">
+      <c r="B113" s="49" t="s">
         <v>10</v>
       </c>
-      <c r="C112" s="49" t="s">
+      <c r="C113" s="49" t="s">
         <v>320</v>
       </c>
-      <c r="D112" s="49" t="b">
-        <v>1</v>
-      </c>
-      <c r="E112" s="49" t="b">
-        <v>1</v>
-      </c>
-      <c r="G112" s="27"/>
-      <c r="H112" s="49" t="s">
+      <c r="D113" s="49" t="b">
+        <v>1</v>
+      </c>
+      <c r="E113" s="49" t="b">
+        <v>1</v>
+      </c>
+      <c r="G113" s="27"/>
+      <c r="H113" s="49" t="s">
         <v>280</v>
       </c>
-      <c r="I112" s="49" t="s">
+      <c r="I113" s="49" t="s">
         <v>280</v>
       </c>
-      <c r="J112" s="49" t="s">
+      <c r="J113" s="49" t="s">
         <v>280</v>
       </c>
-      <c r="K112" s="49" t="s">
+      <c r="K113" s="49" t="s">
         <v>280</v>
       </c>
-      <c r="L112" s="27"/>
-      <c r="M112" s="49" t="s">
+      <c r="L113" s="27"/>
+      <c r="M113" s="49" t="s">
         <v>281</v>
       </c>
-      <c r="N112" s="49" t="s">
+      <c r="N113" s="49" t="s">
         <v>281</v>
       </c>
-      <c r="O112" s="49" t="s">
+      <c r="O113" s="49" t="s">
         <v>281</v>
       </c>
-      <c r="P112" s="49" t="s">
+      <c r="P113" s="49" t="s">
         <v>281</v>
       </c>
-      <c r="Q112" s="27"/>
-    </row>
-    <row r="113" spans="1:18" s="25" customFormat="1" ht="58.3" x14ac:dyDescent="0.4">
-      <c r="A113" s="26" t="s">
+      <c r="Q113" s="27"/>
+    </row>
+    <row r="114" spans="1:18" s="25" customFormat="1" ht="58.3" x14ac:dyDescent="0.4">
+      <c r="A114" s="26" t="s">
         <v>258</v>
       </c>
-      <c r="B113" s="26" t="s">
+      <c r="B114" s="26" t="s">
         <v>82</v>
       </c>
-      <c r="C113" s="26" t="s">
+      <c r="C114" s="26" t="s">
         <v>259</v>
       </c>
-      <c r="D113" s="26" t="b">
-        <v>1</v>
-      </c>
-      <c r="E113" s="26" t="b">
-        <v>1</v>
-      </c>
-      <c r="F113" s="26" t="s">
+      <c r="D114" s="26" t="b">
+        <v>1</v>
+      </c>
+      <c r="E114" s="26" t="b">
+        <v>1</v>
+      </c>
+      <c r="F114" s="26" t="s">
         <v>260</v>
       </c>
-      <c r="G113" s="27"/>
-      <c r="H113" s="26"/>
-      <c r="I113" s="26"/>
-      <c r="J113" s="26"/>
-      <c r="K113" s="26"/>
-      <c r="L113" s="27"/>
-      <c r="M113" s="26"/>
-      <c r="Q113" s="27"/>
-    </row>
-    <row r="114" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A114" s="2" t="s">
+      <c r="G114" s="27"/>
+      <c r="H114" s="26"/>
+      <c r="I114" s="26"/>
+      <c r="J114" s="26"/>
+      <c r="K114" s="26"/>
+      <c r="L114" s="27"/>
+      <c r="M114" s="26"/>
+      <c r="Q114" s="27"/>
+    </row>
+    <row r="115" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A115" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="B114" s="2" t="s">
+      <c r="B115" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="C114" s="2" t="s">
+      <c r="C115" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="D114" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E114" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F114" s="2" t="s">
+      <c r="D115" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E115" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F115" s="2" t="s">
         <v>228</v>
       </c>
-      <c r="G114" s="20"/>
-      <c r="L114" s="20"/>
-      <c r="M114" s="17"/>
-      <c r="N114" s="17"/>
-      <c r="O114" s="17"/>
-      <c r="P114" s="17"/>
-      <c r="Q114" s="27"/>
-    </row>
-    <row r="115" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="R115"/>
+      <c r="G115" s="20"/>
+      <c r="L115" s="20"/>
+      <c r="M115" s="17"/>
+      <c r="N115" s="17"/>
+      <c r="O115" s="17"/>
+      <c r="P115" s="17"/>
+      <c r="Q115" s="27"/>
     </row>
     <row r="116" spans="1:18" x14ac:dyDescent="0.4">
       <c r="R116"/>
@@ -5157,6 +5207,9 @@
     </row>
     <row r="136" spans="18:18" x14ac:dyDescent="0.4">
       <c r="R136"/>
+    </row>
+    <row r="137" spans="18:18" x14ac:dyDescent="0.4">
+      <c r="R137"/>
     </row>
   </sheetData>
   <mergeCells count="8">
@@ -5164,15 +5217,15 @@
     <mergeCell ref="B7:B8"/>
     <mergeCell ref="C7:C8"/>
     <mergeCell ref="D7:D8"/>
-    <mergeCell ref="A45:A46"/>
-    <mergeCell ref="B45:B46"/>
-    <mergeCell ref="C45:C46"/>
-    <mergeCell ref="D45:D46"/>
+    <mergeCell ref="A46:A47"/>
+    <mergeCell ref="B46:B47"/>
+    <mergeCell ref="C46:C47"/>
+    <mergeCell ref="D46:D47"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="F20" r:id="rId1"/>
     <hyperlink ref="F21" r:id="rId2"/>
-    <hyperlink ref="F59" r:id="rId3"/>
+    <hyperlink ref="F60" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="37" fitToHeight="0" orientation="landscape" r:id="rId4"/>

</xml_diff>

<commit_message>
[geonovum] GIT toegang Bot via personal access token
</commit_message>
<xml_diff>
--- a/src/main/resources/input/Geonovum/props/Geonovum.xlsx
+++ b/src/main/resources/input/Geonovum/props/Geonovum.xlsx
@@ -954,9 +954,6 @@
     <t>URL of the Github IO (pages) location</t>
   </si>
   <si>
-    <t>/geonovum/[model-abbreviation]</t>
-  </si>
-  <si>
     <t>git</t>
   </si>
   <si>
@@ -1012,6 +1009,9 @@
   </si>
   <si>
     <t>Yes if MIM format must be generated</t>
+  </si>
+  <si>
+    <t>/Geonovum/[model-abbreviation].git</t>
   </si>
 </sst>
 </file>
@@ -1597,10 +1597,10 @@
   <dimension ref="A1:R139"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="D20" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="D50" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="M33" sqref="M33:P33"/>
+      <selection pane="bottomRight" activeCell="F62" sqref="F62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -2395,13 +2395,13 @@
     </row>
     <row r="27" spans="1:18" s="51" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A27" s="51" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="B27" s="51" t="s">
         <v>5</v>
       </c>
       <c r="C27" s="51" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="D27" s="51" t="b">
         <v>0</v>
@@ -2529,13 +2529,13 @@
     </row>
     <row r="30" spans="1:18" s="46" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A30" s="46" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="B30" s="46" t="s">
         <v>5</v>
       </c>
       <c r="C30" s="46" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="D30" s="46" t="b">
         <v>0</v>
@@ -2645,13 +2645,13 @@
     </row>
     <row r="33" spans="1:18" s="52" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A33" s="52" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="B33" s="52" t="s">
         <v>5</v>
       </c>
       <c r="C33" s="52" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="D33" s="52" t="b">
         <v>0</v>
@@ -3007,7 +3007,7 @@
         <v>1</v>
       </c>
       <c r="F43" s="47" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="G43" s="27"/>
       <c r="H43" s="36"/>
@@ -3521,7 +3521,7 @@
         <v>1</v>
       </c>
       <c r="F62" s="7" t="s">
-        <v>309</v>
+        <v>328</v>
       </c>
       <c r="G62" s="27"/>
       <c r="L62" s="27"/>
@@ -3637,22 +3637,22 @@
     </row>
     <row r="67" spans="1:18" s="46" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A67" s="46" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="B67" s="46" t="s">
         <v>10</v>
       </c>
       <c r="C67" s="46" t="s">
+        <v>313</v>
+      </c>
+      <c r="D67" s="46" t="b">
+        <v>0</v>
+      </c>
+      <c r="E67" s="46" t="b">
+        <v>1</v>
+      </c>
+      <c r="F67" s="46" t="s">
         <v>314</v>
-      </c>
-      <c r="D67" s="46" t="b">
-        <v>0</v>
-      </c>
-      <c r="E67" s="46" t="b">
-        <v>1</v>
-      </c>
-      <c r="F67" s="46" t="s">
-        <v>315</v>
       </c>
       <c r="G67" s="27"/>
       <c r="L67" s="27"/>
@@ -3843,7 +3843,7 @@
         <v>10</v>
       </c>
       <c r="C74" s="48" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="D74" s="48" t="b">
         <v>0</v>
@@ -3862,13 +3862,13 @@
     </row>
     <row r="75" spans="1:18" s="52" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A75" s="52" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="B75" s="52" t="s">
         <v>10</v>
       </c>
       <c r="C75" s="52" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="D75" s="52" t="b">
         <v>0</v>
@@ -3909,13 +3909,13 @@
     </row>
     <row r="77" spans="1:18" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A77" s="44" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="B77" s="44" t="s">
         <v>5</v>
       </c>
       <c r="C77" s="44" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="D77" s="50" t="b">
         <v>0</v>
@@ -4049,7 +4049,7 @@
         <v>0</v>
       </c>
       <c r="F81" s="2" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="G81" s="20"/>
       <c r="L81" s="20"/>
@@ -4105,13 +4105,13 @@
       </c>
       <c r="G83" s="20"/>
       <c r="I83" s="2" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="J83" s="2" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="K83" s="2" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="L83" s="20"/>
       <c r="M83" s="17"/>
@@ -5118,13 +5118,13 @@
     </row>
     <row r="115" spans="1:18" s="49" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A115" s="49" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="B115" s="49" t="s">
         <v>10</v>
       </c>
       <c r="C115" s="49" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="D115" s="49" t="b">
         <v>1</v>

</xml_diff>

<commit_message>
[kadaster & geonovum] Defaults voor createmimformat op no gezet
</commit_message>
<xml_diff>
--- a/src/main/resources/input/Geonovum/props/Geonovum.xlsx
+++ b/src/main/resources/input/Geonovum/props/Geonovum.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="666" uniqueCount="329">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="663" uniqueCount="329">
   <si>
     <t>Name</t>
   </si>
@@ -1597,10 +1597,10 @@
   <dimension ref="A1:R139"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="D50" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B21" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F62" sqref="F62"/>
+      <selection pane="bottomRight" activeCell="A33" sqref="A33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -2663,15 +2663,6 @@
         <v>16</v>
       </c>
       <c r="G33" s="27"/>
-      <c r="I33" s="52" t="s">
-        <v>4</v>
-      </c>
-      <c r="J33" s="52" t="s">
-        <v>4</v>
-      </c>
-      <c r="K33" s="52" t="s">
-        <v>4</v>
-      </c>
       <c r="L33" s="27"/>
       <c r="Q33" s="27"/>
     </row>

</xml_diff>

<commit_message>
Samenbrengen van sub-metamodellen in één MIM 1.1 metamodel
Dit is eerste stap de realisatie van het verzoek van de UG om de
configuratie te vereenvoudigen. De tweede stap is het 100% gelijktrekken
van configuratie met de MIM 1.1 spec.

Er zou als resultaat van deze stap géén veschil moeten zijn tussen de
effectieve configuratie voor, en na deze aanpassing. In de praktijk is
dat niet altijd het geval, omdat BRO feitelijk op 1.0 werkte. BRO
accepteert deze verschillen en herstelt dit in de modellen.

Minor.
</commit_message>
<xml_diff>
--- a/src/main/resources/input/Geonovum/props/Geonovum.xlsx
+++ b/src/main/resources/input/Geonovum/props/Geonovum.xlsx
@@ -1156,7 +1156,7 @@
     <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -1285,6 +1285,9 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1597,10 +1600,10 @@
   <dimension ref="A1:R139"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B21" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B94" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A33" sqref="A33"/>
+      <selection pane="bottomRight" activeCell="N102" sqref="N102:P102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -1808,16 +1811,16 @@
       <c r="R6"/>
     </row>
     <row r="7" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A7" s="53" t="s">
+      <c r="A7" s="54" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="53" t="s">
+      <c r="B7" s="54" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="53" t="s">
+      <c r="C7" s="54" t="s">
         <v>11</v>
       </c>
-      <c r="D7" s="53" t="b">
+      <c r="D7" s="54" t="b">
         <v>1</v>
       </c>
       <c r="E7" s="2" t="b">
@@ -1833,10 +1836,10 @@
       <c r="R7"/>
     </row>
     <row r="8" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="53"/>
-      <c r="B8" s="53"/>
-      <c r="C8" s="53"/>
-      <c r="D8" s="53"/>
+      <c r="A8" s="54"/>
+      <c r="B8" s="54"/>
+      <c r="C8" s="54"/>
+      <c r="D8" s="54"/>
       <c r="G8" s="20"/>
       <c r="L8" s="20"/>
       <c r="M8" s="17"/>
@@ -3090,16 +3093,16 @@
       <c r="R46"/>
     </row>
     <row r="47" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A47" s="53" t="s">
+      <c r="A47" s="54" t="s">
         <v>51</v>
       </c>
-      <c r="B47" s="53" t="s">
+      <c r="B47" s="54" t="s">
         <v>5</v>
       </c>
-      <c r="C47" s="53" t="s">
+      <c r="C47" s="54" t="s">
         <v>52</v>
       </c>
-      <c r="D47" s="53" t="b">
+      <c r="D47" s="54" t="b">
         <v>0</v>
       </c>
       <c r="E47" s="2" t="b">
@@ -3118,10 +3121,10 @@
       <c r="R47"/>
     </row>
     <row r="48" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A48" s="53"/>
-      <c r="B48" s="53"/>
-      <c r="C48" s="53"/>
-      <c r="D48" s="53"/>
+      <c r="A48" s="54"/>
+      <c r="B48" s="54"/>
+      <c r="C48" s="54"/>
+      <c r="D48" s="54"/>
       <c r="G48" s="20"/>
       <c r="L48" s="20"/>
       <c r="M48" s="17"/>
@@ -4639,30 +4642,30 @@
         <v>0</v>
       </c>
       <c r="G102" s="20"/>
-      <c r="H102" s="38" t="s">
-        <v>280</v>
-      </c>
-      <c r="I102" s="38" t="s">
-        <v>280</v>
-      </c>
-      <c r="J102" s="38" t="s">
-        <v>280</v>
-      </c>
-      <c r="K102" s="38" t="s">
-        <v>280</v>
+      <c r="H102" s="53" t="s">
+        <v>282</v>
+      </c>
+      <c r="I102" s="53" t="s">
+        <v>282</v>
+      </c>
+      <c r="J102" s="53" t="s">
+        <v>282</v>
+      </c>
+      <c r="K102" s="53" t="s">
+        <v>282</v>
       </c>
       <c r="L102" s="27"/>
       <c r="M102" s="38" t="s">
-        <v>281</v>
-      </c>
-      <c r="N102" s="38" t="s">
-        <v>281</v>
-      </c>
-      <c r="O102" s="38" t="s">
-        <v>281</v>
-      </c>
-      <c r="P102" s="38" t="s">
-        <v>281</v>
+        <v>283</v>
+      </c>
+      <c r="N102" s="53" t="s">
+        <v>283</v>
+      </c>
+      <c r="O102" s="53" t="s">
+        <v>283</v>
+      </c>
+      <c r="P102" s="53" t="s">
+        <v>283</v>
       </c>
       <c r="Q102" s="27"/>
       <c r="R102"/>

</xml_diff>

<commit_message>
Geonovum: Regressietest behoort niet te publiceren naar GIThub.
Zet passoffice = none.

Bugfix.
</commit_message>
<xml_diff>
--- a/src/main/resources/input/Geonovum/props/Geonovum.xlsx
+++ b/src/main/resources/input/Geonovum/props/Geonovum.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="728" uniqueCount="333">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="727" uniqueCount="333">
   <si>
     <t>Name</t>
   </si>
@@ -1320,10 +1320,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Bad" xfId="3" builtinId="27"/>
@@ -1616,10 +1616,10 @@
   <dimension ref="A1:W140"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="F70" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="D70" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G89" sqref="G89:W89"/>
+      <selection pane="bottomRight" activeCell="R83" sqref="R83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -1847,16 +1847,16 @@
       <c r="T6"/>
     </row>
     <row r="7" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A7" s="55" t="s">
+      <c r="A7" s="56" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="55" t="s">
+      <c r="B7" s="56" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="55" t="s">
+      <c r="C7" s="56" t="s">
         <v>11</v>
       </c>
-      <c r="D7" s="55" t="b">
+      <c r="D7" s="56" t="b">
         <v>1</v>
       </c>
       <c r="E7" s="2" t="b">
@@ -1874,10 +1874,10 @@
       <c r="T7"/>
     </row>
     <row r="8" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="55"/>
-      <c r="B8" s="55"/>
-      <c r="C8" s="55"/>
-      <c r="D8" s="55"/>
+      <c r="A8" s="56"/>
+      <c r="B8" s="56"/>
+      <c r="C8" s="56"/>
+      <c r="D8" s="56"/>
       <c r="G8" s="20"/>
       <c r="L8" s="54"/>
       <c r="M8" s="20"/>
@@ -3251,16 +3251,16 @@
       <c r="T46"/>
     </row>
     <row r="47" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A47" s="55" t="s">
+      <c r="A47" s="56" t="s">
         <v>51</v>
       </c>
-      <c r="B47" s="55" t="s">
+      <c r="B47" s="56" t="s">
         <v>5</v>
       </c>
-      <c r="C47" s="55" t="s">
+      <c r="C47" s="56" t="s">
         <v>52</v>
       </c>
-      <c r="D47" s="55" t="b">
+      <c r="D47" s="56" t="b">
         <v>0</v>
       </c>
       <c r="E47" s="2" t="b">
@@ -3281,10 +3281,10 @@
       <c r="T47"/>
     </row>
     <row r="48" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A48" s="55"/>
-      <c r="B48" s="55"/>
-      <c r="C48" s="55"/>
-      <c r="D48" s="55"/>
+      <c r="A48" s="56"/>
+      <c r="B48" s="56"/>
+      <c r="C48" s="56"/>
+      <c r="D48" s="56"/>
       <c r="G48" s="20"/>
       <c r="L48" s="54"/>
       <c r="M48" s="20"/>
@@ -4327,9 +4327,7 @@
       <c r="K83" s="2" t="s">
         <v>309</v>
       </c>
-      <c r="L83" s="54" t="s">
-        <v>309</v>
-      </c>
+      <c r="L83" s="54"/>
       <c r="M83" s="20"/>
       <c r="N83" s="17"/>
       <c r="O83" s="17"/>
@@ -4528,7 +4526,7 @@
         <v>4</v>
       </c>
       <c r="S89" s="45"/>
-      <c r="T89" s="56"/>
+      <c r="T89" s="55"/>
       <c r="U89" s="44"/>
       <c r="V89" s="44"/>
       <c r="W89" s="44"/>

</xml_diff>

<commit_message>
Aansluiting van Geonovum op NEN3610:2022
Ook de properties zijn bijgewerkt met een nieuwe processing mode:
"NEN3610-2022"

Minor.
</commit_message>
<xml_diff>
--- a/src/main/resources/input/Geonovum/props/Geonovum.xlsx
+++ b/src/main/resources/input/Geonovum/props/Geonovum.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="727" uniqueCount="333">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="877" uniqueCount="341">
   <si>
     <t>Name</t>
   </si>
@@ -1024,6 +1024,30 @@
   </si>
   <si>
     <t>Should a regression test be performed on the results of this run?</t>
+  </si>
+  <si>
+    <t>NEN3610_2022</t>
+  </si>
+  <si>
+    <t>NEN3610-2022: minimum</t>
+  </si>
+  <si>
+    <t>NEN3610-2022: uitgebreid</t>
+  </si>
+  <si>
+    <t>NEN3610-2022: opleveren</t>
+  </si>
+  <si>
+    <t>NEN3610-2022: docrelease</t>
+  </si>
+  <si>
+    <t>NEN3610-2022: regtest</t>
+  </si>
+  <si>
+    <t>Geonovum-NEN3610-2022</t>
+  </si>
+  <si>
+    <t>NEN3610-2022</t>
   </si>
 </sst>
 </file>
@@ -1168,7 +1192,7 @@
     <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -1321,6 +1345,12 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -1613,13 +1643,13 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:W140"/>
+  <dimension ref="A1:AC140"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="D70" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="L81" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="R83" sqref="R83"/>
+      <selection pane="bottomRight" activeCell="T85" sqref="T85:X85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -1642,10 +1672,16 @@
     <col min="17" max="17" width="15.765625" customWidth="1"/>
     <col min="18" max="18" width="16.07421875" customWidth="1"/>
     <col min="19" max="19" width="7.3046875" style="23" customWidth="1"/>
-    <col min="20" max="20" width="32.4609375" style="1" customWidth="1"/>
+    <col min="20" max="20" width="16.15234375" customWidth="1"/>
+    <col min="21" max="21" width="16.07421875" customWidth="1"/>
+    <col min="22" max="22" width="15.69140625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="15.765625" customWidth="1"/>
+    <col min="24" max="24" width="14.23046875" customWidth="1"/>
+    <col min="25" max="25" width="7.3046875" style="23" customWidth="1"/>
+    <col min="26" max="26" width="32.4609375" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" s="4" customFormat="1" ht="37.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:26" s="4" customFormat="1" ht="37.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1697,11 +1733,27 @@
         <v>254</v>
       </c>
       <c r="S1" s="18"/>
-      <c r="T1" s="3" t="s">
+      <c r="T1" s="4" t="s">
+        <v>254</v>
+      </c>
+      <c r="U1" s="4" t="s">
+        <v>254</v>
+      </c>
+      <c r="V1" s="4" t="s">
+        <v>254</v>
+      </c>
+      <c r="W1" s="4" t="s">
+        <v>254</v>
+      </c>
+      <c r="X1" s="4" t="s">
+        <v>254</v>
+      </c>
+      <c r="Y1" s="18"/>
+      <c r="Z1" s="3" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="2" spans="1:20" s="4" customFormat="1" ht="37.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:26" s="4" customFormat="1" ht="56.15" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="F2" s="3"/>
       <c r="G2" s="19"/>
       <c r="H2" s="3" t="s">
@@ -1736,9 +1788,25 @@
         <v>330</v>
       </c>
       <c r="S2" s="19"/>
-      <c r="T2" s="5"/>
-    </row>
-    <row r="3" spans="1:20" s="2" customFormat="1" ht="44.15" thickTop="1" x14ac:dyDescent="0.4">
+      <c r="T2" s="3" t="s">
+        <v>334</v>
+      </c>
+      <c r="U2" s="3" t="s">
+        <v>335</v>
+      </c>
+      <c r="V2" s="3" t="s">
+        <v>336</v>
+      </c>
+      <c r="W2" s="3" t="s">
+        <v>337</v>
+      </c>
+      <c r="X2" s="3" t="s">
+        <v>338</v>
+      </c>
+      <c r="Y2" s="19"/>
+      <c r="Z2" s="5"/>
+    </row>
+    <row r="3" spans="1:26" s="2" customFormat="1" ht="44.15" thickTop="1" x14ac:dyDescent="0.4">
       <c r="A3" s="2" t="s">
         <v>155</v>
       </c>
@@ -1763,9 +1831,15 @@
       <c r="Q3" s="17"/>
       <c r="R3" s="54"/>
       <c r="S3" s="27"/>
-      <c r="T3"/>
-    </row>
-    <row r="4" spans="1:20" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="T3" s="56"/>
+      <c r="U3" s="56"/>
+      <c r="V3" s="56"/>
+      <c r="W3" s="56"/>
+      <c r="X3" s="56"/>
+      <c r="Y3" s="27"/>
+      <c r="Z3"/>
+    </row>
+    <row r="4" spans="1:26" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
@@ -1793,9 +1867,15 @@
       <c r="Q4" s="17"/>
       <c r="R4" s="54"/>
       <c r="S4" s="27"/>
-      <c r="T4"/>
-    </row>
-    <row r="5" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="T4" s="56"/>
+      <c r="U4" s="56"/>
+      <c r="V4" s="56"/>
+      <c r="W4" s="56"/>
+      <c r="X4" s="56"/>
+      <c r="Y4" s="27"/>
+      <c r="Z4"/>
+    </row>
+    <row r="5" spans="1:26" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A5" s="2" t="s">
         <v>7</v>
       </c>
@@ -1823,9 +1903,15 @@
       <c r="Q5" s="17"/>
       <c r="R5" s="54"/>
       <c r="S5" s="27"/>
-      <c r="T5"/>
-    </row>
-    <row r="6" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="T5" s="56"/>
+      <c r="U5" s="56"/>
+      <c r="V5" s="56"/>
+      <c r="W5" s="56"/>
+      <c r="X5" s="56"/>
+      <c r="Y5" s="27"/>
+      <c r="Z5"/>
+    </row>
+    <row r="6" spans="1:26" s="7" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A6" s="7" t="s">
         <v>158</v>
       </c>
@@ -1844,19 +1930,20 @@
       <c r="G6" s="20"/>
       <c r="M6" s="20"/>
       <c r="S6" s="27"/>
-      <c r="T6"/>
-    </row>
-    <row r="7" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A7" s="56" t="s">
+      <c r="Y6" s="27"/>
+      <c r="Z6"/>
+    </row>
+    <row r="7" spans="1:26" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A7" s="58" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="56" t="s">
+      <c r="B7" s="58" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="56" t="s">
+      <c r="C7" s="58" t="s">
         <v>11</v>
       </c>
-      <c r="D7" s="56" t="b">
+      <c r="D7" s="58" t="b">
         <v>1</v>
       </c>
       <c r="E7" s="2" t="b">
@@ -1871,13 +1958,19 @@
       <c r="Q7" s="17"/>
       <c r="R7" s="54"/>
       <c r="S7" s="27"/>
-      <c r="T7"/>
-    </row>
-    <row r="8" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="56"/>
-      <c r="B8" s="56"/>
-      <c r="C8" s="56"/>
-      <c r="D8" s="56"/>
+      <c r="T7" s="56"/>
+      <c r="U7" s="56"/>
+      <c r="V7" s="56"/>
+      <c r="W7" s="56"/>
+      <c r="X7" s="56"/>
+      <c r="Y7" s="27"/>
+      <c r="Z7"/>
+    </row>
+    <row r="8" spans="1:26" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A8" s="58"/>
+      <c r="B8" s="58"/>
+      <c r="C8" s="58"/>
+      <c r="D8" s="58"/>
       <c r="G8" s="20"/>
       <c r="L8" s="54"/>
       <c r="M8" s="20"/>
@@ -1887,9 +1980,15 @@
       <c r="Q8" s="17"/>
       <c r="R8" s="54"/>
       <c r="S8" s="27"/>
-      <c r="T8"/>
-    </row>
-    <row r="9" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="T8" s="56"/>
+      <c r="U8" s="56"/>
+      <c r="V8" s="56"/>
+      <c r="W8" s="56"/>
+      <c r="X8" s="56"/>
+      <c r="Y8" s="27"/>
+      <c r="Z8"/>
+    </row>
+    <row r="9" spans="1:26" s="7" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A9" s="7" t="s">
         <v>161</v>
       </c>
@@ -1911,9 +2010,10 @@
       <c r="G9" s="20"/>
       <c r="M9" s="20"/>
       <c r="S9" s="27"/>
-      <c r="T9"/>
-    </row>
-    <row r="10" spans="1:20" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="Y9" s="27"/>
+      <c r="Z9"/>
+    </row>
+    <row r="10" spans="1:26" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A10" s="2" t="s">
         <v>13</v>
       </c>
@@ -1941,9 +2041,15 @@
       <c r="Q10" s="17"/>
       <c r="R10" s="54"/>
       <c r="S10" s="27"/>
-      <c r="T10"/>
-    </row>
-    <row r="11" spans="1:20" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="T10" s="56"/>
+      <c r="U10" s="56"/>
+      <c r="V10" s="56"/>
+      <c r="W10" s="56"/>
+      <c r="X10" s="56"/>
+      <c r="Y10" s="27"/>
+      <c r="Z10"/>
+    </row>
+    <row r="11" spans="1:26" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A11" s="7" t="s">
         <v>163</v>
       </c>
@@ -1962,9 +2068,10 @@
       <c r="G11" s="20"/>
       <c r="M11" s="20"/>
       <c r="S11" s="27"/>
-      <c r="T11"/>
-    </row>
-    <row r="12" spans="1:20" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="Y11" s="27"/>
+      <c r="Z11"/>
+    </row>
+    <row r="12" spans="1:26" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A12" s="2" t="s">
         <v>136</v>
       </c>
@@ -1992,9 +2099,15 @@
       <c r="Q12" s="17"/>
       <c r="R12" s="54"/>
       <c r="S12" s="27"/>
-      <c r="T12"/>
-    </row>
-    <row r="13" spans="1:20" s="13" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="T12" s="56"/>
+      <c r="U12" s="56"/>
+      <c r="V12" s="56"/>
+      <c r="W12" s="56"/>
+      <c r="X12" s="56"/>
+      <c r="Y12" s="27"/>
+      <c r="Z12"/>
+    </row>
+    <row r="13" spans="1:26" s="13" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A13" s="13" t="s">
         <v>245</v>
       </c>
@@ -2022,9 +2135,15 @@
       <c r="Q13" s="17"/>
       <c r="R13" s="54"/>
       <c r="S13" s="27"/>
-      <c r="T13"/>
-    </row>
-    <row r="14" spans="1:20" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="T13" s="56"/>
+      <c r="U13" s="56"/>
+      <c r="V13" s="56"/>
+      <c r="W13" s="56"/>
+      <c r="X13" s="56"/>
+      <c r="Y13" s="27"/>
+      <c r="Z13"/>
+    </row>
+    <row r="14" spans="1:26" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A14" s="2" t="s">
         <v>15</v>
       </c>
@@ -2052,9 +2171,15 @@
       <c r="Q14" s="17"/>
       <c r="R14" s="54"/>
       <c r="S14" s="27"/>
-      <c r="T14"/>
-    </row>
-    <row r="15" spans="1:20" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="T14" s="56"/>
+      <c r="U14" s="56"/>
+      <c r="V14" s="56"/>
+      <c r="W14" s="56"/>
+      <c r="X14" s="56"/>
+      <c r="Y14" s="27"/>
+      <c r="Z14"/>
+    </row>
+    <row r="15" spans="1:26" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A15" s="2" t="s">
         <v>18</v>
       </c>
@@ -2103,9 +2228,25 @@
         <v>19</v>
       </c>
       <c r="S15" s="27"/>
-      <c r="T15"/>
-    </row>
-    <row r="16" spans="1:20" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="T15" s="56" t="s">
+        <v>19</v>
+      </c>
+      <c r="U15" s="56" t="s">
+        <v>19</v>
+      </c>
+      <c r="V15" s="56" t="s">
+        <v>206</v>
+      </c>
+      <c r="W15" s="56" t="s">
+        <v>206</v>
+      </c>
+      <c r="X15" s="56" t="s">
+        <v>19</v>
+      </c>
+      <c r="Y15" s="27"/>
+      <c r="Z15"/>
+    </row>
+    <row r="16" spans="1:26" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A16" s="2" t="s">
         <v>22</v>
       </c>
@@ -2133,9 +2274,15 @@
       <c r="Q16" s="17"/>
       <c r="R16" s="54"/>
       <c r="S16" s="27"/>
-      <c r="T16"/>
-    </row>
-    <row r="17" spans="1:20" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="T16" s="56"/>
+      <c r="U16" s="56"/>
+      <c r="V16" s="56"/>
+      <c r="W16" s="56"/>
+      <c r="X16" s="56"/>
+      <c r="Y16" s="27"/>
+      <c r="Z16"/>
+    </row>
+    <row r="17" spans="1:26" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A17" s="2" t="s">
         <v>223</v>
       </c>
@@ -2163,9 +2310,15 @@
       <c r="Q17" s="17"/>
       <c r="R17" s="54"/>
       <c r="S17" s="27"/>
-      <c r="T17"/>
-    </row>
-    <row r="18" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="T17" s="56"/>
+      <c r="U17" s="56"/>
+      <c r="V17" s="56"/>
+      <c r="W17" s="56"/>
+      <c r="X17" s="56"/>
+      <c r="Y17" s="27"/>
+      <c r="Z17"/>
+    </row>
+    <row r="18" spans="1:26" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A18" s="2" t="s">
         <v>225</v>
       </c>
@@ -2189,9 +2342,15 @@
       <c r="Q18" s="17"/>
       <c r="R18" s="54"/>
       <c r="S18" s="27"/>
-      <c r="T18"/>
-    </row>
-    <row r="19" spans="1:20" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="T18" s="56"/>
+      <c r="U18" s="56"/>
+      <c r="V18" s="56"/>
+      <c r="W18" s="56"/>
+      <c r="X18" s="56"/>
+      <c r="Y18" s="27"/>
+      <c r="Z18"/>
+    </row>
+    <row r="19" spans="1:26" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A19" s="2" t="s">
         <v>165</v>
       </c>
@@ -2216,9 +2375,15 @@
       <c r="Q19" s="17"/>
       <c r="R19" s="54"/>
       <c r="S19" s="27"/>
-      <c r="T19"/>
-    </row>
-    <row r="20" spans="1:20" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="T19" s="56"/>
+      <c r="U19" s="56"/>
+      <c r="V19" s="56"/>
+      <c r="W19" s="56"/>
+      <c r="X19" s="56"/>
+      <c r="Y19" s="27"/>
+      <c r="Z19"/>
+    </row>
+    <row r="20" spans="1:26" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A20" s="2" t="s">
         <v>138</v>
       </c>
@@ -2246,9 +2411,15 @@
       <c r="Q20" s="17"/>
       <c r="R20" s="54"/>
       <c r="S20" s="27"/>
-      <c r="T20"/>
-    </row>
-    <row r="21" spans="1:20" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="T20" s="56"/>
+      <c r="U20" s="56"/>
+      <c r="V20" s="56"/>
+      <c r="W20" s="56"/>
+      <c r="X20" s="56"/>
+      <c r="Y20" s="27"/>
+      <c r="Z20"/>
+    </row>
+    <row r="21" spans="1:26" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A21" s="2" t="s">
         <v>141</v>
       </c>
@@ -2276,9 +2447,15 @@
       <c r="Q21" s="17"/>
       <c r="R21" s="54"/>
       <c r="S21" s="27"/>
-      <c r="T21"/>
-    </row>
-    <row r="22" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="T21" s="56"/>
+      <c r="U21" s="56"/>
+      <c r="V21" s="56"/>
+      <c r="W21" s="56"/>
+      <c r="X21" s="56"/>
+      <c r="Y21" s="27"/>
+      <c r="Z21"/>
+    </row>
+    <row r="22" spans="1:26" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A22" s="2" t="s">
         <v>144</v>
       </c>
@@ -2327,9 +2504,25 @@
         <v>4</v>
       </c>
       <c r="S22" s="27"/>
-      <c r="T22"/>
-    </row>
-    <row r="23" spans="1:20" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="T22" s="56" t="s">
+        <v>16</v>
+      </c>
+      <c r="U22" s="56" t="s">
+        <v>4</v>
+      </c>
+      <c r="V22" s="56" t="s">
+        <v>4</v>
+      </c>
+      <c r="W22" s="56" t="s">
+        <v>4</v>
+      </c>
+      <c r="X22" s="56" t="s">
+        <v>4</v>
+      </c>
+      <c r="Y22" s="27"/>
+      <c r="Z22"/>
+    </row>
+    <row r="23" spans="1:26" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A23" s="7" t="s">
         <v>26</v>
       </c>
@@ -2351,9 +2544,10 @@
       <c r="G23" s="20"/>
       <c r="M23" s="20"/>
       <c r="S23" s="27"/>
-      <c r="T23"/>
-    </row>
-    <row r="24" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="Y23" s="27"/>
+      <c r="Z23"/>
+    </row>
+    <row r="24" spans="1:26" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A24" s="2" t="s">
         <v>167</v>
       </c>
@@ -2378,9 +2572,15 @@
       <c r="Q24" s="17"/>
       <c r="R24" s="54"/>
       <c r="S24" s="27"/>
-      <c r="T24"/>
-    </row>
-    <row r="25" spans="1:20" s="2" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="T24" s="56"/>
+      <c r="U24" s="56"/>
+      <c r="V24" s="56"/>
+      <c r="W24" s="56"/>
+      <c r="X24" s="56"/>
+      <c r="Y24" s="27"/>
+      <c r="Z24"/>
+    </row>
+    <row r="25" spans="1:26" s="2" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A25" s="2" t="s">
         <v>28</v>
       </c>
@@ -2429,9 +2629,25 @@
         <v>16</v>
       </c>
       <c r="S25" s="27"/>
-      <c r="T25"/>
-    </row>
-    <row r="26" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="T25" s="56" t="s">
+        <v>16</v>
+      </c>
+      <c r="U25" s="56" t="s">
+        <v>16</v>
+      </c>
+      <c r="V25" s="56" t="s">
+        <v>4</v>
+      </c>
+      <c r="W25" s="56" t="s">
+        <v>4</v>
+      </c>
+      <c r="X25" s="56" t="s">
+        <v>16</v>
+      </c>
+      <c r="Y25" s="27"/>
+      <c r="Z25"/>
+    </row>
+    <row r="26" spans="1:26" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A26" s="2" t="s">
         <v>30</v>
       </c>
@@ -2480,9 +2696,25 @@
         <v>4</v>
       </c>
       <c r="S26" s="27"/>
-      <c r="T26"/>
-    </row>
-    <row r="27" spans="1:20" s="51" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="T26" s="56" t="s">
+        <v>16</v>
+      </c>
+      <c r="U26" s="56" t="s">
+        <v>4</v>
+      </c>
+      <c r="V26" s="56" t="s">
+        <v>4</v>
+      </c>
+      <c r="W26" s="56" t="s">
+        <v>4</v>
+      </c>
+      <c r="X26" s="56" t="s">
+        <v>4</v>
+      </c>
+      <c r="Y26" s="27"/>
+      <c r="Z26"/>
+    </row>
+    <row r="27" spans="1:26" s="51" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A27" s="51" t="s">
         <v>322</v>
       </c>
@@ -2531,8 +2763,24 @@
         <v>4</v>
       </c>
       <c r="S27" s="27"/>
-    </row>
-    <row r="28" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="T27" s="56" t="s">
+        <v>16</v>
+      </c>
+      <c r="U27" s="56" t="s">
+        <v>4</v>
+      </c>
+      <c r="V27" s="56" t="s">
+        <v>4</v>
+      </c>
+      <c r="W27" s="56" t="s">
+        <v>4</v>
+      </c>
+      <c r="X27" s="56" t="s">
+        <v>4</v>
+      </c>
+      <c r="Y27" s="27"/>
+    </row>
+    <row r="28" spans="1:26" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A28" s="2" t="s">
         <v>32</v>
       </c>
@@ -2581,9 +2829,25 @@
         <v>16</v>
       </c>
       <c r="S28" s="27"/>
-      <c r="T28"/>
-    </row>
-    <row r="29" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="T28" s="56" t="s">
+        <v>16</v>
+      </c>
+      <c r="U28" s="56" t="s">
+        <v>16</v>
+      </c>
+      <c r="V28" s="56" t="s">
+        <v>4</v>
+      </c>
+      <c r="W28" s="56" t="s">
+        <v>4</v>
+      </c>
+      <c r="X28" s="56" t="s">
+        <v>16</v>
+      </c>
+      <c r="Y28" s="27"/>
+      <c r="Z28"/>
+    </row>
+    <row r="29" spans="1:26" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A29" s="2" t="s">
         <v>146</v>
       </c>
@@ -2632,9 +2896,25 @@
         <v>4</v>
       </c>
       <c r="S29" s="27"/>
-      <c r="T29"/>
-    </row>
-    <row r="30" spans="1:20" s="46" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="T29" s="56" t="s">
+        <v>16</v>
+      </c>
+      <c r="U29" s="56" t="s">
+        <v>4</v>
+      </c>
+      <c r="V29" s="56" t="s">
+        <v>4</v>
+      </c>
+      <c r="W29" s="56" t="s">
+        <v>4</v>
+      </c>
+      <c r="X29" s="56" t="s">
+        <v>4</v>
+      </c>
+      <c r="Y29" s="27"/>
+      <c r="Z29"/>
+    </row>
+    <row r="30" spans="1:26" s="46" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A30" s="46" t="s">
         <v>315</v>
       </c>
@@ -2683,8 +2963,24 @@
         <v>16</v>
       </c>
       <c r="S30" s="27"/>
-    </row>
-    <row r="31" spans="1:20" s="28" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="T30" s="56" t="s">
+        <v>16</v>
+      </c>
+      <c r="U30" s="56" t="s">
+        <v>16</v>
+      </c>
+      <c r="V30" s="56" t="s">
+        <v>16</v>
+      </c>
+      <c r="W30" s="56" t="s">
+        <v>16</v>
+      </c>
+      <c r="X30" s="56" t="s">
+        <v>16</v>
+      </c>
+      <c r="Y30" s="27"/>
+    </row>
+    <row r="31" spans="1:26" s="28" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A31" s="28" t="s">
         <v>261</v>
       </c>
@@ -2711,9 +3007,15 @@
       <c r="M31" s="27"/>
       <c r="R31" s="54"/>
       <c r="S31" s="27"/>
-      <c r="T31"/>
-    </row>
-    <row r="32" spans="1:20" s="30" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="T31" s="56"/>
+      <c r="U31" s="56"/>
+      <c r="V31" s="56"/>
+      <c r="W31" s="56"/>
+      <c r="X31" s="56"/>
+      <c r="Y31" s="27"/>
+      <c r="Z31"/>
+    </row>
+    <row r="32" spans="1:26" s="30" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A32" s="30" t="s">
         <v>266</v>
       </c>
@@ -2762,9 +3064,25 @@
         <v>25</v>
       </c>
       <c r="S32" s="27"/>
-      <c r="T32"/>
-    </row>
-    <row r="33" spans="1:20" s="52" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="T32" s="56" t="s">
+        <v>25</v>
+      </c>
+      <c r="U32" s="56" t="s">
+        <v>25</v>
+      </c>
+      <c r="V32" s="56" t="s">
+        <v>25</v>
+      </c>
+      <c r="W32" s="56" t="s">
+        <v>25</v>
+      </c>
+      <c r="X32" s="56" t="s">
+        <v>25</v>
+      </c>
+      <c r="Y32" s="27"/>
+      <c r="Z32"/>
+    </row>
+    <row r="33" spans="1:26" s="52" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A33" s="52" t="s">
         <v>326</v>
       </c>
@@ -2788,8 +3106,14 @@
       <c r="M33" s="27"/>
       <c r="R33" s="54"/>
       <c r="S33" s="27"/>
-    </row>
-    <row r="34" spans="1:20" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="T33" s="56"/>
+      <c r="U33" s="56"/>
+      <c r="V33" s="56"/>
+      <c r="W33" s="56"/>
+      <c r="X33" s="56"/>
+      <c r="Y33" s="27"/>
+    </row>
+    <row r="34" spans="1:26" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A34" s="2" t="s">
         <v>34</v>
       </c>
@@ -2817,9 +3141,15 @@
       <c r="Q34" s="17"/>
       <c r="R34" s="54"/>
       <c r="S34" s="27"/>
-      <c r="T34"/>
-    </row>
-    <row r="35" spans="1:20" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="T34" s="56"/>
+      <c r="U34" s="56"/>
+      <c r="V34" s="56"/>
+      <c r="W34" s="56"/>
+      <c r="X34" s="56"/>
+      <c r="Y34" s="27"/>
+      <c r="Z34"/>
+    </row>
+    <row r="35" spans="1:26" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A35" s="2" t="s">
         <v>169</v>
       </c>
@@ -2847,9 +3177,15 @@
       <c r="Q35" s="17"/>
       <c r="R35" s="54"/>
       <c r="S35" s="27"/>
-      <c r="T35"/>
-    </row>
-    <row r="36" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="T35" s="56"/>
+      <c r="U35" s="56"/>
+      <c r="V35" s="56"/>
+      <c r="W35" s="56"/>
+      <c r="X35" s="56"/>
+      <c r="Y35" s="27"/>
+      <c r="Z35"/>
+    </row>
+    <row r="36" spans="1:26" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A36" s="2" t="s">
         <v>172</v>
       </c>
@@ -2877,9 +3213,15 @@
       <c r="Q36" s="17"/>
       <c r="R36" s="54"/>
       <c r="S36" s="27"/>
-      <c r="T36"/>
-    </row>
-    <row r="37" spans="1:20" s="43" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="T36" s="56"/>
+      <c r="U36" s="56"/>
+      <c r="V36" s="56"/>
+      <c r="W36" s="56"/>
+      <c r="X36" s="56"/>
+      <c r="Y36" s="27"/>
+      <c r="Z36"/>
+    </row>
+    <row r="37" spans="1:26" s="43" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A37" s="43" t="s">
         <v>287</v>
       </c>
@@ -2903,8 +3245,14 @@
       <c r="M37" s="27"/>
       <c r="R37" s="54"/>
       <c r="S37" s="27"/>
-    </row>
-    <row r="38" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="T37" s="56"/>
+      <c r="U37" s="56"/>
+      <c r="V37" s="56"/>
+      <c r="W37" s="56"/>
+      <c r="X37" s="56"/>
+      <c r="Y37" s="27"/>
+    </row>
+    <row r="38" spans="1:26" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A38" s="2" t="s">
         <v>38</v>
       </c>
@@ -2953,9 +3301,25 @@
         <v>16</v>
       </c>
       <c r="S38" s="27"/>
-      <c r="T38"/>
-    </row>
-    <row r="39" spans="1:20" s="44" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="T38" s="56" t="s">
+        <v>16</v>
+      </c>
+      <c r="U38" s="56" t="s">
+        <v>16</v>
+      </c>
+      <c r="V38" s="56" t="s">
+        <v>4</v>
+      </c>
+      <c r="W38" s="56" t="s">
+        <v>4</v>
+      </c>
+      <c r="X38" s="56" t="s">
+        <v>16</v>
+      </c>
+      <c r="Y38" s="27"/>
+      <c r="Z38"/>
+    </row>
+    <row r="39" spans="1:26" s="44" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A39" s="44" t="s">
         <v>291</v>
       </c>
@@ -3004,9 +3368,25 @@
         <v>16</v>
       </c>
       <c r="S39" s="27"/>
-      <c r="T39"/>
-    </row>
-    <row r="40" spans="1:20" s="2" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="T39" s="44" t="s">
+        <v>16</v>
+      </c>
+      <c r="U39" s="44" t="s">
+        <v>16</v>
+      </c>
+      <c r="V39" s="44" t="s">
+        <v>4</v>
+      </c>
+      <c r="W39" s="44" t="s">
+        <v>4</v>
+      </c>
+      <c r="X39" s="44" t="s">
+        <v>16</v>
+      </c>
+      <c r="Y39" s="27"/>
+      <c r="Z39"/>
+    </row>
+    <row r="40" spans="1:26" s="2" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A40" s="2" t="s">
         <v>40</v>
       </c>
@@ -3055,9 +3435,25 @@
         <v>16</v>
       </c>
       <c r="S40" s="27"/>
-      <c r="T40"/>
-    </row>
-    <row r="41" spans="1:20" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="T40" s="56" t="s">
+        <v>16</v>
+      </c>
+      <c r="U40" s="56" t="s">
+        <v>16</v>
+      </c>
+      <c r="V40" s="56" t="s">
+        <v>4</v>
+      </c>
+      <c r="W40" s="56" t="s">
+        <v>4</v>
+      </c>
+      <c r="X40" s="56" t="s">
+        <v>16</v>
+      </c>
+      <c r="Y40" s="27"/>
+      <c r="Z40"/>
+    </row>
+    <row r="41" spans="1:26" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A41" s="2" t="s">
         <v>42</v>
       </c>
@@ -3085,9 +3481,15 @@
       <c r="Q41" s="17"/>
       <c r="R41" s="54"/>
       <c r="S41" s="27"/>
-      <c r="T41"/>
-    </row>
-    <row r="42" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="T41" s="56"/>
+      <c r="U41" s="56"/>
+      <c r="V41" s="56"/>
+      <c r="W41" s="56"/>
+      <c r="X41" s="56"/>
+      <c r="Y41" s="27"/>
+      <c r="Z41"/>
+    </row>
+    <row r="42" spans="1:26" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A42" s="2" t="s">
         <v>44</v>
       </c>
@@ -3136,9 +3538,25 @@
         <v>4</v>
       </c>
       <c r="S42" s="27"/>
-      <c r="T42"/>
-    </row>
-    <row r="43" spans="1:20" s="30" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="T42" s="56" t="s">
+        <v>16</v>
+      </c>
+      <c r="U42" s="56" t="s">
+        <v>4</v>
+      </c>
+      <c r="V42" s="56" t="s">
+        <v>4</v>
+      </c>
+      <c r="W42" s="56" t="s">
+        <v>4</v>
+      </c>
+      <c r="X42" s="56" t="s">
+        <v>4</v>
+      </c>
+      <c r="Y42" s="27"/>
+      <c r="Z42"/>
+    </row>
+    <row r="43" spans="1:26" s="30" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A43" s="30" t="s">
         <v>265</v>
       </c>
@@ -3170,9 +3588,15 @@
       <c r="Q43" s="41"/>
       <c r="R43" s="54"/>
       <c r="S43" s="27"/>
-      <c r="T43"/>
-    </row>
-    <row r="44" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="T43" s="56"/>
+      <c r="U43" s="56"/>
+      <c r="V43" s="56"/>
+      <c r="W43" s="56"/>
+      <c r="X43" s="56"/>
+      <c r="Y43" s="27"/>
+      <c r="Z43"/>
+    </row>
+    <row r="44" spans="1:26" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A44" s="2" t="s">
         <v>175</v>
       </c>
@@ -3200,9 +3624,15 @@
       <c r="Q44" s="17"/>
       <c r="R44" s="54"/>
       <c r="S44" s="27"/>
-      <c r="T44"/>
-    </row>
-    <row r="45" spans="1:20" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="T44" s="56"/>
+      <c r="U44" s="56"/>
+      <c r="V44" s="56"/>
+      <c r="W44" s="56"/>
+      <c r="X44" s="56"/>
+      <c r="Y44" s="27"/>
+      <c r="Z44"/>
+    </row>
+    <row r="45" spans="1:26" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A45" s="7" t="s">
         <v>46</v>
       </c>
@@ -3224,9 +3654,10 @@
       <c r="G45" s="20"/>
       <c r="M45" s="20"/>
       <c r="S45" s="27"/>
-      <c r="T45"/>
-    </row>
-    <row r="46" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="Y45" s="27"/>
+      <c r="Z45"/>
+    </row>
+    <row r="46" spans="1:26" s="7" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A46" s="7" t="s">
         <v>48</v>
       </c>
@@ -3248,19 +3679,20 @@
       <c r="G46" s="20"/>
       <c r="M46" s="20"/>
       <c r="S46" s="27"/>
-      <c r="T46"/>
-    </row>
-    <row r="47" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A47" s="56" t="s">
+      <c r="Y46" s="27"/>
+      <c r="Z46"/>
+    </row>
+    <row r="47" spans="1:26" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A47" s="58" t="s">
         <v>51</v>
       </c>
-      <c r="B47" s="56" t="s">
+      <c r="B47" s="58" t="s">
         <v>5</v>
       </c>
-      <c r="C47" s="56" t="s">
+      <c r="C47" s="58" t="s">
         <v>52</v>
       </c>
-      <c r="D47" s="56" t="b">
+      <c r="D47" s="58" t="b">
         <v>0</v>
       </c>
       <c r="E47" s="2" t="b">
@@ -3278,13 +3710,19 @@
       <c r="Q47" s="17"/>
       <c r="R47" s="54"/>
       <c r="S47" s="27"/>
-      <c r="T47"/>
-    </row>
-    <row r="48" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A48" s="56"/>
-      <c r="B48" s="56"/>
-      <c r="C48" s="56"/>
-      <c r="D48" s="56"/>
+      <c r="T47" s="56"/>
+      <c r="U47" s="56"/>
+      <c r="V47" s="56"/>
+      <c r="W47" s="56"/>
+      <c r="X47" s="56"/>
+      <c r="Y47" s="27"/>
+      <c r="Z47"/>
+    </row>
+    <row r="48" spans="1:26" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A48" s="58"/>
+      <c r="B48" s="58"/>
+      <c r="C48" s="58"/>
+      <c r="D48" s="58"/>
       <c r="G48" s="20"/>
       <c r="L48" s="54"/>
       <c r="M48" s="20"/>
@@ -3294,9 +3732,15 @@
       <c r="Q48" s="17"/>
       <c r="R48" s="54"/>
       <c r="S48" s="27"/>
-      <c r="T48"/>
-    </row>
-    <row r="49" spans="1:20" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="T48" s="56"/>
+      <c r="U48" s="56"/>
+      <c r="V48" s="56"/>
+      <c r="W48" s="56"/>
+      <c r="X48" s="56"/>
+      <c r="Y48" s="27"/>
+      <c r="Z48"/>
+    </row>
+    <row r="49" spans="1:26" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A49" s="2" t="s">
         <v>177</v>
       </c>
@@ -3321,9 +3765,15 @@
       <c r="Q49" s="17"/>
       <c r="R49" s="54"/>
       <c r="S49" s="27"/>
-      <c r="T49"/>
-    </row>
-    <row r="50" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="T49" s="56"/>
+      <c r="U49" s="56"/>
+      <c r="V49" s="56"/>
+      <c r="W49" s="56"/>
+      <c r="X49" s="56"/>
+      <c r="Y49" s="27"/>
+      <c r="Z49"/>
+    </row>
+    <row r="50" spans="1:26" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A50" s="2" t="s">
         <v>53</v>
       </c>
@@ -3348,9 +3798,15 @@
       <c r="Q50" s="17"/>
       <c r="R50" s="54"/>
       <c r="S50" s="27"/>
-      <c r="T50"/>
-    </row>
-    <row r="51" spans="1:20" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="T50" s="56"/>
+      <c r="U50" s="56"/>
+      <c r="V50" s="56"/>
+      <c r="W50" s="56"/>
+      <c r="X50" s="56"/>
+      <c r="Y50" s="27"/>
+      <c r="Z50"/>
+    </row>
+    <row r="51" spans="1:26" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A51" s="2" t="s">
         <v>55</v>
       </c>
@@ -3378,9 +3834,15 @@
       <c r="Q51" s="17"/>
       <c r="R51" s="54"/>
       <c r="S51" s="27"/>
-      <c r="T51"/>
-    </row>
-    <row r="52" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="T51" s="56"/>
+      <c r="U51" s="56"/>
+      <c r="V51" s="56"/>
+      <c r="W51" s="56"/>
+      <c r="X51" s="56"/>
+      <c r="Y51" s="27"/>
+      <c r="Z51"/>
+    </row>
+    <row r="52" spans="1:26" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A52" s="2" t="s">
         <v>221</v>
       </c>
@@ -3392,9 +3854,6 @@
       <c r="E52" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="F52" s="2" t="s">
-        <v>284</v>
-      </c>
       <c r="G52" s="21"/>
       <c r="H52" s="33" t="s">
         <v>280</v>
@@ -3428,9 +3887,25 @@
         <v>281</v>
       </c>
       <c r="S52" s="27"/>
-      <c r="T52"/>
-    </row>
-    <row r="53" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="T52" s="56" t="s">
+        <v>339</v>
+      </c>
+      <c r="U52" s="56" t="s">
+        <v>339</v>
+      </c>
+      <c r="V52" s="56" t="s">
+        <v>339</v>
+      </c>
+      <c r="W52" s="56" t="s">
+        <v>339</v>
+      </c>
+      <c r="X52" s="56" t="s">
+        <v>339</v>
+      </c>
+      <c r="Y52" s="27"/>
+      <c r="Z52"/>
+    </row>
+    <row r="53" spans="1:26" s="7" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A53" s="7" t="s">
         <v>180</v>
       </c>
@@ -3452,9 +3927,10 @@
       <c r="G53" s="20"/>
       <c r="M53" s="20"/>
       <c r="S53" s="27"/>
-      <c r="T53"/>
-    </row>
-    <row r="54" spans="1:20" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="Y53" s="27"/>
+      <c r="Z53"/>
+    </row>
+    <row r="54" spans="1:26" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A54" s="7" t="s">
         <v>182</v>
       </c>
@@ -3476,9 +3952,10 @@
       <c r="G54" s="20"/>
       <c r="M54" s="20"/>
       <c r="S54" s="27"/>
-      <c r="T54"/>
-    </row>
-    <row r="55" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="Y54" s="27"/>
+      <c r="Z54"/>
+    </row>
+    <row r="55" spans="1:26" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A55" s="2" t="s">
         <v>58</v>
       </c>
@@ -3506,9 +3983,15 @@
       <c r="Q55" s="17"/>
       <c r="R55" s="54"/>
       <c r="S55" s="27"/>
-      <c r="T55"/>
-    </row>
-    <row r="56" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="T55" s="56"/>
+      <c r="U55" s="56"/>
+      <c r="V55" s="56"/>
+      <c r="W55" s="56"/>
+      <c r="X55" s="56"/>
+      <c r="Y55" s="27"/>
+      <c r="Z55"/>
+    </row>
+    <row r="56" spans="1:26" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A56" s="2" t="s">
         <v>60</v>
       </c>
@@ -3536,9 +4019,15 @@
       <c r="Q56" s="17"/>
       <c r="R56" s="54"/>
       <c r="S56" s="27"/>
-      <c r="T56"/>
-    </row>
-    <row r="57" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="T56" s="56"/>
+      <c r="U56" s="56"/>
+      <c r="V56" s="56"/>
+      <c r="W56" s="56"/>
+      <c r="X56" s="56"/>
+      <c r="Y56" s="27"/>
+      <c r="Z56"/>
+    </row>
+    <row r="57" spans="1:26" s="7" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A57" s="7" t="s">
         <v>62</v>
       </c>
@@ -3560,9 +4049,10 @@
       <c r="G57" s="20"/>
       <c r="M57" s="20"/>
       <c r="S57" s="27"/>
-      <c r="T57"/>
-    </row>
-    <row r="58" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="Y57" s="27"/>
+      <c r="Z57"/>
+    </row>
+    <row r="58" spans="1:26" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A58" s="2" t="s">
         <v>185</v>
       </c>
@@ -3590,9 +4080,15 @@
       <c r="Q58" s="17"/>
       <c r="R58" s="54"/>
       <c r="S58" s="27"/>
-      <c r="T58"/>
-    </row>
-    <row r="59" spans="1:20" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="T58" s="56"/>
+      <c r="U58" s="56"/>
+      <c r="V58" s="56"/>
+      <c r="W58" s="56"/>
+      <c r="X58" s="56"/>
+      <c r="Y58" s="27"/>
+      <c r="Z58"/>
+    </row>
+    <row r="59" spans="1:26" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A59" s="16" t="s">
         <v>299</v>
       </c>
@@ -3625,8 +4121,14 @@
       <c r="R59" s="16"/>
       <c r="S59" s="22"/>
       <c r="T59" s="16"/>
-    </row>
-    <row r="60" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="U59" s="16"/>
+      <c r="V59" s="16"/>
+      <c r="W59" s="16"/>
+      <c r="X59" s="16"/>
+      <c r="Y59" s="22"/>
+      <c r="Z59" s="16"/>
+    </row>
+    <row r="60" spans="1:26" s="7" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A60" s="7" t="s">
         <v>304</v>
       </c>
@@ -3648,8 +4150,9 @@
       <c r="G60" s="27"/>
       <c r="M60" s="27"/>
       <c r="S60" s="27"/>
-    </row>
-    <row r="61" spans="1:20" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="Y60" s="27"/>
+    </row>
+    <row r="61" spans="1:26" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A61" s="7" t="s">
         <v>302</v>
       </c>
@@ -3681,8 +4184,14 @@
       <c r="Q61" s="34"/>
       <c r="R61" s="34"/>
       <c r="S61" s="27"/>
-    </row>
-    <row r="62" spans="1:20" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="T61" s="34"/>
+      <c r="U61" s="34"/>
+      <c r="V61" s="34"/>
+      <c r="W61" s="34"/>
+      <c r="X61" s="34"/>
+      <c r="Y61" s="27"/>
+    </row>
+    <row r="62" spans="1:26" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A62" s="7" t="s">
         <v>187</v>
       </c>
@@ -3704,8 +4213,9 @@
       <c r="G62" s="27"/>
       <c r="M62" s="27"/>
       <c r="S62"/>
-    </row>
-    <row r="63" spans="1:20" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="Y62"/>
+    </row>
+    <row r="63" spans="1:26" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A63" s="16" t="s">
         <v>241</v>
       </c>
@@ -3737,9 +4247,15 @@
       <c r="Q63" s="16"/>
       <c r="R63" s="16"/>
       <c r="S63" s="22"/>
-      <c r="T63"/>
-    </row>
-    <row r="64" spans="1:20" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="T63" s="16"/>
+      <c r="U63" s="16"/>
+      <c r="V63" s="16"/>
+      <c r="W63" s="16"/>
+      <c r="X63" s="16"/>
+      <c r="Y63" s="22"/>
+      <c r="Z63"/>
+    </row>
+    <row r="64" spans="1:26" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A64" s="7" t="s">
         <v>189</v>
       </c>
@@ -3761,9 +4277,10 @@
       <c r="G64" s="20"/>
       <c r="M64" s="20"/>
       <c r="S64" s="27"/>
-      <c r="T64"/>
-    </row>
-    <row r="65" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="Y64" s="27"/>
+      <c r="Z64"/>
+    </row>
+    <row r="65" spans="1:26" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A65" s="2" t="s">
         <v>64</v>
       </c>
@@ -3791,9 +4308,15 @@
       <c r="Q65" s="17"/>
       <c r="R65" s="54"/>
       <c r="S65" s="27"/>
-      <c r="T65"/>
-    </row>
-    <row r="66" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="T65" s="56"/>
+      <c r="U65" s="56"/>
+      <c r="V65" s="56"/>
+      <c r="W65" s="56"/>
+      <c r="X65" s="56"/>
+      <c r="Y65" s="27"/>
+      <c r="Z65"/>
+    </row>
+    <row r="66" spans="1:26" s="7" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A66" s="7" t="s">
         <v>66</v>
       </c>
@@ -3815,9 +4338,10 @@
       <c r="G66" s="20"/>
       <c r="M66" s="20"/>
       <c r="S66" s="27"/>
-      <c r="T66"/>
-    </row>
-    <row r="67" spans="1:20" s="46" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="Y66" s="27"/>
+      <c r="Z66"/>
+    </row>
+    <row r="67" spans="1:26" s="46" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A67" s="46" t="s">
         <v>312</v>
       </c>
@@ -3841,8 +4365,14 @@
       <c r="M67" s="27"/>
       <c r="R67" s="54"/>
       <c r="S67" s="27"/>
-    </row>
-    <row r="68" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="T67" s="56"/>
+      <c r="U67" s="56"/>
+      <c r="V67" s="56"/>
+      <c r="W67" s="56"/>
+      <c r="X67" s="56"/>
+      <c r="Y67" s="27"/>
+    </row>
+    <row r="68" spans="1:26" s="7" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A68" t="s">
         <v>263</v>
       </c>
@@ -3864,9 +4394,10 @@
       <c r="G68" s="27"/>
       <c r="M68" s="27"/>
       <c r="S68" s="27"/>
-      <c r="T68"/>
-    </row>
-    <row r="69" spans="1:20" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="Y68" s="27"/>
+      <c r="Z68"/>
+    </row>
+    <row r="69" spans="1:26" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A69" s="2" t="s">
         <v>69</v>
       </c>
@@ -3894,9 +4425,15 @@
       <c r="Q69" s="17"/>
       <c r="R69" s="54"/>
       <c r="S69" s="27"/>
-      <c r="T69"/>
-    </row>
-    <row r="70" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="T69" s="56"/>
+      <c r="U69" s="56"/>
+      <c r="V69" s="56"/>
+      <c r="W69" s="56"/>
+      <c r="X69" s="56"/>
+      <c r="Y69" s="27"/>
+      <c r="Z69"/>
+    </row>
+    <row r="70" spans="1:26" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A70" s="2" t="s">
         <v>71</v>
       </c>
@@ -3924,9 +4461,25 @@
       <c r="Q70" s="17"/>
       <c r="R70" s="54"/>
       <c r="S70" s="27"/>
-      <c r="T70"/>
-    </row>
-    <row r="71" spans="1:20" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="T70" s="56" t="s">
+        <v>333</v>
+      </c>
+      <c r="U70" s="56" t="s">
+        <v>333</v>
+      </c>
+      <c r="V70" s="56" t="s">
+        <v>333</v>
+      </c>
+      <c r="W70" s="56" t="s">
+        <v>333</v>
+      </c>
+      <c r="X70" s="56" t="s">
+        <v>333</v>
+      </c>
+      <c r="Y70" s="27"/>
+      <c r="Z70"/>
+    </row>
+    <row r="71" spans="1:26" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A71" s="2" t="s">
         <v>192</v>
       </c>
@@ -3954,9 +4507,15 @@
       <c r="Q71" s="17"/>
       <c r="R71" s="54"/>
       <c r="S71" s="27"/>
-      <c r="T71"/>
-    </row>
-    <row r="72" spans="1:20" s="24" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="T71" s="56"/>
+      <c r="U71" s="56"/>
+      <c r="V71" s="56"/>
+      <c r="W71" s="56"/>
+      <c r="X71" s="56"/>
+      <c r="Y71" s="27"/>
+      <c r="Z71"/>
+    </row>
+    <row r="72" spans="1:26" s="24" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A72" s="24" t="s">
         <v>255</v>
       </c>
@@ -3980,9 +4539,15 @@
       <c r="M72" s="20"/>
       <c r="R72" s="54"/>
       <c r="S72" s="27"/>
-      <c r="T72"/>
-    </row>
-    <row r="73" spans="1:20" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="T72" s="56"/>
+      <c r="U72" s="56"/>
+      <c r="V72" s="56"/>
+      <c r="W72" s="56"/>
+      <c r="X72" s="56"/>
+      <c r="Y72" s="27"/>
+      <c r="Z72"/>
+    </row>
+    <row r="73" spans="1:26" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A73" s="2" t="s">
         <v>73</v>
       </c>
@@ -4031,9 +4596,25 @@
         <v>283</v>
       </c>
       <c r="S73" s="27"/>
-      <c r="T73"/>
-    </row>
-    <row r="74" spans="1:20" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="T73" s="56" t="s">
+        <v>339</v>
+      </c>
+      <c r="U73" s="56" t="s">
+        <v>339</v>
+      </c>
+      <c r="V73" s="56" t="s">
+        <v>339</v>
+      </c>
+      <c r="W73" s="56" t="s">
+        <v>339</v>
+      </c>
+      <c r="X73" s="56" t="s">
+        <v>339</v>
+      </c>
+      <c r="Y73" s="27"/>
+      <c r="Z73"/>
+    </row>
+    <row r="74" spans="1:26" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A74" s="48" t="s">
         <v>195</v>
       </c>
@@ -4058,9 +4639,15 @@
       <c r="Q74" s="17"/>
       <c r="R74" s="54"/>
       <c r="S74" s="27"/>
-      <c r="T74"/>
-    </row>
-    <row r="75" spans="1:20" s="52" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="T74" s="56"/>
+      <c r="U74" s="56"/>
+      <c r="V74" s="56"/>
+      <c r="W74" s="56"/>
+      <c r="X74" s="56"/>
+      <c r="Y74" s="27"/>
+      <c r="Z74"/>
+    </row>
+    <row r="75" spans="1:26" s="52" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A75" s="52" t="s">
         <v>324</v>
       </c>
@@ -4084,8 +4671,14 @@
       <c r="M75" s="27"/>
       <c r="R75" s="54"/>
       <c r="S75" s="27"/>
-    </row>
-    <row r="76" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="T75" s="56"/>
+      <c r="U75" s="56"/>
+      <c r="V75" s="56"/>
+      <c r="W75" s="56"/>
+      <c r="X75" s="56"/>
+      <c r="Y75" s="27"/>
+    </row>
+    <row r="76" spans="1:26" s="7" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A76" s="7" t="s">
         <v>75</v>
       </c>
@@ -4107,9 +4700,10 @@
       <c r="G76" s="20"/>
       <c r="M76" s="20"/>
       <c r="S76" s="27"/>
-      <c r="T76"/>
-    </row>
-    <row r="77" spans="1:20" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="Y76" s="27"/>
+      <c r="Z76"/>
+    </row>
+    <row r="77" spans="1:26" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A77" s="44" t="s">
         <v>320</v>
       </c>
@@ -4131,8 +4725,9 @@
       <c r="G77" s="27"/>
       <c r="M77" s="27"/>
       <c r="S77" s="27"/>
-    </row>
-    <row r="78" spans="1:20" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="Y77" s="27"/>
+    </row>
+    <row r="78" spans="1:26" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A78" s="2" t="s">
         <v>219</v>
       </c>
@@ -4160,9 +4755,15 @@
       <c r="Q78" s="17"/>
       <c r="R78" s="54"/>
       <c r="S78" s="27"/>
-      <c r="T78"/>
-    </row>
-    <row r="79" spans="1:20" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="T78" s="56"/>
+      <c r="U78" s="56"/>
+      <c r="V78" s="56"/>
+      <c r="W78" s="56"/>
+      <c r="X78" s="56"/>
+      <c r="Y78" s="27"/>
+      <c r="Z78"/>
+    </row>
+    <row r="79" spans="1:26" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A79" s="2" t="s">
         <v>77</v>
       </c>
@@ -4190,9 +4791,15 @@
       <c r="Q79" s="17"/>
       <c r="R79" s="54"/>
       <c r="S79" s="27"/>
-      <c r="T79"/>
-    </row>
-    <row r="80" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="T79" s="56"/>
+      <c r="U79" s="56"/>
+      <c r="V79" s="56"/>
+      <c r="W79" s="56"/>
+      <c r="X79" s="56"/>
+      <c r="Y79" s="27"/>
+      <c r="Z79"/>
+    </row>
+    <row r="80" spans="1:26" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A80" s="2" t="s">
         <v>79</v>
       </c>
@@ -4242,9 +4849,25 @@
         <v>281</v>
       </c>
       <c r="S80" s="27"/>
-      <c r="T80"/>
-    </row>
-    <row r="81" spans="1:23" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="T80" s="56" t="s">
+        <v>339</v>
+      </c>
+      <c r="U80" s="56" t="s">
+        <v>339</v>
+      </c>
+      <c r="V80" s="56" t="s">
+        <v>339</v>
+      </c>
+      <c r="W80" s="56" t="s">
+        <v>339</v>
+      </c>
+      <c r="X80" s="56" t="s">
+        <v>339</v>
+      </c>
+      <c r="Y80" s="27"/>
+      <c r="Z80"/>
+    </row>
+    <row r="81" spans="1:29" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A81" s="2" t="s">
         <v>81</v>
       </c>
@@ -4272,9 +4895,15 @@
       <c r="Q81" s="17"/>
       <c r="R81" s="54"/>
       <c r="S81" s="27"/>
-      <c r="T81"/>
-    </row>
-    <row r="82" spans="1:23" s="7" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="T81" s="56"/>
+      <c r="U81" s="56"/>
+      <c r="V81" s="56"/>
+      <c r="W81" s="56"/>
+      <c r="X81" s="56"/>
+      <c r="Y81" s="27"/>
+      <c r="Z81"/>
+    </row>
+    <row r="82" spans="1:29" s="7" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A82" s="7" t="s">
         <v>84</v>
       </c>
@@ -4296,9 +4925,10 @@
       <c r="G82" s="20"/>
       <c r="M82" s="20"/>
       <c r="S82" s="27"/>
-      <c r="T82"/>
-    </row>
-    <row r="83" spans="1:23" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="Y82" s="27"/>
+      <c r="Z82"/>
+    </row>
+    <row r="83" spans="1:29" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A83" s="2" t="s">
         <v>196</v>
       </c>
@@ -4335,9 +4965,15 @@
       <c r="Q83" s="17"/>
       <c r="R83" s="54"/>
       <c r="S83" s="27"/>
-      <c r="T83"/>
-    </row>
-    <row r="84" spans="1:23" s="7" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="T83" s="56"/>
+      <c r="U83" s="56"/>
+      <c r="V83" s="56"/>
+      <c r="W83" s="56"/>
+      <c r="X83" s="56"/>
+      <c r="Y83" s="27"/>
+      <c r="Z83"/>
+    </row>
+    <row r="84" spans="1:29" s="7" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A84" s="7" t="s">
         <v>199</v>
       </c>
@@ -4359,9 +4995,10 @@
       <c r="G84" s="20"/>
       <c r="M84" s="20"/>
       <c r="S84" s="27"/>
-      <c r="T84"/>
-    </row>
-    <row r="85" spans="1:23" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="Y84" s="27"/>
+      <c r="Z84"/>
+    </row>
+    <row r="85" spans="1:29" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A85" s="2" t="s">
         <v>86</v>
       </c>
@@ -4410,9 +5047,25 @@
         <v>281</v>
       </c>
       <c r="S85" s="27"/>
-      <c r="T85"/>
-    </row>
-    <row r="86" spans="1:23" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="T85" s="56" t="s">
+        <v>340</v>
+      </c>
+      <c r="U85" s="57" t="s">
+        <v>340</v>
+      </c>
+      <c r="V85" s="57" t="s">
+        <v>340</v>
+      </c>
+      <c r="W85" s="57" t="s">
+        <v>340</v>
+      </c>
+      <c r="X85" s="57" t="s">
+        <v>340</v>
+      </c>
+      <c r="Y85" s="27"/>
+      <c r="Z85"/>
+    </row>
+    <row r="86" spans="1:29" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A86" s="2" t="s">
         <v>88</v>
       </c>
@@ -4440,9 +5093,15 @@
       <c r="Q86" s="17"/>
       <c r="R86" s="54"/>
       <c r="S86" s="27"/>
-      <c r="T86"/>
-    </row>
-    <row r="87" spans="1:23" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="T86" s="56"/>
+      <c r="U86" s="56"/>
+      <c r="V86" s="56"/>
+      <c r="W86" s="56"/>
+      <c r="X86" s="56"/>
+      <c r="Y86" s="27"/>
+      <c r="Z86"/>
+    </row>
+    <row r="87" spans="1:29" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A87" s="7" t="s">
         <v>92</v>
       </c>
@@ -4464,9 +5123,10 @@
       <c r="G87" s="20"/>
       <c r="M87" s="20"/>
       <c r="S87" s="27"/>
-      <c r="T87"/>
-    </row>
-    <row r="88" spans="1:23" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="Y87" s="27"/>
+      <c r="Z87"/>
+    </row>
+    <row r="88" spans="1:29" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A88" s="7" t="s">
         <v>149</v>
       </c>
@@ -4488,9 +5148,10 @@
       <c r="G88" s="20"/>
       <c r="M88" s="20"/>
       <c r="S88" s="27"/>
-      <c r="T88"/>
-    </row>
-    <row r="89" spans="1:23" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="Y88" s="27"/>
+      <c r="Z88"/>
+    </row>
+    <row r="89" spans="1:29" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A89" s="44" t="s">
         <v>331</v>
       </c>
@@ -4526,12 +5187,20 @@
         <v>4</v>
       </c>
       <c r="S89" s="45"/>
-      <c r="T89" s="55"/>
+      <c r="T89" s="44"/>
       <c r="U89" s="44"/>
       <c r="V89" s="44"/>
       <c r="W89" s="44"/>
-    </row>
-    <row r="90" spans="1:23" s="2" customFormat="1" ht="58.3" x14ac:dyDescent="0.4">
+      <c r="X89" s="44" t="s">
+        <v>4</v>
+      </c>
+      <c r="Y89" s="45"/>
+      <c r="Z89" s="55"/>
+      <c r="AA89" s="44"/>
+      <c r="AB89" s="44"/>
+      <c r="AC89" s="44"/>
+    </row>
+    <row r="90" spans="1:29" s="2" customFormat="1" ht="58.3" x14ac:dyDescent="0.4">
       <c r="A90" s="2" t="s">
         <v>96</v>
       </c>
@@ -4559,9 +5228,15 @@
       <c r="Q90" s="17"/>
       <c r="R90" s="54"/>
       <c r="S90" s="27"/>
-      <c r="T90"/>
-    </row>
-    <row r="91" spans="1:23" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="T90" s="56"/>
+      <c r="U90" s="56"/>
+      <c r="V90" s="56"/>
+      <c r="W90" s="56"/>
+      <c r="X90" s="56"/>
+      <c r="Y90" s="27"/>
+      <c r="Z90"/>
+    </row>
+    <row r="91" spans="1:29" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A91" s="2" t="s">
         <v>226</v>
       </c>
@@ -4606,9 +5281,25 @@
         <v>16</v>
       </c>
       <c r="S91" s="27"/>
-      <c r="T91"/>
-    </row>
-    <row r="92" spans="1:23" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="T91" s="56" t="s">
+        <v>16</v>
+      </c>
+      <c r="U91" s="56" t="s">
+        <v>16</v>
+      </c>
+      <c r="V91" s="56" t="s">
+        <v>4</v>
+      </c>
+      <c r="W91" s="56" t="s">
+        <v>4</v>
+      </c>
+      <c r="X91" s="56" t="s">
+        <v>16</v>
+      </c>
+      <c r="Y91" s="27"/>
+      <c r="Z91"/>
+    </row>
+    <row r="92" spans="1:29" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A92" s="2" t="s">
         <v>151</v>
       </c>
@@ -4636,9 +5327,15 @@
       <c r="Q92" s="17"/>
       <c r="R92" s="54"/>
       <c r="S92" s="27"/>
-      <c r="T92"/>
-    </row>
-    <row r="93" spans="1:23" s="31" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="T92" s="56"/>
+      <c r="U92" s="56"/>
+      <c r="V92" s="56"/>
+      <c r="W92" s="56"/>
+      <c r="X92" s="56"/>
+      <c r="Y92" s="27"/>
+      <c r="Z92"/>
+    </row>
+    <row r="93" spans="1:29" s="31" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A93" s="31" t="s">
         <v>99</v>
       </c>
@@ -4662,9 +5359,15 @@
       <c r="M93" s="27"/>
       <c r="R93" s="54"/>
       <c r="S93" s="27"/>
-      <c r="T93"/>
-    </row>
-    <row r="94" spans="1:23" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="T93" s="56"/>
+      <c r="U93" s="56"/>
+      <c r="V93" s="56"/>
+      <c r="W93" s="56"/>
+      <c r="X93" s="56"/>
+      <c r="Y93" s="27"/>
+      <c r="Z93"/>
+    </row>
+    <row r="94" spans="1:29" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A94" s="2" t="s">
         <v>201</v>
       </c>
@@ -4692,9 +5395,15 @@
       <c r="Q94" s="17"/>
       <c r="R94" s="54"/>
       <c r="S94" s="27"/>
-      <c r="T94"/>
-    </row>
-    <row r="95" spans="1:23" s="14" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="T94" s="56"/>
+      <c r="U94" s="56"/>
+      <c r="V94" s="56"/>
+      <c r="W94" s="56"/>
+      <c r="X94" s="56"/>
+      <c r="Y94" s="27"/>
+      <c r="Z94"/>
+    </row>
+    <row r="95" spans="1:29" s="14" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A95" s="14" t="s">
         <v>249</v>
       </c>
@@ -4722,9 +5431,15 @@
       <c r="Q95" s="17"/>
       <c r="R95" s="54"/>
       <c r="S95" s="27"/>
-      <c r="T95"/>
-    </row>
-    <row r="96" spans="1:23" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="T95" s="56"/>
+      <c r="U95" s="56"/>
+      <c r="V95" s="56"/>
+      <c r="W95" s="56"/>
+      <c r="X95" s="56"/>
+      <c r="Y95" s="27"/>
+      <c r="Z95"/>
+    </row>
+    <row r="96" spans="1:29" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A96" s="2" t="s">
         <v>222</v>
       </c>
@@ -4751,9 +5466,15 @@
       <c r="Q96" s="35"/>
       <c r="R96" s="54"/>
       <c r="S96" s="27"/>
-      <c r="T96"/>
-    </row>
-    <row r="97" spans="1:20" s="2" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="T96" s="56"/>
+      <c r="U96" s="56"/>
+      <c r="V96" s="56"/>
+      <c r="W96" s="56"/>
+      <c r="X96" s="56"/>
+      <c r="Y96" s="27"/>
+      <c r="Z96"/>
+    </row>
+    <row r="97" spans="1:26" s="2" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A97" s="2" t="s">
         <v>101</v>
       </c>
@@ -4781,9 +5502,15 @@
       <c r="Q97" s="17"/>
       <c r="R97" s="54"/>
       <c r="S97" s="27"/>
-      <c r="T97"/>
-    </row>
-    <row r="98" spans="1:20" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="T97" s="56"/>
+      <c r="U97" s="56"/>
+      <c r="V97" s="56"/>
+      <c r="W97" s="56"/>
+      <c r="X97" s="56"/>
+      <c r="Y97" s="27"/>
+      <c r="Z97"/>
+    </row>
+    <row r="98" spans="1:26" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A98" t="s">
         <v>293</v>
       </c>
@@ -4805,9 +5532,10 @@
       <c r="G98" s="27"/>
       <c r="M98" s="27"/>
       <c r="S98" s="27"/>
-      <c r="T98"/>
-    </row>
-    <row r="99" spans="1:20" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="Y98" s="27"/>
+      <c r="Z98"/>
+    </row>
+    <row r="99" spans="1:26" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A99" s="2" t="s">
         <v>103</v>
       </c>
@@ -4835,9 +5563,15 @@
       <c r="Q99" s="17"/>
       <c r="R99" s="54"/>
       <c r="S99" s="27"/>
-      <c r="T99"/>
-    </row>
-    <row r="100" spans="1:20" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="T99" s="56"/>
+      <c r="U99" s="56"/>
+      <c r="V99" s="56"/>
+      <c r="W99" s="56"/>
+      <c r="X99" s="56"/>
+      <c r="Y99" s="27"/>
+      <c r="Z99"/>
+    </row>
+    <row r="100" spans="1:26" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A100" s="2" t="s">
         <v>105</v>
       </c>
@@ -4865,9 +5599,15 @@
       <c r="Q100" s="17"/>
       <c r="R100" s="54"/>
       <c r="S100" s="27"/>
-      <c r="T100"/>
-    </row>
-    <row r="101" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="T100" s="56"/>
+      <c r="U100" s="56"/>
+      <c r="V100" s="56"/>
+      <c r="W100" s="56"/>
+      <c r="X100" s="56"/>
+      <c r="Y100" s="27"/>
+      <c r="Z100"/>
+    </row>
+    <row r="101" spans="1:26" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A101" s="2" t="s">
         <v>204</v>
       </c>
@@ -4892,9 +5632,15 @@
       <c r="Q101" s="17"/>
       <c r="R101" s="54"/>
       <c r="S101" s="27"/>
-      <c r="T101"/>
-    </row>
-    <row r="102" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="T101" s="56"/>
+      <c r="U101" s="56"/>
+      <c r="V101" s="56"/>
+      <c r="W101" s="56"/>
+      <c r="X101" s="56"/>
+      <c r="Y101" s="27"/>
+      <c r="Z101"/>
+    </row>
+    <row r="102" spans="1:26" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A102" s="2" t="s">
         <v>107</v>
       </c>
@@ -4922,9 +5668,15 @@
       <c r="Q102" s="17"/>
       <c r="R102" s="54"/>
       <c r="S102" s="27"/>
-      <c r="T102"/>
-    </row>
-    <row r="103" spans="1:20" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="T102" s="56"/>
+      <c r="U102" s="56"/>
+      <c r="V102" s="56"/>
+      <c r="W102" s="56"/>
+      <c r="X102" s="56"/>
+      <c r="Y102" s="27"/>
+      <c r="Z102"/>
+    </row>
+    <row r="103" spans="1:26" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A103" s="2" t="s">
         <v>111</v>
       </c>
@@ -4973,9 +5725,25 @@
         <v>283</v>
       </c>
       <c r="S103" s="27"/>
-      <c r="T103"/>
-    </row>
-    <row r="104" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="T103" s="56" t="s">
+        <v>339</v>
+      </c>
+      <c r="U103" s="56" t="s">
+        <v>339</v>
+      </c>
+      <c r="V103" s="56" t="s">
+        <v>339</v>
+      </c>
+      <c r="W103" s="56" t="s">
+        <v>339</v>
+      </c>
+      <c r="X103" s="56" t="s">
+        <v>339</v>
+      </c>
+      <c r="Y103" s="27"/>
+      <c r="Z103"/>
+    </row>
+    <row r="104" spans="1:26" s="7" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A104" s="7" t="s">
         <v>113</v>
       </c>
@@ -4997,9 +5765,10 @@
       <c r="G104" s="20"/>
       <c r="M104" s="20"/>
       <c r="S104" s="27"/>
-      <c r="T104"/>
-    </row>
-    <row r="105" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="Y104" s="27"/>
+      <c r="Z104"/>
+    </row>
+    <row r="105" spans="1:26" s="7" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A105" s="7" t="s">
         <v>115</v>
       </c>
@@ -5021,9 +5790,10 @@
       <c r="G105" s="20"/>
       <c r="M105" s="20"/>
       <c r="S105" s="27"/>
-      <c r="T105"/>
-    </row>
-    <row r="106" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="Y105" s="27"/>
+      <c r="Z105"/>
+    </row>
+    <row r="106" spans="1:26" s="7" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A106" s="7" t="s">
         <v>117</v>
       </c>
@@ -5045,9 +5815,10 @@
       <c r="G106" s="20"/>
       <c r="M106" s="20"/>
       <c r="S106" s="27"/>
-      <c r="T106"/>
-    </row>
-    <row r="107" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="Y106" s="27"/>
+      <c r="Z106"/>
+    </row>
+    <row r="107" spans="1:26" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A107" s="2" t="s">
         <v>119</v>
       </c>
@@ -5096,9 +5867,25 @@
         <v>4</v>
       </c>
       <c r="S107" s="27"/>
-      <c r="T107"/>
-    </row>
-    <row r="108" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="T107" s="56" t="s">
+        <v>4</v>
+      </c>
+      <c r="U107" s="56" t="s">
+        <v>4</v>
+      </c>
+      <c r="V107" s="56" t="s">
+        <v>4</v>
+      </c>
+      <c r="W107" s="56" t="s">
+        <v>4</v>
+      </c>
+      <c r="X107" s="56" t="s">
+        <v>4</v>
+      </c>
+      <c r="Y107" s="27"/>
+      <c r="Z107"/>
+    </row>
+    <row r="108" spans="1:26" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A108" s="2" t="s">
         <v>121</v>
       </c>
@@ -5147,9 +5934,25 @@
         <v>4</v>
       </c>
       <c r="S108" s="27"/>
-      <c r="T108"/>
-    </row>
-    <row r="109" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="T108" s="56" t="s">
+        <v>4</v>
+      </c>
+      <c r="U108" s="56" t="s">
+        <v>4</v>
+      </c>
+      <c r="V108" s="56" t="s">
+        <v>4</v>
+      </c>
+      <c r="W108" s="56" t="s">
+        <v>4</v>
+      </c>
+      <c r="X108" s="56" t="s">
+        <v>4</v>
+      </c>
+      <c r="Y108" s="27"/>
+      <c r="Z108"/>
+    </row>
+    <row r="109" spans="1:26" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A109" s="2" t="s">
         <v>123</v>
       </c>
@@ -5198,9 +6001,25 @@
         <v>4</v>
       </c>
       <c r="S109" s="27"/>
-      <c r="T109"/>
-    </row>
-    <row r="110" spans="1:20" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="T109" s="56" t="s">
+        <v>16</v>
+      </c>
+      <c r="U109" s="56" t="s">
+        <v>4</v>
+      </c>
+      <c r="V109" s="56" t="s">
+        <v>4</v>
+      </c>
+      <c r="W109" s="56" t="s">
+        <v>4</v>
+      </c>
+      <c r="X109" s="56" t="s">
+        <v>4</v>
+      </c>
+      <c r="Y109" s="27"/>
+      <c r="Z109"/>
+    </row>
+    <row r="110" spans="1:26" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A110" s="2" t="s">
         <v>153</v>
       </c>
@@ -5249,11 +6068,27 @@
         <v>16</v>
       </c>
       <c r="S110" s="27"/>
-      <c r="T110" t="s">
+      <c r="T110" s="56" t="s">
+        <v>16</v>
+      </c>
+      <c r="U110" s="56" t="s">
+        <v>16</v>
+      </c>
+      <c r="V110" s="56" t="s">
+        <v>4</v>
+      </c>
+      <c r="W110" s="56" t="s">
+        <v>4</v>
+      </c>
+      <c r="X110" s="56" t="s">
+        <v>16</v>
+      </c>
+      <c r="Y110" s="27"/>
+      <c r="Z110" t="s">
         <v>297</v>
       </c>
     </row>
-    <row r="111" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="111" spans="1:26" s="7" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A111" t="s">
         <v>295</v>
       </c>
@@ -5304,10 +6139,26 @@
       </c>
       <c r="S111" s="27"/>
       <c r="T111" t="s">
+        <v>16</v>
+      </c>
+      <c r="U111" t="s">
+        <v>16</v>
+      </c>
+      <c r="V111" t="s">
+        <v>4</v>
+      </c>
+      <c r="W111" t="s">
+        <v>4</v>
+      </c>
+      <c r="X111" t="s">
+        <v>16</v>
+      </c>
+      <c r="Y111" s="27"/>
+      <c r="Z111" t="s">
         <v>298</v>
       </c>
     </row>
-    <row r="112" spans="1:20" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="112" spans="1:26" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A112" s="7" t="s">
         <v>125</v>
       </c>
@@ -5329,8 +6180,9 @@
       <c r="G112" s="20"/>
       <c r="M112" s="20"/>
       <c r="S112" s="27"/>
-    </row>
-    <row r="113" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="Y112" s="27"/>
+    </row>
+    <row r="113" spans="1:26" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A113" s="2" t="s">
         <v>128</v>
       </c>
@@ -5379,8 +6231,24 @@
         <v>4</v>
       </c>
       <c r="S113" s="27"/>
-    </row>
-    <row r="114" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="T113" s="56" t="s">
+        <v>16</v>
+      </c>
+      <c r="U113" s="56" t="s">
+        <v>4</v>
+      </c>
+      <c r="V113" s="56" t="s">
+        <v>4</v>
+      </c>
+      <c r="W113" s="56" t="s">
+        <v>4</v>
+      </c>
+      <c r="X113" s="56" t="s">
+        <v>4</v>
+      </c>
+      <c r="Y113" s="27"/>
+    </row>
+    <row r="114" spans="1:26" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A114" s="2" t="s">
         <v>240</v>
       </c>
@@ -5429,8 +6297,24 @@
         <v>4</v>
       </c>
       <c r="S114" s="27"/>
-    </row>
-    <row r="115" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="T114" s="56" t="s">
+        <v>16</v>
+      </c>
+      <c r="U114" s="56" t="s">
+        <v>4</v>
+      </c>
+      <c r="V114" s="56" t="s">
+        <v>4</v>
+      </c>
+      <c r="W114" s="56" t="s">
+        <v>4</v>
+      </c>
+      <c r="X114" s="56" t="s">
+        <v>4</v>
+      </c>
+      <c r="Y114" s="27"/>
+    </row>
+    <row r="115" spans="1:26" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A115" s="2" t="s">
         <v>131</v>
       </c>
@@ -5458,8 +6342,14 @@
       <c r="Q115" s="17"/>
       <c r="R115" s="54"/>
       <c r="S115" s="27"/>
-    </row>
-    <row r="116" spans="1:20" s="49" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="T115" s="56"/>
+      <c r="U115" s="56"/>
+      <c r="V115" s="56"/>
+      <c r="W115" s="56"/>
+      <c r="X115" s="56"/>
+      <c r="Y115" s="27"/>
+    </row>
+    <row r="116" spans="1:26" s="49" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A116" s="49" t="s">
         <v>318</v>
       </c>
@@ -5508,8 +6398,24 @@
         <v>281</v>
       </c>
       <c r="S116" s="27"/>
-    </row>
-    <row r="117" spans="1:20" s="25" customFormat="1" ht="58.3" x14ac:dyDescent="0.4">
+      <c r="T116" s="56" t="s">
+        <v>339</v>
+      </c>
+      <c r="U116" s="56" t="s">
+        <v>339</v>
+      </c>
+      <c r="V116" s="56" t="s">
+        <v>339</v>
+      </c>
+      <c r="W116" s="56" t="s">
+        <v>339</v>
+      </c>
+      <c r="X116" s="56" t="s">
+        <v>339</v>
+      </c>
+      <c r="Y116" s="27"/>
+    </row>
+    <row r="117" spans="1:26" s="25" customFormat="1" ht="58.3" x14ac:dyDescent="0.4">
       <c r="A117" s="26" t="s">
         <v>258</v>
       </c>
@@ -5538,8 +6444,14 @@
       <c r="N117" s="26"/>
       <c r="R117" s="54"/>
       <c r="S117" s="27"/>
-    </row>
-    <row r="118" spans="1:20" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="T117" s="56"/>
+      <c r="U117" s="56"/>
+      <c r="V117" s="56"/>
+      <c r="W117" s="56"/>
+      <c r="X117" s="56"/>
+      <c r="Y117" s="27"/>
+    </row>
+    <row r="118" spans="1:26" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A118" s="2" t="s">
         <v>133</v>
       </c>
@@ -5567,72 +6479,78 @@
       <c r="Q118" s="17"/>
       <c r="R118" s="54"/>
       <c r="S118" s="27"/>
-    </row>
-    <row r="119" spans="1:20" x14ac:dyDescent="0.4">
-      <c r="T119"/>
-    </row>
-    <row r="120" spans="1:20" x14ac:dyDescent="0.4">
-      <c r="T120"/>
-    </row>
-    <row r="121" spans="1:20" x14ac:dyDescent="0.4">
-      <c r="T121"/>
-    </row>
-    <row r="122" spans="1:20" x14ac:dyDescent="0.4">
-      <c r="T122"/>
-    </row>
-    <row r="123" spans="1:20" x14ac:dyDescent="0.4">
-      <c r="T123"/>
-    </row>
-    <row r="124" spans="1:20" x14ac:dyDescent="0.4">
-      <c r="T124"/>
-    </row>
-    <row r="125" spans="1:20" x14ac:dyDescent="0.4">
-      <c r="T125"/>
-    </row>
-    <row r="126" spans="1:20" x14ac:dyDescent="0.4">
-      <c r="T126"/>
-    </row>
-    <row r="127" spans="1:20" x14ac:dyDescent="0.4">
-      <c r="T127"/>
-    </row>
-    <row r="128" spans="1:20" x14ac:dyDescent="0.4">
-      <c r="T128"/>
-    </row>
-    <row r="129" spans="20:20" x14ac:dyDescent="0.4">
-      <c r="T129"/>
-    </row>
-    <row r="130" spans="20:20" x14ac:dyDescent="0.4">
-      <c r="T130"/>
-    </row>
-    <row r="131" spans="20:20" x14ac:dyDescent="0.4">
-      <c r="T131"/>
-    </row>
-    <row r="132" spans="20:20" x14ac:dyDescent="0.4">
-      <c r="T132"/>
-    </row>
-    <row r="133" spans="20:20" x14ac:dyDescent="0.4">
-      <c r="T133"/>
-    </row>
-    <row r="134" spans="20:20" x14ac:dyDescent="0.4">
-      <c r="T134"/>
-    </row>
-    <row r="135" spans="20:20" x14ac:dyDescent="0.4">
-      <c r="T135"/>
-    </row>
-    <row r="136" spans="20:20" x14ac:dyDescent="0.4">
-      <c r="T136"/>
-    </row>
-    <row r="137" spans="20:20" x14ac:dyDescent="0.4">
-      <c r="T137"/>
-    </row>
-    <row r="138" spans="20:20" x14ac:dyDescent="0.4">
-      <c r="T138"/>
-    </row>
-    <row r="139" spans="20:20" x14ac:dyDescent="0.4">
-      <c r="T139"/>
-    </row>
-    <row r="140" spans="20:20" x14ac:dyDescent="0.4">
-      <c r="T140"/>
+      <c r="T118" s="56"/>
+      <c r="U118" s="56"/>
+      <c r="V118" s="56"/>
+      <c r="W118" s="56"/>
+      <c r="X118" s="56"/>
+      <c r="Y118" s="27"/>
+    </row>
+    <row r="119" spans="1:26" x14ac:dyDescent="0.4">
+      <c r="Z119"/>
+    </row>
+    <row r="120" spans="1:26" x14ac:dyDescent="0.4">
+      <c r="Z120"/>
+    </row>
+    <row r="121" spans="1:26" x14ac:dyDescent="0.4">
+      <c r="Z121"/>
+    </row>
+    <row r="122" spans="1:26" x14ac:dyDescent="0.4">
+      <c r="Z122"/>
+    </row>
+    <row r="123" spans="1:26" x14ac:dyDescent="0.4">
+      <c r="Z123"/>
+    </row>
+    <row r="124" spans="1:26" x14ac:dyDescent="0.4">
+      <c r="Z124"/>
+    </row>
+    <row r="125" spans="1:26" x14ac:dyDescent="0.4">
+      <c r="Z125"/>
+    </row>
+    <row r="126" spans="1:26" x14ac:dyDescent="0.4">
+      <c r="Z126"/>
+    </row>
+    <row r="127" spans="1:26" x14ac:dyDescent="0.4">
+      <c r="Z127"/>
+    </row>
+    <row r="128" spans="1:26" x14ac:dyDescent="0.4">
+      <c r="Z128"/>
+    </row>
+    <row r="129" spans="26:26" x14ac:dyDescent="0.4">
+      <c r="Z129"/>
+    </row>
+    <row r="130" spans="26:26" x14ac:dyDescent="0.4">
+      <c r="Z130"/>
+    </row>
+    <row r="131" spans="26:26" x14ac:dyDescent="0.4">
+      <c r="Z131"/>
+    </row>
+    <row r="132" spans="26:26" x14ac:dyDescent="0.4">
+      <c r="Z132"/>
+    </row>
+    <row r="133" spans="26:26" x14ac:dyDescent="0.4">
+      <c r="Z133"/>
+    </row>
+    <row r="134" spans="26:26" x14ac:dyDescent="0.4">
+      <c r="Z134"/>
+    </row>
+    <row r="135" spans="26:26" x14ac:dyDescent="0.4">
+      <c r="Z135"/>
+    </row>
+    <row r="136" spans="26:26" x14ac:dyDescent="0.4">
+      <c r="Z136"/>
+    </row>
+    <row r="137" spans="26:26" x14ac:dyDescent="0.4">
+      <c r="Z137"/>
+    </row>
+    <row r="138" spans="26:26" x14ac:dyDescent="0.4">
+      <c r="Z138"/>
+    </row>
+    <row r="139" spans="26:26" x14ac:dyDescent="0.4">
+      <c r="Z139"/>
+    </row>
+    <row r="140" spans="26:26" x14ac:dyDescent="0.4">
+      <c r="Z140"/>
     </row>
   </sheetData>
   <mergeCells count="8">

</xml_diff>

<commit_message>
Geonovum: Correcte extensie naam voor NEN3610-2022 modellen
Bugfix in properties
</commit_message>
<xml_diff>
--- a/src/main/resources/input/Geonovum/props/Geonovum.xlsx
+++ b/src/main/resources/input/Geonovum/props/Geonovum.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\gitprojects\Imvertor-Maven\src\main\resources\input\Geonovum\props\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0A7DC56-3037-435A-B1A5-679E53E2FD3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6B7092A-9021-4637-A996-8BCC258160C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38290" yWindow="2280" windowWidth="38620" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="20057" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Geonovum" sheetId="3" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="904" uniqueCount="353">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="834" uniqueCount="350">
   <si>
     <t>Name</t>
   </si>
@@ -874,12 +874,6 @@
     <t>MIMLM</t>
   </si>
   <si>
-    <t>Geonovum-MIMCM</t>
-  </si>
-  <si>
-    <t>Geonovum-MIMLM</t>
-  </si>
-  <si>
     <t>Geonovum</t>
   </si>
   <si>
@@ -1043,9 +1037,6 @@
   </si>
   <si>
     <t>NEN3610-2022: regtest</t>
-  </si>
-  <si>
-    <t>Geonovum-NEN3610-2022</t>
   </si>
   <si>
     <t>NEN3610-2022</t>
@@ -1584,10 +1575,10 @@
   <dimension ref="A1:AC144"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B73" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B81" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F76" sqref="F76"/>
+      <selection pane="bottomRight" activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -1707,7 +1698,7 @@
         <v>276</v>
       </c>
       <c r="L2" s="3" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="M2" s="15"/>
       <c r="N2" s="3" t="s">
@@ -1723,23 +1714,23 @@
         <v>279</v>
       </c>
       <c r="R2" s="3" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="S2" s="15"/>
       <c r="T2" s="3" t="s">
+        <v>332</v>
+      </c>
+      <c r="U2" s="3" t="s">
+        <v>333</v>
+      </c>
+      <c r="V2" s="3" t="s">
         <v>334</v>
       </c>
-      <c r="U2" s="3" t="s">
+      <c r="W2" s="3" t="s">
         <v>335</v>
       </c>
-      <c r="V2" s="3" t="s">
+      <c r="X2" s="3" t="s">
         <v>336</v>
-      </c>
-      <c r="W2" s="3" t="s">
-        <v>337</v>
-      </c>
-      <c r="X2" s="3" t="s">
-        <v>338</v>
       </c>
       <c r="Y2" s="15"/>
       <c r="Z2" s="5"/>
@@ -2148,7 +2139,7 @@
         <v>1</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="G18" s="16"/>
       <c r="M18" s="16"/>
@@ -2195,7 +2186,7 @@
         <v>1</v>
       </c>
       <c r="F20" s="20" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="G20" s="16"/>
       <c r="M20" s="16"/>
@@ -2220,7 +2211,7 @@
         <v>1</v>
       </c>
       <c r="F21" s="20" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="G21" s="16"/>
       <c r="M21" s="16"/>
@@ -2478,13 +2469,13 @@
     </row>
     <row r="27" spans="1:26" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A27" s="2" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="B27" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="D27" s="2" t="b">
         <v>0</v>
@@ -2678,13 +2669,13 @@
     </row>
     <row r="30" spans="1:26" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A30" s="2" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="B30" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="D30" s="2" t="b">
         <v>0</v>
@@ -2836,13 +2827,13 @@
     </row>
     <row r="33" spans="1:26" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A33" s="2" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B33" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="D33" s="2" t="b">
         <v>0</v>
@@ -2935,22 +2926,22 @@
     </row>
     <row r="37" spans="1:26" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A37" s="2" t="s">
+        <v>285</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>286</v>
+      </c>
+      <c r="C37" s="2" t="s">
         <v>287</v>
       </c>
-      <c r="B37" s="2" t="s">
+      <c r="D37" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E37" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F37" s="2" t="s">
         <v>288</v>
-      </c>
-      <c r="C37" s="2" t="s">
-        <v>289</v>
-      </c>
-      <c r="D37" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E37" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F37" s="2" t="s">
-        <v>290</v>
       </c>
       <c r="G37" s="16"/>
       <c r="M37" s="16"/>
@@ -3026,13 +3017,13 @@
     </row>
     <row r="39" spans="1:26" s="21" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A39" s="21" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="B39" s="21" t="s">
         <v>5</v>
       </c>
       <c r="C39" s="21" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="D39" s="21" t="b">
         <v>0</v>
@@ -3267,7 +3258,7 @@
         <v>1</v>
       </c>
       <c r="F43" s="23" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="G43" s="16"/>
       <c r="M43" s="16"/>
@@ -3455,8 +3446,8 @@
       <c r="Y51" s="16"/>
       <c r="Z51"/>
     </row>
-    <row r="52" spans="1:26" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A52" s="2" t="s">
+    <row r="52" spans="1:26" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A52" s="8" t="s">
         <v>221</v>
       </c>
       <c r="B52" s="8"/>
@@ -3468,53 +3459,8 @@
         <v>0</v>
       </c>
       <c r="G52" s="17"/>
-      <c r="H52" s="2" t="s">
-        <v>280</v>
-      </c>
-      <c r="I52" s="2" t="s">
-        <v>280</v>
-      </c>
-      <c r="J52" s="2" t="s">
-        <v>280</v>
-      </c>
-      <c r="K52" s="2" t="s">
-        <v>280</v>
-      </c>
-      <c r="L52" s="2" t="s">
-        <v>280</v>
-      </c>
       <c r="M52" s="17"/>
-      <c r="N52" s="2" t="s">
-        <v>281</v>
-      </c>
-      <c r="O52" s="2" t="s">
-        <v>281</v>
-      </c>
-      <c r="P52" s="2" t="s">
-        <v>281</v>
-      </c>
-      <c r="Q52" s="2" t="s">
-        <v>281</v>
-      </c>
-      <c r="R52" s="2" t="s">
-        <v>281</v>
-      </c>
       <c r="S52" s="16"/>
-      <c r="T52" s="2" t="s">
-        <v>339</v>
-      </c>
-      <c r="U52" s="2" t="s">
-        <v>339</v>
-      </c>
-      <c r="V52" s="2" t="s">
-        <v>339</v>
-      </c>
-      <c r="W52" s="2" t="s">
-        <v>339</v>
-      </c>
-      <c r="X52" s="2" t="s">
-        <v>339</v>
-      </c>
       <c r="Y52" s="16"/>
       <c r="Z52"/>
     </row>
@@ -3670,13 +3616,13 @@
     </row>
     <row r="59" spans="1:26" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A59" s="13" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="B59" s="13" t="s">
         <v>10</v>
       </c>
       <c r="C59" s="12" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="D59" s="13" t="b">
         <v>0</v>
@@ -3685,7 +3631,7 @@
         <v>1</v>
       </c>
       <c r="F59" s="13" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="G59" s="18"/>
       <c r="H59" s="13"/>
@@ -3710,22 +3656,22 @@
     </row>
     <row r="60" spans="1:26" s="7" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A60" s="7" t="s">
+        <v>302</v>
+      </c>
+      <c r="B60" s="7" t="s">
+        <v>303</v>
+      </c>
+      <c r="C60" s="7" t="s">
         <v>304</v>
       </c>
-      <c r="B60" s="7" t="s">
+      <c r="D60" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="E60" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="F60" s="7" t="s">
         <v>305</v>
-      </c>
-      <c r="C60" s="7" t="s">
-        <v>306</v>
-      </c>
-      <c r="D60" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="E60" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="F60" s="7" t="s">
-        <v>307</v>
       </c>
       <c r="G60" s="16"/>
       <c r="M60" s="16"/>
@@ -3734,13 +3680,13 @@
     </row>
     <row r="61" spans="1:26" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A61" s="7" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="B61" s="7" t="s">
         <v>90</v>
       </c>
       <c r="C61" s="7" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="D61" s="7" t="b">
         <v>0</v>
@@ -3749,7 +3695,7 @@
         <v>1</v>
       </c>
       <c r="F61" s="20" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="G61" s="16"/>
       <c r="H61" s="20"/>
@@ -3788,7 +3734,7 @@
         <v>1</v>
       </c>
       <c r="F62" s="7" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="G62" s="16"/>
       <c r="M62" s="16"/>
@@ -3912,13 +3858,13 @@
     </row>
     <row r="67" spans="1:26" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A67" s="2" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="B67" s="2" t="s">
         <v>10</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="D67" s="2" t="b">
         <v>0</v>
@@ -3927,7 +3873,7 @@
         <v>1</v>
       </c>
       <c r="F67" s="2" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="G67" s="16"/>
       <c r="M67" s="16"/>
@@ -4007,19 +3953,19 @@
       <c r="M70" s="16"/>
       <c r="S70" s="16"/>
       <c r="T70" s="2" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="U70" s="2" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="V70" s="2" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="W70" s="2" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="X70" s="2" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="Y70" s="16"/>
       <c r="Z70"/>
@@ -4074,8 +4020,8 @@
       <c r="Y72" s="16"/>
       <c r="Z72"/>
     </row>
-    <row r="73" spans="1:26" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A73" s="2" t="s">
+    <row r="73" spans="1:26" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A73" s="8" t="s">
         <v>73</v>
       </c>
       <c r="B73" s="2" t="s">
@@ -4091,65 +4037,20 @@
         <v>0</v>
       </c>
       <c r="G73" s="16"/>
-      <c r="H73" s="2" t="s">
-        <v>282</v>
-      </c>
-      <c r="I73" s="2" t="s">
-        <v>282</v>
-      </c>
-      <c r="J73" s="2" t="s">
-        <v>282</v>
-      </c>
-      <c r="K73" s="2" t="s">
-        <v>282</v>
-      </c>
-      <c r="L73" s="2" t="s">
-        <v>282</v>
-      </c>
       <c r="M73" s="16"/>
-      <c r="N73" s="2" t="s">
-        <v>283</v>
-      </c>
-      <c r="O73" s="2" t="s">
-        <v>283</v>
-      </c>
-      <c r="P73" s="2" t="s">
-        <v>283</v>
-      </c>
-      <c r="Q73" s="2" t="s">
-        <v>283</v>
-      </c>
-      <c r="R73" s="2" t="s">
-        <v>283</v>
-      </c>
       <c r="S73" s="16"/>
-      <c r="T73" s="2" t="s">
-        <v>339</v>
-      </c>
-      <c r="U73" s="2" t="s">
-        <v>339</v>
-      </c>
-      <c r="V73" s="2" t="s">
-        <v>339</v>
-      </c>
-      <c r="W73" s="2" t="s">
-        <v>339</v>
-      </c>
-      <c r="X73" s="2" t="s">
-        <v>339</v>
-      </c>
       <c r="Y73" s="16"/>
       <c r="Z73"/>
     </row>
     <row r="74" spans="1:26" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A74" s="2" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
       <c r="B74" s="2" t="s">
         <v>10</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="D74" s="2" t="b">
         <v>0</v>
@@ -4158,7 +4059,7 @@
         <v>1</v>
       </c>
       <c r="F74" s="2" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
       <c r="G74" s="16"/>
       <c r="M74" s="16"/>
@@ -4167,13 +4068,13 @@
     </row>
     <row r="75" spans="1:26" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A75" s="2" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="B75" s="2" t="s">
         <v>242</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="D75" s="2" t="b">
         <v>0</v>
@@ -4182,7 +4083,7 @@
         <v>1</v>
       </c>
       <c r="F75" s="2" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
       <c r="G75" s="16"/>
       <c r="M75" s="16"/>
@@ -4191,13 +4092,13 @@
     </row>
     <row r="76" spans="1:26" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A76" s="2" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="B76" s="2" t="s">
         <v>10</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="D76" s="2" t="b">
         <v>0</v>
@@ -4207,48 +4108,62 @@
       </c>
       <c r="G76" s="16"/>
       <c r="H76" s="2" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
       <c r="I76" s="2" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
       <c r="J76" s="2" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
       <c r="K76" s="2" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
       <c r="L76" s="2" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
       <c r="M76" s="16"/>
       <c r="N76" s="2" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
       <c r="O76" s="2" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
       <c r="P76" s="2" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
       <c r="Q76" s="2" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
       <c r="R76" s="2" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
       <c r="S76" s="16"/>
-      <c r="T76"/>
+      <c r="T76" s="2" t="s">
+        <v>337</v>
+      </c>
+      <c r="U76" s="2" t="s">
+        <v>337</v>
+      </c>
+      <c r="V76" s="2" t="s">
+        <v>337</v>
+      </c>
+      <c r="W76" s="2" t="s">
+        <v>337</v>
+      </c>
+      <c r="X76" s="2" t="s">
+        <v>337</v>
+      </c>
     </row>
     <row r="77" spans="1:26" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A77" s="2" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
       <c r="B77" s="2" t="s">
         <v>242</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
       <c r="D77" s="2" t="b">
         <v>0</v>
@@ -4269,7 +4184,7 @@
         <v>10</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="D78" s="2" t="b">
         <v>0</v>
@@ -4285,13 +4200,13 @@
     </row>
     <row r="79" spans="1:26" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A79" s="2" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="B79" s="2" t="s">
         <v>10</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="D79" s="2" t="b">
         <v>0</v>
@@ -4334,13 +4249,13 @@
     </row>
     <row r="81" spans="1:29" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A81" s="21" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="B81" s="21" t="s">
         <v>5</v>
       </c>
       <c r="C81" s="21" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="D81" s="2" t="b">
         <v>0</v>
@@ -4406,7 +4321,7 @@
       <c r="Y83" s="16"/>
       <c r="Z83"/>
     </row>
-    <row r="84" spans="1:29" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="84" spans="1:29" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A84" s="2" t="s">
         <v>79</v>
       </c>
@@ -4423,53 +4338,8 @@
         <v>0</v>
       </c>
       <c r="G84" s="16"/>
-      <c r="H84" s="2" t="s">
-        <v>280</v>
-      </c>
-      <c r="I84" s="2" t="s">
-        <v>280</v>
-      </c>
-      <c r="J84" s="2" t="s">
-        <v>280</v>
-      </c>
-      <c r="K84" s="2" t="s">
-        <v>280</v>
-      </c>
-      <c r="L84" s="2" t="s">
-        <v>280</v>
-      </c>
       <c r="M84" s="16"/>
-      <c r="N84" s="2" t="s">
-        <v>281</v>
-      </c>
-      <c r="O84" s="2" t="s">
-        <v>281</v>
-      </c>
-      <c r="P84" s="2" t="s">
-        <v>281</v>
-      </c>
-      <c r="Q84" s="2" t="s">
-        <v>281</v>
-      </c>
-      <c r="R84" s="2" t="s">
-        <v>281</v>
-      </c>
       <c r="S84" s="16"/>
-      <c r="T84" s="2" t="s">
-        <v>339</v>
-      </c>
-      <c r="U84" s="2" t="s">
-        <v>339</v>
-      </c>
-      <c r="V84" s="2" t="s">
-        <v>339</v>
-      </c>
-      <c r="W84" s="2" t="s">
-        <v>339</v>
-      </c>
-      <c r="X84" s="2" t="s">
-        <v>339</v>
-      </c>
       <c r="Y84" s="16"/>
       <c r="Z84"/>
     </row>
@@ -4490,7 +4360,7 @@
         <v>0</v>
       </c>
       <c r="F85" s="2" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="G85" s="16"/>
       <c r="M85" s="16"/>
@@ -4515,7 +4385,7 @@
         <v>0</v>
       </c>
       <c r="F86" s="7" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="G86" s="16"/>
       <c r="M86" s="16"/>
@@ -4544,24 +4414,24 @@
       </c>
       <c r="G87" s="16"/>
       <c r="I87" s="2" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="J87" s="2" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="K87" s="2" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="M87" s="16"/>
       <c r="S87" s="16"/>
       <c r="U87" s="2" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="V87" s="2" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="W87" s="2" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="Y87" s="16"/>
       <c r="Z87"/>
@@ -4641,19 +4511,19 @@
       </c>
       <c r="S89" s="16"/>
       <c r="T89" s="2" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="U89" s="2" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="V89" s="2" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="W89" s="2" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="X89" s="2" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="Y89" s="16"/>
       <c r="Z89"/>
@@ -4735,13 +4605,13 @@
     </row>
     <row r="93" spans="1:29" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A93" s="21" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="B93" s="21" t="s">
         <v>5</v>
       </c>
       <c r="C93" s="21" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="D93" s="21" t="b">
         <v>0</v>
@@ -4983,7 +4853,7 @@
         <v>1</v>
       </c>
       <c r="F100" s="2" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="G100" s="16"/>
       <c r="M100" s="16"/>
@@ -5018,13 +4888,13 @@
     </row>
     <row r="102" spans="1:26" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A102" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="B102" t="s">
         <v>10</v>
       </c>
       <c r="C102" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="D102" t="b">
         <v>1</v>
@@ -5033,7 +4903,7 @@
         <v>1</v>
       </c>
       <c r="F102" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="G102" s="16"/>
       <c r="M102" s="16"/>
@@ -5139,7 +5009,7 @@
       <c r="Z106"/>
     </row>
     <row r="107" spans="1:26" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A107" s="2" t="s">
+      <c r="A107" s="8" t="s">
         <v>111</v>
       </c>
       <c r="B107" s="2" t="s">
@@ -5155,53 +5025,8 @@
         <v>0</v>
       </c>
       <c r="G107" s="16"/>
-      <c r="H107" s="2" t="s">
-        <v>282</v>
-      </c>
-      <c r="I107" s="2" t="s">
-        <v>282</v>
-      </c>
-      <c r="J107" s="2" t="s">
-        <v>282</v>
-      </c>
-      <c r="K107" s="2" t="s">
-        <v>282</v>
-      </c>
-      <c r="L107" s="2" t="s">
-        <v>282</v>
-      </c>
       <c r="M107" s="16"/>
-      <c r="N107" s="2" t="s">
-        <v>283</v>
-      </c>
-      <c r="O107" s="2" t="s">
-        <v>283</v>
-      </c>
-      <c r="P107" s="2" t="s">
-        <v>283</v>
-      </c>
-      <c r="Q107" s="2" t="s">
-        <v>283</v>
-      </c>
-      <c r="R107" s="2" t="s">
-        <v>283</v>
-      </c>
       <c r="S107" s="16"/>
-      <c r="T107" s="2" t="s">
-        <v>339</v>
-      </c>
-      <c r="U107" s="2" t="s">
-        <v>339</v>
-      </c>
-      <c r="V107" s="2" t="s">
-        <v>339</v>
-      </c>
-      <c r="W107" s="2" t="s">
-        <v>339</v>
-      </c>
-      <c r="X107" s="2" t="s">
-        <v>339</v>
-      </c>
       <c r="Y107" s="16"/>
       <c r="Z107"/>
     </row>
@@ -5547,18 +5372,18 @@
       </c>
       <c r="Y114" s="16"/>
       <c r="Z114" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
     </row>
     <row r="115" spans="1:26" s="7" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A115" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="B115" t="s">
         <v>5</v>
       </c>
       <c r="C115" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="D115" t="b">
         <v>0</v>
@@ -5617,7 +5442,7 @@
       </c>
       <c r="Y115" s="16"/>
       <c r="Z115" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
     </row>
     <row r="116" spans="1:26" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
@@ -5793,22 +5618,22 @@
         <v>0</v>
       </c>
       <c r="F119" s="2" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="G119" s="16"/>
       <c r="M119" s="16"/>
       <c r="S119" s="16"/>
       <c r="Y119" s="16"/>
     </row>
-    <row r="120" spans="1:26" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A120" s="2" t="s">
-        <v>318</v>
+    <row r="120" spans="1:26" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A120" s="8" t="s">
+        <v>316</v>
       </c>
       <c r="B120" s="2" t="s">
         <v>10</v>
       </c>
       <c r="C120" s="2" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="D120" s="2" t="b">
         <v>1</v>
@@ -5817,53 +5642,8 @@
         <v>1</v>
       </c>
       <c r="G120" s="16"/>
-      <c r="H120" s="2" t="s">
-        <v>280</v>
-      </c>
-      <c r="I120" s="2" t="s">
-        <v>280</v>
-      </c>
-      <c r="J120" s="2" t="s">
-        <v>280</v>
-      </c>
-      <c r="K120" s="2" t="s">
-        <v>280</v>
-      </c>
-      <c r="L120" s="2" t="s">
-        <v>280</v>
-      </c>
       <c r="M120" s="16"/>
-      <c r="N120" s="2" t="s">
-        <v>281</v>
-      </c>
-      <c r="O120" s="2" t="s">
-        <v>281</v>
-      </c>
-      <c r="P120" s="2" t="s">
-        <v>281</v>
-      </c>
-      <c r="Q120" s="2" t="s">
-        <v>281</v>
-      </c>
-      <c r="R120" s="2" t="s">
-        <v>281</v>
-      </c>
       <c r="S120" s="16"/>
-      <c r="T120" s="2" t="s">
-        <v>339</v>
-      </c>
-      <c r="U120" s="2" t="s">
-        <v>339</v>
-      </c>
-      <c r="V120" s="2" t="s">
-        <v>339</v>
-      </c>
-      <c r="W120" s="2" t="s">
-        <v>339</v>
-      </c>
-      <c r="X120" s="2" t="s">
-        <v>339</v>
-      </c>
       <c r="Y120" s="16"/>
     </row>
     <row r="121" spans="1:26" s="2" customFormat="1" ht="58.3" x14ac:dyDescent="0.4">

</xml_diff>